<commit_message>
Update input method to currency box(amount and income)
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\OneDrive\Документы\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="330" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C55468D-7368-4EB8-9F32-6EE5F92F61D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208FC231-F260-4641-886E-664AB5CE0F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11295" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,61 +65,19 @@
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>957,51 лв.</t>
+    <t>23,45 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Грийн Марк ООД</t>
-  </si>
-  <si>
-    <t>Грийн Марк</t>
-  </si>
-  <si>
-    <t>2 251,33 лв.</t>
-  </si>
-  <si>
-    <t>Жанет ООД</t>
-  </si>
-  <si>
-    <t>Жанет - Несебър</t>
-  </si>
-  <si>
-    <t>2 119,58 лв.</t>
-  </si>
-  <si>
-    <t>2 604,10 лв.</t>
-  </si>
-  <si>
-    <t>Росси ООД</t>
-  </si>
-  <si>
-    <t>Росси</t>
-  </si>
-  <si>
-    <t>15 399,44 лв.</t>
-  </si>
-  <si>
-    <t>Кредитни известия</t>
-  </si>
-  <si>
-    <t>Кредитно</t>
-  </si>
-  <si>
-    <t>63,28 лв.</t>
-  </si>
-  <si>
-    <t>20,35 лв.</t>
-  </si>
-  <si>
-    <t>98,88 лв.</t>
+    <t>Понс-Комерс ЕООД</t>
+  </si>
+  <si>
+    <t>Понс Комерс</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от доставки: </t>
-  </si>
-  <si>
-    <t>23 331,96 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -252,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,14 +223,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEDEDED"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -395,14 +347,29 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFA6A6A6"/>
       </left>
       <right style="thin">
         <color rgb="FFA6A6A6"/>
       </right>
-      <top style="thin">
-        <color rgb="FFA6A6A6"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color rgb="FFA6A6A6"/>
@@ -410,74 +377,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA6A6A6"/>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA6A6A6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFA6A6A6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA6A6A6"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA6A6A6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFA6A6A6"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA6A6A6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA6A6A6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA6A6A6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA6A6A6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFA6A6A6"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA6A6A6"/>
       </top>
       <bottom style="thin">
         <color rgb="FFA6A6A6"/>
@@ -602,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -661,48 +568,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -718,16 +598,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,19 +619,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,22 +968,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6328125" customWidth="1"/>
+    <col min="2" max="2" width="32.6328125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1117,19 +997,19 @@
       <c r="G1" s="4"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45528</v>
+        <v>45541</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1031,7 @@
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1161,379 +1041,205 @@
       <c r="G4" s="15"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="22">
         <v>1</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22">
-        <v>1001161891</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="D6" s="24"/>
+      <c r="E6" s="25">
+        <v>1001166789</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="30"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>2</v>
-      </c>
-      <c r="B7" s="23" t="s">
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="C7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="C8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25">
-        <v>1001161930</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>3</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="21" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="C9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22">
-        <v>1001161931</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>4</v>
-      </c>
-      <c r="B9" s="23" t="s">
+      <c r="G9" s="1"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="C10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25">
-        <v>1001161932</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
-        <v>5</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22">
-        <v>1001161952</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>1</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22">
-        <v>1001161946</v>
-      </c>
-      <c r="F12" s="20" t="s">
+      <c r="F13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="37"/>
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>2</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25">
-        <v>1001161947</v>
-      </c>
-      <c r="F13" s="23" t="s">
+      <c r="D14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35">
-        <v>3</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38">
-        <v>1001161948</v>
-      </c>
-      <c r="F14" s="36" t="s">
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="39"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="41"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="44" t="s">
+      <c r="C17" s="42"/>
+      <c r="E17" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D18" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="41" t="s">
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B20" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="46"/>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="46"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C18" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="46"/>
-    </row>
-    <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="46"/>
-    </row>
-    <row r="20" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="48"/>
-    </row>
-    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="50"/>
-      <c r="H21" s="51"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="17"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="54"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="55"/>
-      <c r="E25" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="17"/>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="56">
-        <v>45530</v>
-      </c>
-      <c r="E29" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
+    </row>
+    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="43">
+        <v>45542</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
+  <mergeCells count="30">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>

<commit_message>
Disable day report export button withuot interen connection
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\OneDrive\Документы\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208FC231-F260-4641-886E-664AB5CE0F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="407" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A685417C-D91A-4AD0-AB98-2B8C085D2B44}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -62,24 +62,141 @@
     <t>Платено лв.</t>
   </si>
   <si>
+    <t>Плащане в брой</t>
+  </si>
+  <si>
+    <t>961,33 лв.</t>
+  </si>
+  <si>
+    <t>Галатея ЕН 99 ООД</t>
+  </si>
+  <si>
+    <t>Галатея</t>
+  </si>
+  <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>23,45 лв.</t>
+    <t>162,00 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Понс-Комерс ЕООД</t>
-  </si>
-  <si>
-    <t>Понс Комерс</t>
+    <t>Олдес ЕООД</t>
+  </si>
+  <si>
+    <t>Бългериан Скай Сървис Кетъринг</t>
+  </si>
+  <si>
+    <t>186,00 лв.</t>
+  </si>
+  <si>
+    <t>Едис Кетъринг ЕООД</t>
+  </si>
+  <si>
+    <t>Едис Терминал 2</t>
+  </si>
+  <si>
+    <t>90,50 лв.</t>
+  </si>
+  <si>
+    <t>Лагардер Травъл Ритейл ЕООД</t>
+  </si>
+  <si>
+    <t>Онда Терминал 2</t>
+  </si>
+  <si>
+    <t>626,26 лв.</t>
+  </si>
+  <si>
+    <t>Култ Гурме Кетъринг ЕООД</t>
+  </si>
+  <si>
+    <t>Кулинарен цех</t>
+  </si>
+  <si>
+    <t>1 173,49 лв.</t>
+  </si>
+  <si>
+    <t>Фили Вайб АД</t>
+  </si>
+  <si>
+    <t>Пица Лаб</t>
+  </si>
+  <si>
+    <t>344,18 лв.</t>
+  </si>
+  <si>
+    <t>Брадърс Комерс ООД</t>
+  </si>
+  <si>
+    <t>Брадърс Комерс София</t>
+  </si>
+  <si>
+    <t>657,95 лв.</t>
+  </si>
+  <si>
+    <t>Саза Тур ЕООД</t>
+  </si>
+  <si>
+    <t>Премиер Хотел</t>
+  </si>
+  <si>
+    <t>131,24 лв.</t>
+  </si>
+  <si>
+    <t>Разходи</t>
+  </si>
+  <si>
+    <t>Разход</t>
+  </si>
+  <si>
+    <t>-40,96 лв.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">СВ 2241 КК </t>
+  </si>
+  <si>
+    <t>Заден стоп</t>
+  </si>
+  <si>
+    <t>Отчет на парите</t>
+  </si>
+  <si>
+    <t>1 -</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>46 -</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
+  </si>
+  <si>
+    <t>920,00 лв.</t>
+  </si>
+  <si>
+    <t>Тотал:</t>
+  </si>
+  <si>
+    <t>920,50 лв.</t>
+  </si>
+  <si>
+    <t>Преброена сума</t>
+  </si>
+  <si>
+    <t>Разлика</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
+    <t>4 332,95 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
   </si>
   <si>
@@ -92,13 +209,25 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
+    <t>3 371,62 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
+    <t>40,96 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
+    <t>920,37 лв.</t>
+  </si>
+  <si>
     <t>Ресто:</t>
+  </si>
+  <si>
+    <t>0,13 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -210,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,8 +352,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -347,6 +482,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -401,6 +551,36 @@
       <top style="thin">
         <color rgb="FFA6A6A6"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -491,9 +671,44 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -509,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,24 +783,88 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -598,16 +877,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,19 +898,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -968,7 +1247,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1004,7 +1283,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45541</v>
+        <v>45544</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1042,204 +1321,490 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="22">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="22">
+        <v>1001165123</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="30"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25">
-        <v>1001166789</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="26"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="29">
+        <v>1</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22">
+        <v>1001165052</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="C8" s="28" t="s">
+      <c r="G8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="32" t="s">
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="33">
+        <v>2</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25">
+        <v>1001165056</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>3</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22">
+        <v>1001165058</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="33">
+        <v>4</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25">
+        <v>1001165125</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>5</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22">
+        <v>1001165126</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="33">
+        <v>6</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25">
+        <v>1001165127</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
+        <v>7</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22">
+        <v>1001165130</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="33">
+        <v>8</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="C9" s="28" t="s">
+      <c r="C15" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="C10" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="33"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C11" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="33"/>
-    </row>
-    <row r="12" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B12" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="41"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25">
+        <v>1001165145</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="42"/>
-      <c r="E17" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D18" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B20" s="39" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="43">
-        <v>45542</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="A16" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="35">
+        <v>1</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38">
+        <v>90920240</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="44"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="46"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="51"/>
+    </row>
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B21" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="53"/>
+      <c r="C22" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="63"/>
+    </row>
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B23" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="63"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="54"/>
+      <c r="C24" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="63"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C25" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="63"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="65"/>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="67"/>
+      <c r="H27" s="68"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="71"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="72"/>
+      <c r="E31" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D32" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="17"/>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B34" s="69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="73">
+        <v>45544</v>
+      </c>
+      <c r="E35" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:H11"/>
+  <mergeCells count="43">
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:H16"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>

<commit_message>
Refactoring load invoice from list view to MVVM model.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="407" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A685417C-D91A-4AD0-AB98-2B8C085D2B44}"/>
+  <xr:revisionPtr revIDLastSave="427" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8246418F-06C2-44F2-A919-F9550655EA0F}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,7 +65,7 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>961,33 лв.</t>
+    <t>1 741,13 лв.</t>
   </si>
   <si>
     <t>Галатея ЕН 99 ООД</t>
@@ -74,67 +74,61 @@
     <t>Галатея</t>
   </si>
   <si>
+    <t>24,54 лв.</t>
+  </si>
+  <si>
+    <t>615,41 лв.</t>
+  </si>
+  <si>
+    <t>Експрес Фууд Трейд ООД</t>
+  </si>
+  <si>
+    <t>Борса Станев</t>
+  </si>
+  <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>162,00 лв.</t>
+    <t>328,96 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Олдес ЕООД</t>
-  </si>
-  <si>
-    <t>Бългериан Скай Сървис Кетъринг</t>
-  </si>
-  <si>
-    <t>186,00 лв.</t>
-  </si>
-  <si>
-    <t>Едис Кетъринг ЕООД</t>
-  </si>
-  <si>
-    <t>Едис Терминал 2</t>
-  </si>
-  <si>
-    <t>90,50 лв.</t>
-  </si>
-  <si>
-    <t>Лагардер Травъл Ритейл ЕООД</t>
-  </si>
-  <si>
-    <t>Онда Терминал 2</t>
-  </si>
-  <si>
-    <t>626,26 лв.</t>
-  </si>
-  <si>
-    <t>Култ Гурме Кетъринг ЕООД</t>
-  </si>
-  <si>
-    <t>Кулинарен цех</t>
-  </si>
-  <si>
-    <t>1 173,49 лв.</t>
-  </si>
-  <si>
-    <t>Фили Вайб АД</t>
-  </si>
-  <si>
-    <t>Пица Лаб</t>
-  </si>
-  <si>
-    <t>344,18 лв.</t>
-  </si>
-  <si>
-    <t>Брадърс Комерс ООД</t>
-  </si>
-  <si>
-    <t>Брадърс Комерс София</t>
-  </si>
-  <si>
-    <t>657,95 лв.</t>
+    <t>Ексклузив Маркет ЕООД</t>
+  </si>
+  <si>
+    <t>Тейст кофи енд мор - София</t>
+  </si>
+  <si>
+    <t>562,80 лв.</t>
+  </si>
+  <si>
+    <t>Силвър Уингс България ООД</t>
+  </si>
+  <si>
+    <t>Силвър Уингс България</t>
+  </si>
+  <si>
+    <t>481,24 лв.</t>
+  </si>
+  <si>
+    <t>Пюър Трейдинг ЕООД</t>
+  </si>
+  <si>
+    <t>Гранд бистро</t>
+  </si>
+  <si>
+    <t>199,74 лв.</t>
+  </si>
+  <si>
+    <t>Ниа 2016 ЕООД</t>
+  </si>
+  <si>
+    <t>Евро Холд</t>
+  </si>
+  <si>
+    <t>1 455,92 лв.</t>
   </si>
   <si>
     <t>Саза Тур ЕООД</t>
@@ -143,7 +137,7 @@
     <t>Премиер Хотел</t>
   </si>
   <si>
-    <t>131,24 лв.</t>
+    <t>66,74 лв.</t>
   </si>
   <si>
     <t>Разходи</t>
@@ -152,13 +146,13 @@
     <t>Разход</t>
   </si>
   <si>
-    <t>-40,96 лв.</t>
+    <t>-5,00 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">СВ 2241 КК </t>
   </si>
   <si>
-    <t>Заден стоп</t>
+    <t>Вход Булгарплод</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -167,22 +161,37 @@
     <t>1 -</t>
   </si>
   <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>46 -</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>920,00 лв.</t>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>3 -</t>
+  </si>
+  <si>
+    <t>5,00 лв.</t>
+  </si>
+  <si>
+    <t>15,00 лв.</t>
+  </si>
+  <si>
+    <t>10,00 лв.</t>
+  </si>
+  <si>
+    <t>47 -</t>
+  </si>
+  <si>
+    <t>50,00 лв.</t>
+  </si>
+  <si>
+    <t>2 350,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>920,50 лв.</t>
+    <t>2 376,10 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -194,7 +203,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>4 332,95 лв.</t>
+    <t>5 476,48 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -209,25 +218,22 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>3 371,62 лв.</t>
+    <t>3 095,40 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
-    <t>40,96 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>920,37 лв.</t>
+    <t>2 376,08 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,13 лв.</t>
+    <t>0,02 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -724,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,14 +814,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -828,27 +834,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1247,7 +1265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1283,7 +1301,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45544</v>
+        <v>45546</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1344,7 +1362,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001165123</v>
+        <v>1001165628</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1355,196 +1373,196 @@
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="31">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25">
+        <v>1001165731</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="23" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>16</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001165052</v>
+        <v>1001165740</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="33">
-        <v>2</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25">
-        <v>1001165056</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>14</v>
-      </c>
+      <c r="A9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001165058</v>
+        <v>1001165624</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="33">
-        <v>4</v>
+      <c r="A11" s="31">
+        <v>2</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001165125</v>
+        <v>1001165627</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001165126</v>
+        <v>1001165629</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="33">
-        <v>6</v>
+      <c r="A13" s="31">
+        <v>4</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001165127</v>
+        <v>1001165726</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001165130</v>
+        <v>1001165734</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="33">
-        <v>8</v>
+      <c r="A15" s="31">
+        <v>6</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001165145</v>
+        <v>1001165735</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="34"/>
+        <v>18</v>
+      </c>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
-        <v>36</v>
+      <c r="A16" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
@@ -1552,247 +1570,275 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="32"/>
+      <c r="H16" s="34"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="35">
         <v>1</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="38">
-        <v>90920240</v>
+        <v>110920240</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44"/>
+      <c r="C18" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="48"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B19" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="50"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="D20" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="52"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="42" t="s">
+      <c r="C21" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="D21" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="46"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="51"/>
-    </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B21" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="55" t="s">
+      <c r="E21" s="54"/>
+      <c r="F21" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="61" t="s">
+      <c r="H21" s="57"/>
+    </row>
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B22" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="53"/>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="59"/>
+      <c r="C23" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="69"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B24" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="63"/>
-    </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B23" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="63"/>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="54"/>
-      <c r="C24" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="62" t="s">
+      <c r="C24" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="68" t="s">
         <v>57</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="63"/>
+      <c r="H24" s="69"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C25" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="62" t="s">
+      <c r="B25" s="60"/>
+      <c r="C25" s="63" t="s">
         <v>59</v>
       </c>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="68" t="s">
+        <v>60</v>
+      </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="63"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B26" s="69" t="s">
+      <c r="H25" s="69"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C26" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="69"/>
+    </row>
+    <row r="27" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="70" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="71"/>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="65"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="70" t="s">
+      <c r="F28" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="67"/>
-      <c r="H27" s="68"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="17"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="74"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="71" t="s">
+      <c r="B29" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="71"/>
+      <c r="D29" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
+      <c r="B30" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="77"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="72"/>
-      <c r="E31" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D32" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B34" s="69" t="s">
+      <c r="B32" s="78" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="73">
-        <v>45544</v>
-      </c>
-      <c r="E35" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
+      <c r="C32" s="78"/>
+      <c r="E32" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="78"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D33" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B35" s="75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="79">
+        <v>45546</v>
+      </c>
+      <c r="E36" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="F27:H27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:H32"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="F25:H25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:H18"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
@@ -1801,9 +1847,9 @@
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
Automatic set next day in DayReportId text box when today day report is create.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="427" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8246418F-06C2-44F2-A919-F9550655EA0F}"/>
+  <xr:revisionPtr revIDLastSave="582" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7361A3C5-06AE-484B-B116-7D6B18B4DC75}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,94 +65,151 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>1 741,13 лв.</t>
-  </si>
-  <si>
-    <t>Галатея ЕН 99 ООД</t>
-  </si>
-  <si>
-    <t>Галатея</t>
-  </si>
-  <si>
-    <t>24,54 лв.</t>
-  </si>
-  <si>
-    <t>615,41 лв.</t>
-  </si>
-  <si>
-    <t>Експрес Фууд Трейд ООД</t>
-  </si>
-  <si>
-    <t>Борса Станев</t>
+    <t>3 305,50 лв.</t>
+  </si>
+  <si>
+    <t>Фуудс 1990 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Данте</t>
+  </si>
+  <si>
+    <t>221,63 лв.</t>
+  </si>
+  <si>
+    <t>Бизнес Клуб - Валентина Петрова ЕООД</t>
+  </si>
+  <si>
+    <t>Бизнес хотел Валентина</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>328,96 лв.</t>
+    <t>2 807,98 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Ексклузив Маркет ЕООД</t>
-  </si>
-  <si>
-    <t>Тейст кофи енд мор - София</t>
-  </si>
-  <si>
-    <t>562,80 лв.</t>
-  </si>
-  <si>
-    <t>Силвър Уингс България ООД</t>
-  </si>
-  <si>
-    <t>Силвър Уингс България</t>
-  </si>
-  <si>
-    <t>481,24 лв.</t>
-  </si>
-  <si>
-    <t>Пюър Трейдинг ЕООД</t>
-  </si>
-  <si>
-    <t>Гранд бистро</t>
-  </si>
-  <si>
-    <t>199,74 лв.</t>
-  </si>
-  <si>
-    <t>Ниа 2016 ЕООД</t>
-  </si>
-  <si>
-    <t>Евро Холд</t>
-  </si>
-  <si>
-    <t>1 455,92 лв.</t>
-  </si>
-  <si>
-    <t>Саза Тур ЕООД</t>
-  </si>
-  <si>
-    <t>Премиер Хотел</t>
-  </si>
-  <si>
-    <t>66,74 лв.</t>
-  </si>
-  <si>
-    <t>Разходи</t>
-  </si>
-  <si>
-    <t>Разход</t>
-  </si>
-  <si>
-    <t>-5,00 лв.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">СВ 2241 КК </t>
-  </si>
-  <si>
-    <t>Вход Булгарплод</t>
+    <t>Едеа Ритейл АД</t>
+  </si>
+  <si>
+    <t>Едеа Магарин Русе</t>
+  </si>
+  <si>
+    <t>583,33 лв.</t>
+  </si>
+  <si>
+    <t>Живис ООД</t>
+  </si>
+  <si>
+    <t>Живис</t>
+  </si>
+  <si>
+    <t>322,50 лв.</t>
+  </si>
+  <si>
+    <t>Лагардер Травъл Ритейл ЕООД</t>
+  </si>
+  <si>
+    <t>Уан минът ЕС253 Добрич</t>
+  </si>
+  <si>
+    <t>2 572,43 лв.</t>
+  </si>
+  <si>
+    <t>Море 2020 ООД</t>
+  </si>
+  <si>
+    <t>Стария Чинар</t>
+  </si>
+  <si>
+    <t>3 565,20 лв.</t>
+  </si>
+  <si>
+    <t>Триада -ГТ ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Триада</t>
+  </si>
+  <si>
+    <t>2 747,63 лв.</t>
+  </si>
+  <si>
+    <t>Хепи Лейди ООД</t>
+  </si>
+  <si>
+    <t>Хепи кухня майка</t>
+  </si>
+  <si>
+    <t>1 645,93 лв.</t>
+  </si>
+  <si>
+    <t>Трънчев ООД</t>
+  </si>
+  <si>
+    <t>Магазин Булмаг</t>
+  </si>
+  <si>
+    <t>560,60 лв.</t>
+  </si>
+  <si>
+    <t>Барико Просеко Бар</t>
+  </si>
+  <si>
+    <t>751,63 лв.</t>
+  </si>
+  <si>
+    <t>Вазаро Комерс ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Вазаро</t>
+  </si>
+  <si>
+    <t>203,03 лв.</t>
+  </si>
+  <si>
+    <t>1 219,06 лв.</t>
+  </si>
+  <si>
+    <t>Сабросо 2012 ООД</t>
+  </si>
+  <si>
+    <t>Бурата</t>
+  </si>
+  <si>
+    <t>3 702,56 лв.</t>
+  </si>
+  <si>
+    <t>Железов 2017 ЕООД</t>
+  </si>
+  <si>
+    <t>Борса Дева</t>
+  </si>
+  <si>
+    <t>537,80 лв.</t>
+  </si>
+  <si>
+    <t>1 383,91 лв.</t>
+  </si>
+  <si>
+    <t>3 587,56 лв.</t>
+  </si>
+  <si>
+    <t>Кредитни известия</t>
+  </si>
+  <si>
+    <t>Кредитно</t>
+  </si>
+  <si>
+    <t>10,72 лв.</t>
+  </si>
+  <si>
+    <t>7,21 лв.</t>
+  </si>
+  <si>
+    <t>624,24 лв.</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -161,37 +218,58 @@
     <t>1 -</t>
   </si>
   <si>
+    <t>0,05 лв.</t>
+  </si>
+  <si>
     <t>0,10 лв.</t>
   </si>
   <si>
+    <t>2 -</t>
+  </si>
+  <si>
     <t>1,00 лв.</t>
   </si>
   <si>
-    <t>3 -</t>
+    <t>2,00 лв.</t>
   </si>
   <si>
     <t>5,00 лв.</t>
   </si>
   <si>
-    <t>15,00 лв.</t>
+    <t>25 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>47 -</t>
+    <t>250,00 лв.</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
+  </si>
+  <si>
+    <t>37 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>2 350,00 лв.</t>
+    <t>1 850,00 лв.</t>
+  </si>
+  <si>
+    <t>14 -</t>
+  </si>
+  <si>
+    <t>100,00 лв.</t>
+  </si>
+  <si>
+    <t>1 400,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>2 376,10 лв.</t>
+    <t>3 527,15 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -203,7 +281,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>5 476,48 лв.</t>
+    <t>29 718,28 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -218,7 +296,7 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>3 095,40 лв.</t>
+    <t>26 191,15 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -227,7 +305,7 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>2 376,08 лв.</t>
+    <t>3 527,13 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
@@ -1265,7 +1343,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1301,7 +1379,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45546</v>
+        <v>45547</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1362,7 +1440,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001165628</v>
+        <v>1001165799</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1377,14 +1455,14 @@
         <v>2</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001165731</v>
+        <v>1001165819</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1395,461 +1473,726 @@
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="29">
+      <c r="A8" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="29">
+        <v>1</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22">
+        <v>1001165796</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="31">
+        <v>2</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25">
+        <v>1001165797</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22">
+        <v>1001165798</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="31">
+        <v>4</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25">
+        <v>1001165800</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
+        <v>5</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22">
+        <v>1001165801</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>6</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25">
+        <v>1001165802</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
+        <v>7</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22">
+        <v>1001165804</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="31">
+        <v>8</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25">
+        <v>1001165818</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
+        <v>9</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22">
+        <v>1001165820</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="31">
+        <v>10</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25">
+        <v>1001165832</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>11</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22">
+        <v>1001165857</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="31">
+        <v>12</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25">
+        <v>1001165861</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>13</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22">
+        <v>1001165862</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="31">
         <v>14</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="B22" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25">
+        <v>1001165878</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="29">
         <v>15</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22">
-        <v>1001165740</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="34"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
+      <c r="B23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22">
+        <v>1001165884</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="29">
         <v>1</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22">
-        <v>1001165624</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="31">
+      <c r="B25" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22">
+        <v>1001165564</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
         <v>2</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B26" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25">
-        <v>1001165627</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
+      <c r="D26" s="24"/>
+      <c r="E26" s="25">
+        <v>1001165582</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="35">
         <v>3</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22">
-        <v>1001165629</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="31">
-        <v>4</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25">
-        <v>1001165726</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="29">
-        <v>5</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22">
-        <v>1001165734</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="31">
-        <v>6</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25">
-        <v>1001165735</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="34"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="35">
-        <v>1</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38">
-        <v>110920240</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C18" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B19" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="H19" s="50"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="52"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="57"/>
-    </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B22" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="61" t="s">
+      <c r="B27" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38">
+        <v>1001165583</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="67" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="59"/>
-      <c r="C23" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="69"/>
-    </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B24" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="63" t="s">
+      <c r="H27" s="39"/>
+    </row>
+    <row r="28" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C28" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="69"/>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="60"/>
-      <c r="C25" s="63" t="s">
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="48"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="68" t="s">
+      <c r="C29" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="69"/>
-    </row>
-    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C26" s="64" t="s">
+      <c r="D29" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="50"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="69"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="65" t="s">
+      <c r="D30" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="52"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="70" t="s">
+      <c r="C31" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="10"/>
-      <c r="H27" s="71"/>
-    </row>
-    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="66" t="s">
+      <c r="D31" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="72" t="s">
+      <c r="E31" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="50"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="G28" s="73"/>
-      <c r="H28" s="74"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="77" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="77"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="78"/>
-      <c r="E32" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D33" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="35" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B35" s="75" t="s">
+      <c r="D32" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="45" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="79">
-        <v>45546</v>
-      </c>
-      <c r="E36" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
+      <c r="F32" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="52"/>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="57"/>
+    </row>
+    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B34" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="59"/>
+      <c r="C35" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B36" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="69"/>
+    </row>
+    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="60"/>
+      <c r="C37" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="69"/>
+    </row>
+    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="69"/>
+    </row>
+    <row r="39" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="71"/>
+    </row>
+    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="73"/>
+      <c r="H40" s="74"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="77"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="77"/>
+      <c r="C43" s="77"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="78"/>
+      <c r="E44" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D45" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B47" s="75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="79">
+        <v>45548</v>
+      </c>
+      <c r="E48" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
+  <mergeCells count="53">
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:H28"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
Add functionality to can add more than one invoice with same invoice ID in one day report. This make possible to split pay method on one invoice.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="582" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7361A3C5-06AE-484B-B116-7D6B18B4DC75}"/>
+  <xr:revisionPtr revIDLastSave="648" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{892996BE-1BBF-48B5-BFE5-1AEAD1D01CEE}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,7 +65,19 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>3 305,50 лв.</t>
+    <t>361,33 лв.</t>
+  </si>
+  <si>
+    <t>100,00 лв.</t>
+  </si>
+  <si>
+    <t>(A)--&gt;Миналият Век ЕООД</t>
+  </si>
+  <si>
+    <t>Миналият век</t>
+  </si>
+  <si>
+    <t>35,93 лв.</t>
   </si>
   <si>
     <t>Фуудс 1990 ООД</t>
@@ -74,31 +86,55 @@
     <t>Ресторант Данте</t>
   </si>
   <si>
-    <t>221,63 лв.</t>
-  </si>
-  <si>
-    <t>Бизнес Клуб - Валентина Петрова ЕООД</t>
-  </si>
-  <si>
-    <t>Бизнес хотел Валентина</t>
+    <t>33,22 лв.</t>
+  </si>
+  <si>
+    <t>Пици Викторов ЕООД</t>
+  </si>
+  <si>
+    <t>Пица на дърва</t>
+  </si>
+  <si>
+    <t>Плащане с карта</t>
+  </si>
+  <si>
+    <t>261,33 лв.</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>2 807,98 лв.</t>
+    <t>1 326,83 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
+    <t>Порт Варна ООД</t>
+  </si>
+  <si>
+    <t>Стария чинар Варна</t>
+  </si>
+  <si>
+    <t>1 043,29 лв.</t>
+  </si>
+  <si>
+    <t>Море 2020 ООД</t>
+  </si>
+  <si>
+    <t>Стария Чинар</t>
+  </si>
+  <si>
+    <t>2 358,36 лв.</t>
+  </si>
+  <si>
     <t>Едеа Ритейл АД</t>
   </si>
   <si>
     <t>Едеа Магарин Русе</t>
   </si>
   <si>
-    <t>583,33 лв.</t>
+    <t>550,67 лв.</t>
   </si>
   <si>
     <t>Живис ООД</t>
@@ -107,70 +143,58 @@
     <t>Живис</t>
   </si>
   <si>
-    <t>322,50 лв.</t>
+    <t>1 847,33 лв.</t>
+  </si>
+  <si>
+    <t>Трънчев ООД</t>
+  </si>
+  <si>
+    <t>Магазин Булмаг</t>
+  </si>
+  <si>
+    <t>5 894,06 лв.</t>
+  </si>
+  <si>
+    <t>Хепи Лейди ООД</t>
+  </si>
+  <si>
+    <t>Хепи кухня майка</t>
+  </si>
+  <si>
+    <t>710,65 лв.</t>
   </si>
   <si>
     <t>Лагардер Травъл Ритейл ЕООД</t>
   </si>
   <si>
+    <t>Барико Просеко Бар</t>
+  </si>
+  <si>
+    <t>2 660,79 лв.</t>
+  </si>
+  <si>
+    <t>Триада -ГТ ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Триада</t>
+  </si>
+  <si>
+    <t>931,54 лв.</t>
+  </si>
+  <si>
+    <t>Изида ООД</t>
+  </si>
+  <si>
+    <t>Хотел Изида</t>
+  </si>
+  <si>
+    <t>148,50 лв.</t>
+  </si>
+  <si>
     <t>Уан минът ЕС253 Добрич</t>
   </si>
   <si>
-    <t>2 572,43 лв.</t>
-  </si>
-  <si>
-    <t>Море 2020 ООД</t>
-  </si>
-  <si>
-    <t>Стария Чинар</t>
-  </si>
-  <si>
-    <t>3 565,20 лв.</t>
-  </si>
-  <si>
-    <t>Триада -ГТ ООД</t>
-  </si>
-  <si>
-    <t>Дистрибутор Триада</t>
-  </si>
-  <si>
-    <t>2 747,63 лв.</t>
-  </si>
-  <si>
-    <t>Хепи Лейди ООД</t>
-  </si>
-  <si>
-    <t>Хепи кухня майка</t>
-  </si>
-  <si>
-    <t>1 645,93 лв.</t>
-  </si>
-  <si>
-    <t>Трънчев ООД</t>
-  </si>
-  <si>
-    <t>Магазин Булмаг</t>
-  </si>
-  <si>
-    <t>560,60 лв.</t>
-  </si>
-  <si>
-    <t>Барико Просеко Бар</t>
-  </si>
-  <si>
-    <t>751,63 лв.</t>
-  </si>
-  <si>
-    <t>Вазаро Комерс ООД</t>
-  </si>
-  <si>
-    <t>Дистрибутор Вазаро</t>
-  </si>
-  <si>
-    <t>203,03 лв.</t>
-  </si>
-  <si>
-    <t>1 219,06 лв.</t>
+    <t>1 019,03 лв.</t>
   </si>
   <si>
     <t>Сабросо 2012 ООД</t>
@@ -179,7 +203,7 @@
     <t>Бурата</t>
   </si>
   <si>
-    <t>3 702,56 лв.</t>
+    <t>79,09 лв.</t>
   </si>
   <si>
     <t>Железов 2017 ЕООД</t>
@@ -188,13 +212,31 @@
     <t>Борса Дева</t>
   </si>
   <si>
-    <t>537,80 лв.</t>
-  </si>
-  <si>
-    <t>1 383,91 лв.</t>
-  </si>
-  <si>
-    <t>3 587,56 лв.</t>
+    <t>189,52 лв.</t>
+  </si>
+  <si>
+    <t>3 002,29 лв.</t>
+  </si>
+  <si>
+    <t>2 222,85 лв.</t>
+  </si>
+  <si>
+    <t>201,10 лв.</t>
+  </si>
+  <si>
+    <t>Балкански Център Дипломат ООД</t>
+  </si>
+  <si>
+    <t>Дипломат Хотел</t>
+  </si>
+  <si>
+    <t>280,24 лв.</t>
+  </si>
+  <si>
+    <t>Хаус Маркет България АД</t>
+  </si>
+  <si>
+    <t>Икеа Варна</t>
   </si>
   <si>
     <t>Кредитни известия</t>
@@ -203,13 +245,34 @@
     <t>Кредитно</t>
   </si>
   <si>
-    <t>10,72 лв.</t>
-  </si>
-  <si>
-    <t>7,21 лв.</t>
-  </si>
-  <si>
-    <t>624,24 лв.</t>
+    <t>20,32 лв.</t>
+  </si>
+  <si>
+    <t>Неплатени</t>
+  </si>
+  <si>
+    <t>539,50 лв.</t>
+  </si>
+  <si>
+    <t>506,28 лв.</t>
+  </si>
+  <si>
+    <t>За кредитно</t>
+  </si>
+  <si>
+    <t>3 305,33 лв.</t>
+  </si>
+  <si>
+    <t>3 125,97 лв.</t>
+  </si>
+  <si>
+    <t>179,36 лв.</t>
+  </si>
+  <si>
+    <t>0,00 лв.</t>
+  </si>
+  <si>
+    <t>В брой</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -218,58 +281,46 @@
     <t>1 -</t>
   </si>
   <si>
-    <t>0,05 лв.</t>
-  </si>
-  <si>
     <t>0,10 лв.</t>
   </si>
   <si>
-    <t>2 -</t>
-  </si>
-  <si>
-    <t>1,00 лв.</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>5,00 лв.</t>
-  </si>
-  <si>
-    <t>25 -</t>
-  </si>
-  <si>
-    <t>10,00 лв.</t>
-  </si>
-  <si>
-    <t>250,00 лв.</t>
+    <t>4 -</t>
+  </si>
+  <si>
+    <t>0,20 лв.</t>
+  </si>
+  <si>
+    <t>0,80 лв.</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>5 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>37 -</t>
+    <t>52 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>1 850,00 лв.</t>
-  </si>
-  <si>
-    <t>14 -</t>
-  </si>
-  <si>
-    <t>100,00 лв.</t>
-  </si>
-  <si>
-    <t>1 400,00 лв.</t>
+    <t>2 600,00 лв.</t>
+  </si>
+  <si>
+    <t>11 -</t>
+  </si>
+  <si>
+    <t>1 100,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>3 527,15 лв.</t>
+    <t>3 801,40 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -281,22 +332,22 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>29 718,28 лв.</t>
+    <t>28 920,81 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
   </si>
   <si>
-    <t>0,00 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сума от неплатени сметки: </t>
   </si>
   <si>
+    <t>653,27 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>26 191,15 лв.</t>
+    <t>24 466,14 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -305,13 +356,7 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>3 527,13 лв.</t>
-  </si>
-  <si>
     <t>Ресто:</t>
-  </si>
-  <si>
-    <t>0,02 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -1343,7 +1388,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1379,7 +1424,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45547</v>
+        <v>45554</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1433,20 +1478,20 @@
         <v>1</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001165799</v>
+        <v>1001167596</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H6" s="30"/>
     </row>
@@ -1455,734 +1500,855 @@
         <v>2</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001165819</v>
+        <v>1001167614</v>
       </c>
       <c r="F7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="29">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22">
+        <v>1001167680</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="30"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="34"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>1</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="22">
+        <v>1001167596</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>1</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22">
+        <v>1001167541</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="31">
+        <v>2</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25">
+        <v>1001167542</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
+        <v>3</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22">
+        <v>1001167543</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="31">
+        <v>4</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25">
+        <v>1001167544</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="32"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="29">
+        <v>5</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22">
+        <v>1001167578</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="31">
+        <v>6</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25">
+        <v>1001167580</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="29">
+        <v>7</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22">
+        <v>1001167591</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="31">
+        <v>8</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25">
+        <v>1001167609</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
+        <v>9</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22">
+        <v>1001167610</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="30"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="31">
+        <v>10</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25">
+        <v>1001167615</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="29">
+        <v>11</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22">
+        <v>1001167617</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="31">
         <v>12</v>
       </c>
-      <c r="H7" s="32"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="33" t="s">
+      <c r="B23" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25">
+        <v>1001167630</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="29">
+        <v>13</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22">
+        <v>1001167632</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="30"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="31">
+        <v>14</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25">
+        <v>1001167634</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="29">
         <v>15</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="34"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="29">
+      <c r="B26" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22">
+        <v>1001167642</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="31">
+        <v>16</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25">
+        <v>1001167660</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="32"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="29">
+        <v>17</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22">
+        <v>1001167672</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="34"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22">
-        <v>1001165796</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="20" t="s">
+      <c r="B30" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22">
+        <v>1001166992</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="34"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="29">
+        <v>1</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="31">
+      <c r="C32" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22">
+        <v>1001167539</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="31">
         <v>2</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25">
-        <v>1001165797</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="32"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
+      <c r="B33" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25">
+        <v>1001167592</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="35">
         <v>3</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22">
-        <v>1001165798</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="31">
-        <v>4</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25">
-        <v>1001165800</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="29">
-        <v>5</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22">
-        <v>1001165801</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="31">
-        <v>6</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25">
-        <v>1001165802</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
-        <v>7</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22">
-        <v>1001165804</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="31">
-        <v>8</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25">
-        <v>1001165818</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
-        <v>9</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22">
-        <v>1001165820</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="31">
+      <c r="B34" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38">
+        <v>1001167673</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25">
-        <v>1001165832</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="29">
-        <v>11</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22">
-        <v>1001165857</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="31">
-        <v>12</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25">
-        <v>1001165861</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="29">
-        <v>13</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22">
-        <v>1001165862</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="31">
-        <v>14</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25">
-        <v>1001165878</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="32"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="29">
-        <v>15</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22">
-        <v>1001165884</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="30"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="34"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="29">
-        <v>1</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22">
-        <v>1001165564</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="30"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="31">
-        <v>2</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25">
-        <v>1001165582</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="H26" s="32"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="35">
-        <v>3</v>
-      </c>
-      <c r="B27" s="36" t="s">
+      <c r="H53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F55" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="37"/>
-      <c r="E27" s="38">
-        <v>1001165583</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="39"/>
-    </row>
-    <row r="28" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C28" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="48"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G31" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="41" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="52"/>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="56" t="s">
+      <c r="G55" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C56" s="53"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" s="57"/>
+    </row>
+    <row r="57" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B57" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="67" t="s">
+        <v>98</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="59"/>
+      <c r="C58" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="H33" s="57"/>
-    </row>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B34" s="58" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="59"/>
-      <c r="C35" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="69"/>
-    </row>
-    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B36" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="69"/>
-    </row>
-    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="60"/>
-      <c r="C37" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="69"/>
-    </row>
-    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C38" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="69"/>
-    </row>
-    <row r="39" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="71"/>
-    </row>
-    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="66" t="s">
-        <v>90</v>
-      </c>
-      <c r="F40" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="18" t="s">
+      <c r="G58" s="1"/>
+      <c r="H58" s="69"/>
+    </row>
+    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B59" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="69"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="60"/>
+      <c r="C60" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C61" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="75" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="77" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="77"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="78"/>
-      <c r="E44" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D45" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B47" s="75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="79">
-        <v>45548</v>
-      </c>
-      <c r="E48" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="71"/>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="E63" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="G63" s="73"/>
+      <c r="H63" s="74"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" s="77"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="77"/>
+      <c r="C66" s="77"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="78"/>
+      <c r="E67" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" s="78"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D68" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B70" s="75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="79">
+        <v>45555</v>
+      </c>
+      <c r="E71" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:H36"/>
+  <mergeCells count="60">
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -2191,8 +2357,8 @@
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
Bug fixed where excel task not ending aftet excel exporter complete whork.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B51037FC-0F06-445C-9014-46ECFF23AFF9}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{344D920C-1DF3-40C9-B7F8-54B1124D961F}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,111 +65,57 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>301,87 лв.</t>
-  </si>
-  <si>
-    <t>Еъртрейд АД</t>
-  </si>
-  <si>
-    <t>Корията</t>
-  </si>
-  <si>
-    <t>390,92 лв.</t>
-  </si>
-  <si>
-    <t>Олдес ЕООД</t>
-  </si>
-  <si>
-    <t>Столова Олдес</t>
+    <t>26,94 лв.</t>
+  </si>
+  <si>
+    <t>Галатея ЕН 99 ООД</t>
+  </si>
+  <si>
+    <t>Галатея</t>
+  </si>
+  <si>
+    <t>483,24 лв.</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>186,00 лв.</t>
+    <t>2 062,26 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
+    <t>Саза Тур ЕООД</t>
+  </si>
+  <si>
+    <t>Премиер Хотел</t>
+  </si>
+  <si>
+    <t>90,50 лв.</t>
+  </si>
+  <si>
+    <t>Лагардер Травъл Ритейл ЕООД</t>
+  </si>
+  <si>
+    <t>Онда Терминал 2</t>
+  </si>
+  <si>
+    <t>125,98 лв.</t>
+  </si>
+  <si>
+    <t>Онда Терминал 1 ЕС240</t>
+  </si>
+  <si>
+    <t>376,28 лв.</t>
+  </si>
+  <si>
     <t>Едис Кетъринг ЕООД</t>
   </si>
   <si>
     <t>Едис Терминал 2</t>
   </si>
   <si>
-    <t>125,98 лв.</t>
-  </si>
-  <si>
-    <t>Лагардер Травъл Ритейл ЕООД</t>
-  </si>
-  <si>
-    <t>Онда Терминал 1 ЕС240</t>
-  </si>
-  <si>
-    <t>84,64 лв.</t>
-  </si>
-  <si>
-    <t>Никимар - 78 ЕООД</t>
-  </si>
-  <si>
-    <t>Ями-Ями Силвър Стар</t>
-  </si>
-  <si>
-    <t>2 423,57 лв.</t>
-  </si>
-  <si>
-    <t>Саранда Дистрибюшън ООД</t>
-  </si>
-  <si>
-    <t>Саранда Дистрибюшън</t>
-  </si>
-  <si>
-    <t>175,20 лв.</t>
-  </si>
-  <si>
-    <t>Пюър Трейдинг ЕООД</t>
-  </si>
-  <si>
-    <t>Гранд бистро</t>
-  </si>
-  <si>
-    <t>4 633,02 лв.</t>
-  </si>
-  <si>
-    <t>Грийн Марк Логистика ООД</t>
-  </si>
-  <si>
-    <t>Грийн Марк</t>
-  </si>
-  <si>
-    <t>957,51 лв.</t>
-  </si>
-  <si>
-    <t>677,94 лв.</t>
-  </si>
-  <si>
-    <t>2 195,07 лв.</t>
-  </si>
-  <si>
-    <t>Онда Кафе - Кухня Майка</t>
-  </si>
-  <si>
-    <t>135,76 лв.</t>
-  </si>
-  <si>
-    <t>Онда Терминал 2</t>
-  </si>
-  <si>
-    <t>128,60 лв.</t>
-  </si>
-  <si>
-    <t>Култ Гурме Кетъринг ЕООД</t>
-  </si>
-  <si>
-    <t>Кулинарен цех</t>
-  </si>
-  <si>
     <t>337,68 лв.</t>
   </si>
   <si>
@@ -185,40 +131,25 @@
     <t>1 -</t>
   </si>
   <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
     <t>0,20 лв.</t>
   </si>
   <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>4 -</t>
-  </si>
-  <si>
-    <t>5,00 лв.</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>13 -</t>
+    <t>10,00 лв.</t>
+  </si>
+  <si>
+    <t>10 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>650,00 лв.</t>
+    <t>500,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>692,80 лв.</t>
+    <t>510,20 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -230,7 +161,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>12 753,76 лв.</t>
+    <t>3 502,88 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -245,7 +176,7 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>12 060,97 лв.</t>
+    <t>2 992,70 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -254,13 +185,13 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>692,79 лв.</t>
+    <t>510,18 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,01 лв.</t>
+    <t>0,02 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -757,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -849,15 +780,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -868,10 +799,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -883,8 +810,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1292,7 +1217,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1328,7 +1253,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45562</v>
+        <v>45558</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1389,7 +1314,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001169837</v>
+        <v>1001165514</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1404,14 +1329,14 @@
         <v>2</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001169841</v>
+        <v>1001165523</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1423,7 +1348,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1438,20 +1363,20 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="22">
-        <v>1001169609</v>
+        <v>1001165527</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H9" s="30"/>
     </row>
@@ -1460,20 +1385,20 @@
         <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="25">
-        <v>1001169610</v>
+        <v>1001168449</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H10" s="32"/>
     </row>
@@ -1482,20 +1407,20 @@
         <v>3</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="22">
-        <v>1001169611</v>
+        <v>1001168450</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H11" s="30"/>
     </row>
@@ -1504,474 +1429,271 @@
         <v>4</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="25">
-        <v>1001169614</v>
+        <v>1001168464</v>
       </c>
       <c r="F12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="35">
+        <v>5</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38">
+        <v>1001168521</v>
+      </c>
+      <c r="F13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="29">
-        <v>5</v>
-      </c>
-      <c r="B13" s="20" t="s">
+      <c r="G13" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C15" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22">
-        <v>1001169637</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="31">
-        <v>6</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="D15" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="F15" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25">
-        <v>1001169716</v>
-      </c>
-      <c r="F14" s="23" t="s">
+      <c r="G15" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="48"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
-        <v>7</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22">
-        <v>1001169750</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="31">
-        <v>8</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25">
-        <v>1001169825</v>
-      </c>
-      <c r="F16" s="23" t="s">
+      <c r="D16" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="50"/>
+      <c r="F16" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="G16" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
-        <v>9</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="21" t="s">
+      <c r="G16" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="53"/>
+    </row>
+    <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B17" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22">
-        <v>1001169833</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="31">
-        <v>10</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="24" t="s">
+      <c r="C17" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25">
-        <v>1001169839</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="55"/>
+      <c r="C18" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="65"/>
+    </row>
+    <row r="19" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B19" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="29">
-        <v>11</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22">
-        <v>1001169840</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="35">
-        <v>12</v>
-      </c>
-      <c r="B20" s="36" t="s">
+      <c r="G19" s="1"/>
+      <c r="H19" s="65"/>
+    </row>
+    <row r="20" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="56"/>
+      <c r="C20" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38">
-        <v>1001169857</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C21" s="46" t="s">
+      <c r="G20" s="1"/>
+      <c r="H20" s="65"/>
+    </row>
+    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="40" t="s">
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="65"/>
+    </row>
+    <row r="22" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="43" t="s">
+      <c r="G22" s="10"/>
+      <c r="H22" s="67"/>
+    </row>
+    <row r="23" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="E23" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="D24" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="52"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="C25" s="73"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="42" t="s">
+      <c r="C27" s="74"/>
+      <c r="E27" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D28" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="50"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55" t="s">
+      <c r="E28" s="17"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="30" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B30" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="57"/>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B26" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="59"/>
-      <c r="C27" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="69"/>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B28" s="58" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="69"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="60"/>
-      <c r="C29" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="69"/>
-    </row>
-    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="69"/>
-    </row>
-    <row r="31" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B31" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="71"/>
-    </row>
-    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="76" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="66" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" s="73"/>
-      <c r="H32" s="74"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B33" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B34" s="77" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="77"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B36" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="78"/>
-      <c r="E36" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D37" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="17"/>
-    </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="39" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B39" s="75" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="79">
-        <v>45562</v>
-      </c>
-      <c r="E40" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
+    </row>
+    <row r="31" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="75">
+        <v>45558</v>
+      </c>
+      <c r="E31" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="G25:H25"/>
+  <mergeCells count="39">
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>

</xml_diff>

<commit_message>
Stable 1.1 MySql DB only for companies and objects
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\OneDrive\Документы\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="838" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33F394F3-7EE2-4137-BF8C-B2109218C8FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEBA47A-8620-43B0-BE7D-36365865115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="139">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,333 +65,228 @@
     <t>Плащане в брой</t>
   </si>
   <si>
+    <t>172,25 лв.</t>
+  </si>
+  <si>
+    <t>Чери и Ко ЕООД</t>
+  </si>
+  <si>
+    <t>Бирария Трафа - Овча купел</t>
+  </si>
+  <si>
+    <t>91,74 лв.</t>
+  </si>
+  <si>
+    <t>Пешева Ми 96 ЕООД</t>
+  </si>
+  <si>
+    <t>Бакалин</t>
+  </si>
+  <si>
+    <t>126,54 лв.</t>
+  </si>
+  <si>
+    <t>Момо М ЕООД</t>
+  </si>
+  <si>
+    <t>Хотел Горна Баня</t>
+  </si>
+  <si>
+    <t>404,16 лв.</t>
+  </si>
+  <si>
+    <t>Трасе ООД</t>
+  </si>
+  <si>
+    <t>Гастро Бар Трасе</t>
+  </si>
+  <si>
+    <t>91,18 лв.</t>
+  </si>
+  <si>
+    <t>Стобис ООД</t>
+  </si>
+  <si>
+    <t>Хранителен Магазин - СБА Стобис</t>
+  </si>
+  <si>
+    <t>235,39 лв.</t>
+  </si>
+  <si>
+    <t>Маги - ИВ ЕООД</t>
+  </si>
+  <si>
+    <t>Пицария Ветрило - Борово</t>
+  </si>
+  <si>
+    <t>75,85 лв.</t>
+  </si>
+  <si>
+    <t>Жа Ни Комерс 2016 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Дъ Ринг</t>
+  </si>
+  <si>
+    <t>126,98 лв.</t>
+  </si>
+  <si>
+    <t>Зебрано 1 ООД</t>
+  </si>
+  <si>
+    <t>Ола - МОЛ България</t>
+  </si>
+  <si>
+    <t>122,88 лв.</t>
+  </si>
+  <si>
+    <t>Хранителен Магазин - Стобис Борово</t>
+  </si>
+  <si>
+    <t>293,98 лв.</t>
+  </si>
+  <si>
+    <t>Додо - Мирослав Дунеловски ЕТ</t>
+  </si>
+  <si>
+    <t>Додо - Мирослав Дунеловски</t>
+  </si>
+  <si>
+    <t>609,84 лв.</t>
+  </si>
+  <si>
+    <t>Пи Ем Фууд ЕООД</t>
+  </si>
+  <si>
+    <t>Хасиенда</t>
+  </si>
+  <si>
+    <t>114,71 лв.</t>
+  </si>
+  <si>
+    <t>Хранителен Магазин - Стобис Лагера</t>
+  </si>
+  <si>
+    <t>294,21 лв.</t>
+  </si>
+  <si>
+    <t>АК Фемили ООД</t>
+  </si>
+  <si>
+    <t>Пицария - Красно село</t>
+  </si>
+  <si>
+    <t>249,60 лв.</t>
+  </si>
+  <si>
+    <t>Пицария Ветрило - Стрелбище</t>
+  </si>
+  <si>
+    <t>157,99 лв.</t>
+  </si>
+  <si>
+    <t>Групата БГ  ЕООД</t>
+  </si>
+  <si>
+    <t>Кайро Релакс Бар</t>
+  </si>
+  <si>
+    <t>213,83 лв.</t>
+  </si>
+  <si>
+    <t>126,07 лв.</t>
+  </si>
+  <si>
+    <t>Бримекс ЕООД</t>
+  </si>
+  <si>
+    <t>Пекарна Бримекс</t>
+  </si>
+  <si>
+    <t>77,77 лв.</t>
+  </si>
+  <si>
+    <t>109,22 лв.</t>
+  </si>
+  <si>
+    <t>Пица Енд Бабълс ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Енд Бабълс</t>
+  </si>
+  <si>
+    <t>1 523,80 лв.</t>
+  </si>
+  <si>
+    <t>Ем Найт Фууд ООД</t>
+  </si>
+  <si>
+    <t>Инсомния - Овча Купел</t>
+  </si>
+  <si>
+    <t>Плащане по банка</t>
+  </si>
+  <si>
+    <t>94,04 лв.</t>
+  </si>
+  <si>
+    <t>Банка</t>
+  </si>
+  <si>
+    <t>Джи ЕН Продакшън ООД</t>
+  </si>
+  <si>
+    <t>Неро Фор Хоум</t>
+  </si>
+  <si>
+    <t>318,52 лв.</t>
+  </si>
+  <si>
+    <t>Сепарит ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Розе</t>
+  </si>
+  <si>
+    <t>291,12 лв.</t>
+  </si>
+  <si>
+    <t>Планината ЕООД</t>
+  </si>
+  <si>
+    <t>Магазин Монте</t>
+  </si>
+  <si>
+    <t>356,39 лв.</t>
+  </si>
+  <si>
+    <t>Перфето БГ ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Перфетто</t>
+  </si>
+  <si>
+    <t>Кредитни известия</t>
+  </si>
+  <si>
+    <t>Кредитно</t>
+  </si>
+  <si>
+    <t>-111,56 лв.</t>
+  </si>
+  <si>
+    <t>Неплатени</t>
+  </si>
+  <si>
+    <t>Интер Гардън ООД</t>
+  </si>
+  <si>
+    <t>161,60 лв.</t>
+  </si>
+  <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Сохо Кафе ООД</t>
-  </si>
-  <si>
-    <t>Сохо Кафе - МОЛ България</t>
-  </si>
-  <si>
-    <t>181,70 лв.</t>
-  </si>
-  <si>
-    <t>МД-МГ ООД</t>
-  </si>
-  <si>
-    <t>Пица на дърва - Павлово</t>
-  </si>
-  <si>
-    <t>141,19 лв.</t>
-  </si>
-  <si>
-    <t>КСД Трейд ЕООД</t>
-  </si>
-  <si>
-    <t>Патрико 43</t>
-  </si>
-  <si>
-    <t>81,49 лв.</t>
-  </si>
-  <si>
-    <t>Бобзи Бейк ЕООД</t>
-  </si>
-  <si>
-    <t>Бобзи Бейк</t>
-  </si>
-  <si>
-    <t>151,28 лв.</t>
-  </si>
-  <si>
-    <t>Б Дизайн С ЕООД</t>
-  </si>
-  <si>
-    <t>Нож и Вилица - Бъкстон</t>
-  </si>
-  <si>
-    <t>74,40 лв.</t>
-  </si>
-  <si>
-    <t>Мамин Кольо София ЕООД</t>
-  </si>
-  <si>
-    <t>Механа Мамин Кольо - Цар Борис</t>
-  </si>
-  <si>
-    <t>261,64 лв.</t>
-  </si>
-  <si>
-    <t>Франджипани ООД</t>
-  </si>
-  <si>
-    <t>Сно Бар</t>
-  </si>
-  <si>
-    <t>322,42 лв.</t>
-  </si>
-  <si>
-    <t>Групата БГ  ЕООД</t>
-  </si>
-  <si>
-    <t>Кайро Релакс Бар</t>
-  </si>
-  <si>
-    <t>252,82 лв.</t>
-  </si>
-  <si>
-    <t>Маги - ИВ ЕООД</t>
-  </si>
-  <si>
-    <t>Пицария Ветрило - Стрелбище</t>
-  </si>
-  <si>
-    <t>88,34 лв.</t>
-  </si>
-  <si>
-    <t>Бейкън ООД</t>
-  </si>
-  <si>
-    <t>Бейкън</t>
-  </si>
-  <si>
-    <t>330,71 лв.</t>
-  </si>
-  <si>
-    <t>Пи Ем Фууд ЕООД</t>
-  </si>
-  <si>
-    <t>Хасиенда</t>
-  </si>
-  <si>
-    <t>368,93 лв.</t>
-  </si>
-  <si>
-    <t>Давиан ООД</t>
-  </si>
-  <si>
-    <t>Адоро - Нишава</t>
-  </si>
-  <si>
-    <t>201,01 лв.</t>
-  </si>
-  <si>
-    <t>Пицария Ветрило - Борово</t>
-  </si>
-  <si>
-    <t>65,28 лв.</t>
-  </si>
-  <si>
-    <t>100,94 лв.</t>
-  </si>
-  <si>
-    <t>Давчеви ООД</t>
-  </si>
-  <si>
-    <t>Паперино</t>
-  </si>
-  <si>
-    <t>252,36 лв.</t>
-  </si>
-  <si>
-    <t>Инкони ЕООД</t>
-  </si>
-  <si>
-    <t>Берьозка - Тодор Каблешков</t>
-  </si>
-  <si>
-    <t>455,51 лв.</t>
-  </si>
-  <si>
-    <t>СК Сървиз ЕООД</t>
-  </si>
-  <si>
-    <t>Спагети Къмпани - МОЛ България</t>
-  </si>
-  <si>
-    <t>59,68 лв.</t>
-  </si>
-  <si>
-    <t>АК Фемили ООД</t>
-  </si>
-  <si>
-    <t>Пицария - Красно село</t>
-  </si>
-  <si>
-    <t>629,87 лв.</t>
-  </si>
-  <si>
-    <t>Арте Фууд ООД</t>
-  </si>
-  <si>
-    <t>Арте Джелато - Кейк и Пица</t>
-  </si>
-  <si>
-    <t>163,80 лв.</t>
-  </si>
-  <si>
-    <t>Боне Трейд ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Боне - Павлово</t>
-  </si>
-  <si>
-    <t>163,68 лв.</t>
-  </si>
-  <si>
-    <t>Маймет 21 ЕООД</t>
-  </si>
-  <si>
-    <t>Сладкарница Симид</t>
-  </si>
-  <si>
-    <t>409,24 лв.</t>
-  </si>
-  <si>
-    <t>151,76 лв.</t>
-  </si>
-  <si>
-    <t>Густо Гурме ЕООД</t>
-  </si>
-  <si>
-    <t>Густо Гурме</t>
-  </si>
-  <si>
-    <t>95,00 лв.</t>
-  </si>
-  <si>
-    <t>Бомила ЕООД</t>
-  </si>
-  <si>
-    <t>Тирол-Т - Бокар</t>
-  </si>
-  <si>
-    <t>113,72 лв.</t>
-  </si>
-  <si>
-    <t>Валпо ЕООД</t>
-  </si>
-  <si>
-    <t>Махана Винаената - Овча купел</t>
-  </si>
-  <si>
-    <t>70,68 лв.</t>
-  </si>
-  <si>
-    <t>Оупен Туризъм ЕООД</t>
-  </si>
-  <si>
-    <t>Ликьор Стор</t>
-  </si>
-  <si>
-    <t>194,03 лв.</t>
-  </si>
-  <si>
-    <t>Зефир 2002 ООД</t>
-  </si>
-  <si>
-    <t>Механа Каруцата</t>
-  </si>
-  <si>
-    <t>169,92 лв.</t>
-  </si>
-  <si>
-    <t>Пица на дърва - Красно село</t>
-  </si>
-  <si>
-    <t>119,62 лв.</t>
-  </si>
-  <si>
-    <t>Пица Миа 2022 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Миа София - Овча купел</t>
-  </si>
-  <si>
-    <t>54,86 лв.</t>
-  </si>
-  <si>
-    <t>136,62 лв.</t>
-  </si>
-  <si>
-    <t>Симона И Ко ООД</t>
-  </si>
-  <si>
-    <t>Арт хотел Симона</t>
-  </si>
-  <si>
-    <t>116,96 лв.</t>
-  </si>
-  <si>
-    <t>Пит Стоп - 2019 ЕООД</t>
-  </si>
-  <si>
-    <t>Пит Стоп Кафетерия</t>
-  </si>
-  <si>
-    <t>Плащане с карта</t>
-  </si>
-  <si>
-    <t>231,49 лв.</t>
-  </si>
-  <si>
-    <t>Старата Италия ЕООД</t>
-  </si>
-  <si>
-    <t>Старата италия</t>
-  </si>
-  <si>
-    <t>Плащане по банка</t>
-  </si>
-  <si>
-    <t>231,97 лв.</t>
-  </si>
-  <si>
-    <t>Банка</t>
-  </si>
-  <si>
-    <t>Арт 2000 ООД</t>
-  </si>
-  <si>
-    <t>Виктория - Абакус</t>
-  </si>
-  <si>
-    <t>431,59 лв.</t>
-  </si>
-  <si>
-    <t>Джи ЕН Продакшън ООД</t>
-  </si>
-  <si>
-    <t>Неро Фор Хоум</t>
-  </si>
-  <si>
-    <t>276,54 лв.</t>
-  </si>
-  <si>
-    <t>Енддиет ЕООД</t>
-  </si>
-  <si>
-    <t>Кетъринг Енджи Партер</t>
-  </si>
-  <si>
-    <t>353,11 лв.</t>
-  </si>
-  <si>
-    <t>Д Мийт Бокс ООД</t>
-  </si>
-  <si>
-    <t>Магазин за вино Д Мийт Бокс 2</t>
-  </si>
-  <si>
-    <t>Неплатени</t>
-  </si>
-  <si>
-    <t>Мелинс ООД</t>
-  </si>
-  <si>
-    <t>526,02 лв.</t>
-  </si>
-  <si>
     <t>В брой</t>
   </si>
   <si>
@@ -401,79 +296,97 @@
     <t>1 -</t>
   </si>
   <si>
+    <t>0,02 лв.</t>
+  </si>
+  <si>
+    <t>2 -</t>
+  </si>
+  <si>
+    <t>0,05 лв.</t>
+  </si>
+  <si>
     <t>0,10 лв.</t>
   </si>
   <si>
-    <t>2 -</t>
+    <t>6 -</t>
+  </si>
+  <si>
+    <t>0,60 лв.</t>
+  </si>
+  <si>
+    <t>9 -</t>
   </si>
   <si>
     <t>0,20 лв.</t>
   </si>
   <si>
-    <t>0,40 лв.</t>
-  </si>
-  <si>
-    <t>17 -</t>
+    <t>1,80 лв.</t>
+  </si>
+  <si>
+    <t>4 -</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
+    <t>8 -</t>
   </si>
   <si>
     <t>1,00 лв.</t>
   </si>
   <si>
-    <t>17,00 лв.</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>6 -</t>
+    <t>8,00 лв.</t>
+  </si>
+  <si>
+    <t>4,00 лв.</t>
   </si>
   <si>
     <t>5,00 лв.</t>
   </si>
   <si>
-    <t>30,00 лв.</t>
-  </si>
-  <si>
-    <t>50 -</t>
-  </si>
-  <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>500,00 лв.</t>
-  </si>
-  <si>
-    <t>94 -</t>
+    <t>38 -</t>
+  </si>
+  <si>
+    <t>380,00 лв.</t>
+  </si>
+  <si>
+    <t>45 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>1 880,00 лв.</t>
-  </si>
-  <si>
-    <t>39 -</t>
+    <t>900,00 лв.</t>
+  </si>
+  <si>
+    <t>70 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>1 950,00 лв.</t>
-  </si>
-  <si>
-    <t>16 -</t>
+    <t>3 500,00 лв.</t>
+  </si>
+  <si>
+    <t>3 -</t>
   </si>
   <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>1 600,00 лв.</t>
+    <t>300,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>5 979,50 лв.</t>
+    <t>5 106,52 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -485,7 +398,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>8 030,18 лв.</t>
+    <t>6 439,66 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -497,22 +410,25 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>1 293,21 лв.</t>
+    <t>1 060,07 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
+    <t>111,56 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>5 979,46 лв.</t>
+    <t>5 106,43 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,04 лв.</t>
+    <t>0,09 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -1544,7 +1460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1580,7 +1496,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45572</v>
+        <v>45573</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1641,7 +1557,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>919477</v>
+        <v>1001171380</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1663,7 +1579,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001171805</v>
+        <v>1001171393</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1685,7 +1601,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001171806</v>
+        <v>1001171394</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1707,7 +1623,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001171808</v>
+        <v>1001171399</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
@@ -1729,7 +1645,7 @@
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001171809</v>
+        <v>1001172196</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>21</v>
@@ -1751,7 +1667,7 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001171810</v>
+        <v>1001172197</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>24</v>
@@ -1773,7 +1689,7 @@
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001171811</v>
+        <v>1001172198</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>27</v>
@@ -1795,7 +1711,7 @@
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001171812</v>
+        <v>1001172201</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>30</v>
@@ -1810,14 +1726,14 @@
         <v>9</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001171817</v>
+        <v>1001172205</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>33</v>
@@ -1832,20 +1748,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>38</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001171818</v>
+        <v>1001172208</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="32"/>
     </row>
@@ -1854,20 +1770,20 @@
         <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001171819</v>
+        <v>1001172215</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="30"/>
     </row>
@@ -1876,20 +1792,20 @@
         <v>12</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="25">
-        <v>1001171820</v>
+        <v>1001172217</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" s="32"/>
     </row>
@@ -1898,20 +1814,20 @@
         <v>13</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
-        <v>1001171822</v>
+        <v>1001172250</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H18" s="30"/>
     </row>
@@ -1920,20 +1836,20 @@
         <v>14</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="25">
-        <v>1001171823</v>
+        <v>1001172251</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H19" s="32"/>
     </row>
@@ -1949,7 +1865,7 @@
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
-        <v>1001171824</v>
+        <v>1001172258</v>
       </c>
       <c r="F20" s="20" t="s">
         <v>48</v>
@@ -1964,14 +1880,14 @@
         <v>16</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="25">
-        <v>1001171825</v>
+        <v>1001172262</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>51</v>
@@ -1986,20 +1902,20 @@
         <v>17</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
-        <v>1001171827</v>
+        <v>1001172264</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H22" s="30"/>
     </row>
@@ -2008,20 +1924,20 @@
         <v>18</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="25">
-        <v>1001171828</v>
+        <v>1001172266</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H23" s="32"/>
     </row>
@@ -2030,20 +1946,20 @@
         <v>19</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22">
-        <v>1001171830</v>
+        <v>1001172398</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H24" s="30"/>
     </row>
@@ -2052,459 +1968,195 @@
         <v>20</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="25">
-        <v>1001171833</v>
+        <v>1001172406</v>
       </c>
       <c r="F25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="34"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="29">
+        <v>1</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22">
+        <v>1001172249</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="32"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="29">
-        <v>21</v>
-      </c>
-      <c r="B26" s="20" t="s">
+      <c r="G27" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="31">
+        <v>2</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25">
+        <v>1001172257</v>
+      </c>
+      <c r="F28" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22">
-        <v>1001171835</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="30"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="31">
-        <v>22</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25">
-        <v>1001171838</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="32"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="29">
-        <v>23</v>
-      </c>
-      <c r="B28" s="20" t="s">
+      <c r="G28" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="29">
+        <v>3</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22">
-        <v>1001171842</v>
-      </c>
-      <c r="F28" s="20" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="22">
+        <v>1001172261</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="31">
-        <v>24</v>
-      </c>
-      <c r="B29" s="23" t="s">
+      <c r="G29" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>4</v>
+      </c>
+      <c r="B30" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C30" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25">
-        <v>1001171867</v>
-      </c>
-      <c r="F29" s="23" t="s">
+      <c r="D30" s="24"/>
+      <c r="E30" s="25">
+        <v>1001172267</v>
+      </c>
+      <c r="F30" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G29" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="32"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="29">
-        <v>25</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22">
-        <v>1001172016</v>
-      </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="32"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" s="30"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="31">
-        <v>26</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25">
-        <v>1001172045</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" s="32"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="29">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22">
-        <v>1001172086</v>
+        <v>1001171678</v>
       </c>
       <c r="F32" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="35">
+        <v>1</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="38">
+        <v>1001171375</v>
+      </c>
+      <c r="F34" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="G32" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="30"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="31">
-        <v>28</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25">
-        <v>1001172087</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="32"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="29">
-        <v>29</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22">
-        <v>1001172089</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H34" s="30"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="31">
-        <v>30</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25">
-        <v>1001172093</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H35" s="32"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="29">
-        <v>31</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="22">
-        <v>1001172096</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="30"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="31">
-        <v>32</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25">
-        <v>1001172099</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" s="32"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="34"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="29">
-        <v>1</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22">
-        <v>1001171826</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="30"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="34"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="29">
-        <v>1</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22">
-        <v>1001171807</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="H41" s="30"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="31">
-        <v>2</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="24"/>
-      <c r="E42" s="25">
-        <v>1001171821</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H42" s="32"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="29">
-        <v>3</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22">
-        <v>1001172092</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="H43" s="30"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="31">
-        <v>4</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25">
-        <v>1001172117</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="32"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="34"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="35">
-        <v>1</v>
-      </c>
-      <c r="B46" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" s="37"/>
-      <c r="E46" s="38">
-        <v>1001172085</v>
-      </c>
-      <c r="F46" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="39"/>
+      <c r="H34" s="39"/>
     </row>
     <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C52" s="46" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
@@ -2514,302 +2166,325 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="40" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="G53" s="42" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="41" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="C54" s="51" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="E54" s="45" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="F54" s="44" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="G54" s="44" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H54" s="52"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55" s="40" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="C55" s="49" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="G55" s="42" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="H55" s="50"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="41" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="E56" s="45" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="F56" s="44" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="G56" s="44" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="H56" s="52"/>
     </row>
-    <row r="57" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B57" s="40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D57" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="E57" s="54"/>
-      <c r="F57" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="G57" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="H57" s="57"/>
-    </row>
-    <row r="58" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B58" s="58" t="s">
-        <v>146</v>
-      </c>
-      <c r="C58" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="D58" s="62"/>
-      <c r="E58" s="62"/>
-      <c r="F58" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="G58" s="4"/>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="59"/>
-      <c r="C59" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="69"/>
+        <v>95</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="H57" s="50"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="H58" s="52"/>
+    </row>
+    <row r="59" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C59" s="53"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="54"/>
+      <c r="F59" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="G59" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="H59" s="57"/>
     </row>
     <row r="60" spans="2:8" ht="16" x14ac:dyDescent="0.35">
       <c r="B60" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="69"/>
+      <c r="C60" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="62"/>
+      <c r="E60" s="62"/>
+      <c r="F60" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="5"/>
     </row>
     <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="60"/>
+      <c r="B61" s="59"/>
       <c r="C61" s="63" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="D61" s="64"/>
       <c r="E61" s="64"/>
       <c r="F61" s="68" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="69"/>
     </row>
-    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C62" s="64" t="s">
-        <v>154</v>
+    <row r="62" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B62" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="63" t="s">
+        <v>122</v>
       </c>
       <c r="D62" s="64"/>
       <c r="E62" s="64"/>
       <c r="F62" s="68" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="69"/>
     </row>
-    <row r="63" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="75" t="s">
-        <v>159</v>
-      </c>
-      <c r="C63" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="70" t="s">
-        <v>156</v>
-      </c>
-      <c r="G63" s="10"/>
-      <c r="H63" s="71"/>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="60"/>
+      <c r="C63" s="63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="68" t="s">
+        <v>124</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="69"/>
     </row>
     <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="76" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F64" s="72" t="s">
-        <v>158</v>
-      </c>
-      <c r="G64" s="73"/>
-      <c r="H64" s="74"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="77" t="s">
-        <v>163</v>
-      </c>
-      <c r="C66" s="77"/>
+      <c r="C64" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="64"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="69"/>
+    </row>
+    <row r="65" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B65" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="65"/>
+      <c r="E65" s="65"/>
+      <c r="F65" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="G65" s="10"/>
+      <c r="H65" s="71"/>
+    </row>
+    <row r="66" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="E66" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="G66" s="73"/>
+      <c r="H66" s="74"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="77"/>
-      <c r="C67" s="77"/>
+      <c r="B67" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" s="17"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="C68" s="78"/>
-      <c r="E68" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="F68" s="78"/>
-      <c r="G68" s="78"/>
-      <c r="H68" s="78"/>
+      <c r="B68" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="77"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D69" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="71" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B71" s="75" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="79">
+      <c r="B69" s="77"/>
+      <c r="C69" s="77"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B70" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="78"/>
+      <c r="E70" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" s="78"/>
+      <c r="G70" s="78"/>
+      <c r="H70" s="78"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D71" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E71" s="17"/>
+    </row>
+    <row r="72" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="73" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B73" s="75" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B74" s="79">
         <v>45573</v>
       </c>
-      <c r="E72" s="78" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="78"/>
+      <c r="E74" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="F74" s="78"/>
+      <c r="G74" s="78"/>
+      <c r="H74" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="E72:H72"/>
+  <mergeCells count="60">
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="E74:H74"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="E70:H70"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="F63:H63"/>
+    <mergeCell ref="C64:E64"/>
     <mergeCell ref="F64:H64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G59:H59"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="F60:H60"/>
     <mergeCell ref="C61:E61"/>
     <mergeCell ref="F61:H61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:H40"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A31:H31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="A33:H33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A26:H26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C17:D17"/>

</xml_diff>

<commit_message>
Change MYSQL client, Income text box is disable when not needed.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\OneDrive\Документы\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEBA47A-8620-43B0-BE7D-36365865115B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="650" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A66EF075-5A04-42D5-9A55-96A165C5CB19}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,226 +65,229 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>172,25 лв.</t>
-  </si>
-  <si>
-    <t>Чери и Ко ЕООД</t>
-  </si>
-  <si>
-    <t>Бирария Трафа - Овча купел</t>
-  </si>
-  <si>
-    <t>91,74 лв.</t>
-  </si>
-  <si>
-    <t>Пешева Ми 96 ЕООД</t>
-  </si>
-  <si>
-    <t>Бакалин</t>
-  </si>
-  <si>
-    <t>126,54 лв.</t>
-  </si>
-  <si>
-    <t>Момо М ЕООД</t>
-  </si>
-  <si>
-    <t>Хотел Горна Баня</t>
-  </si>
-  <si>
-    <t>404,16 лв.</t>
-  </si>
-  <si>
-    <t>Трасе ООД</t>
-  </si>
-  <si>
-    <t>Гастро Бар Трасе</t>
-  </si>
-  <si>
-    <t>91,18 лв.</t>
-  </si>
-  <si>
-    <t>Стобис ООД</t>
-  </si>
-  <si>
-    <t>Хранителен Магазин - СБА Стобис</t>
-  </si>
-  <si>
-    <t>235,39 лв.</t>
+    <t>0,00 лв.</t>
+  </si>
+  <si>
+    <t>Сохо Кафе ООД</t>
+  </si>
+  <si>
+    <t>Сохо Кафе - МОЛ България</t>
+  </si>
+  <si>
+    <t>98,50 лв.</t>
+  </si>
+  <si>
+    <t>Десерт Архитектура ООД</t>
+  </si>
+  <si>
+    <t>Пекарна - цех</t>
+  </si>
+  <si>
+    <t>339,29 лв.</t>
+  </si>
+  <si>
+    <t>Зефир 2002 - Жанел 2000 ДЗЗД</t>
+  </si>
+  <si>
+    <t>Бианко Карело</t>
+  </si>
+  <si>
+    <t>355,85 лв.</t>
+  </si>
+  <si>
+    <t>Франджипани ООД</t>
+  </si>
+  <si>
+    <t>Сно Бар</t>
+  </si>
+  <si>
+    <t>115,66 лв.</t>
+  </si>
+  <si>
+    <t>Градски Хан ООД</t>
+  </si>
+  <si>
+    <t>Градски Хан</t>
+  </si>
+  <si>
+    <t>145,16 лв.</t>
+  </si>
+  <si>
+    <t>Старата Италия ЕООД</t>
+  </si>
+  <si>
+    <t>Старата италия</t>
+  </si>
+  <si>
+    <t>79,43 лв.</t>
+  </si>
+  <si>
+    <t>Давчеви ООД</t>
+  </si>
+  <si>
+    <t>Паперино</t>
+  </si>
+  <si>
+    <t>74,40 лв.</t>
+  </si>
+  <si>
+    <t>ГМ Група ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Алекзандър</t>
+  </si>
+  <si>
+    <t>370,82 лв.</t>
   </si>
   <si>
     <t>Маги - ИВ ЕООД</t>
   </si>
   <si>
-    <t>Пицария Ветрило - Борово</t>
-  </si>
-  <si>
-    <t>75,85 лв.</t>
-  </si>
-  <si>
-    <t>Жа Ни Комерс 2016 ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Дъ Ринг</t>
-  </si>
-  <si>
-    <t>126,98 лв.</t>
-  </si>
-  <si>
-    <t>Зебрано 1 ООД</t>
-  </si>
-  <si>
-    <t>Ола - МОЛ България</t>
-  </si>
-  <si>
-    <t>122,88 лв.</t>
-  </si>
-  <si>
-    <t>Хранителен Магазин - Стобис Борово</t>
-  </si>
-  <si>
-    <t>293,98 лв.</t>
-  </si>
-  <si>
-    <t>Додо - Мирослав Дунеловски ЕТ</t>
-  </si>
-  <si>
-    <t>Додо - Мирослав Дунеловски</t>
-  </si>
-  <si>
-    <t>609,84 лв.</t>
-  </si>
-  <si>
-    <t>Пи Ем Фууд ЕООД</t>
-  </si>
-  <si>
-    <t>Хасиенда</t>
-  </si>
-  <si>
-    <t>114,71 лв.</t>
-  </si>
-  <si>
-    <t>Хранителен Магазин - Стобис Лагера</t>
-  </si>
-  <si>
-    <t>294,21 лв.</t>
-  </si>
-  <si>
-    <t>АК Фемили ООД</t>
-  </si>
-  <si>
-    <t>Пицария - Красно село</t>
-  </si>
-  <si>
-    <t>249,60 лв.</t>
-  </si>
-  <si>
     <t>Пицария Ветрило - Стрелбище</t>
   </si>
   <si>
-    <t>157,99 лв.</t>
-  </si>
-  <si>
-    <t>Групата БГ  ЕООД</t>
-  </si>
-  <si>
-    <t>Кайро Релакс Бар</t>
-  </si>
-  <si>
-    <t>213,83 лв.</t>
-  </si>
-  <si>
-    <t>126,07 лв.</t>
-  </si>
-  <si>
-    <t>Бримекс ЕООД</t>
-  </si>
-  <si>
-    <t>Пекарна Бримекс</t>
-  </si>
-  <si>
-    <t>77,77 лв.</t>
-  </si>
-  <si>
-    <t>109,22 лв.</t>
-  </si>
-  <si>
-    <t>Пица Енд Бабълс ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Енд Бабълс</t>
-  </si>
-  <si>
-    <t>1 523,80 лв.</t>
-  </si>
-  <si>
-    <t>Ем Найт Фууд ООД</t>
-  </si>
-  <si>
-    <t>Инсомния - Овча Купел</t>
+    <t>425,27 лв.</t>
+  </si>
+  <si>
+    <t>СК Сървиз ЕООД</t>
+  </si>
+  <si>
+    <t>Спагети Къмпани - МОЛ България</t>
+  </si>
+  <si>
+    <t>162,78 лв.</t>
+  </si>
+  <si>
+    <t>Густо Гурме ЕООД</t>
+  </si>
+  <si>
+    <t>Густо Гурме</t>
+  </si>
+  <si>
+    <t>628,32 лв.</t>
+  </si>
+  <si>
+    <t>МД-МГ ООД</t>
+  </si>
+  <si>
+    <t>Пица на дърва - Павлово</t>
+  </si>
+  <si>
+    <t>246,18 лв.</t>
+  </si>
+  <si>
+    <t>Давиан ООД</t>
+  </si>
+  <si>
+    <t>Адоро - Нишава</t>
+  </si>
+  <si>
+    <t>306,23 лв.</t>
+  </si>
+  <si>
+    <t>Пица Миа 2022 ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Миа София - Овча купел</t>
+  </si>
+  <si>
+    <t>792,88 лв.</t>
+  </si>
+  <si>
+    <t>Валпо ЕООД</t>
+  </si>
+  <si>
+    <t>Махана Винаената - Овча купел</t>
+  </si>
+  <si>
+    <t>159,96 лв.</t>
+  </si>
+  <si>
+    <t>Пица на дърва - Красно село</t>
+  </si>
+  <si>
+    <t>27,53 лв.</t>
+  </si>
+  <si>
+    <t>201,82 лв.</t>
+  </si>
+  <si>
+    <t>101,72 лв.</t>
+  </si>
+  <si>
+    <t>Антик 2020 ЕООД</t>
+  </si>
+  <si>
+    <t>Бар и Динър Антик</t>
+  </si>
+  <si>
+    <t>545,81 лв.</t>
+  </si>
+  <si>
+    <t>Мелинс ООД</t>
+  </si>
+  <si>
+    <t>Фейс - Горна баня</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>94,04 лв.</t>
+    <t>82,49 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
+    <t>Арт 2000 ООД</t>
+  </si>
+  <si>
+    <t>Виктория - Абакус</t>
+  </si>
+  <si>
+    <t>231,54 лв.</t>
+  </si>
+  <si>
     <t>Джи ЕН Продакшън ООД</t>
   </si>
   <si>
     <t>Неро Фор Хоум</t>
   </si>
   <si>
-    <t>318,52 лв.</t>
-  </si>
-  <si>
-    <t>Сепарит ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Розе</t>
-  </si>
-  <si>
-    <t>291,12 лв.</t>
-  </si>
-  <si>
-    <t>Планината ЕООД</t>
-  </si>
-  <si>
-    <t>Магазин Монте</t>
-  </si>
-  <si>
-    <t>356,39 лв.</t>
-  </si>
-  <si>
-    <t>Перфето БГ ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Перфетто</t>
-  </si>
-  <si>
-    <t>Кредитни известия</t>
-  </si>
-  <si>
-    <t>Кредитно</t>
-  </si>
-  <si>
-    <t>-111,56 лв.</t>
+    <t>175,97 лв.</t>
+  </si>
+  <si>
+    <t>Слокоша ЕООД</t>
+  </si>
+  <si>
+    <t>Бесо</t>
+  </si>
+  <si>
+    <t>128,59 лв.</t>
+  </si>
+  <si>
+    <t>Хайв Айти ЕООД</t>
+  </si>
+  <si>
+    <t>Артизан Фактори</t>
+  </si>
+  <si>
+    <t>Стари сметки</t>
+  </si>
+  <si>
+    <t>319,78 лв.</t>
+  </si>
+  <si>
+    <t>Зефир 2002 ООД</t>
+  </si>
+  <si>
+    <t>Механа Каруцата</t>
   </si>
   <si>
     <t>Неплатени</t>
   </si>
   <si>
-    <t>Интер Гардън ООД</t>
-  </si>
-  <si>
-    <t>161,60 лв.</t>
-  </si>
-  <si>
-    <t>0,00 лв.</t>
+    <t>258,55 лв.</t>
   </si>
   <si>
     <t>В брой</t>
@@ -293,100 +296,55 @@
     <t>Отчет на парите</t>
   </si>
   <si>
-    <t>1 -</t>
-  </si>
-  <si>
-    <t>0,02 лв.</t>
-  </si>
-  <si>
-    <t>2 -</t>
-  </si>
-  <si>
-    <t>0,05 лв.</t>
-  </si>
-  <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>6 -</t>
-  </si>
-  <si>
-    <t>0,60 лв.</t>
-  </si>
-  <si>
-    <t>9 -</t>
-  </si>
-  <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>1,80 лв.</t>
-  </si>
-  <si>
-    <t>4 -</t>
-  </si>
-  <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>8 -</t>
-  </si>
-  <si>
-    <t>1,00 лв.</t>
-  </si>
-  <si>
-    <t>8,00 лв.</t>
-  </si>
-  <si>
-    <t>4,00 лв.</t>
+    <t>3 -</t>
   </si>
   <si>
     <t>5,00 лв.</t>
   </si>
   <si>
+    <t>15,00 лв.</t>
+  </si>
+  <si>
+    <t>16 -</t>
+  </si>
+  <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>38 -</t>
-  </si>
-  <si>
-    <t>380,00 лв.</t>
-  </si>
-  <si>
-    <t>45 -</t>
+    <t>160,00 лв.</t>
+  </si>
+  <si>
+    <t>36 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>900,00 лв.</t>
-  </si>
-  <si>
-    <t>70 -</t>
+    <t>720,00 лв.</t>
+  </si>
+  <si>
+    <t>62 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>3 500,00 лв.</t>
-  </si>
-  <si>
-    <t>3 -</t>
+    <t>3 100,00 лв.</t>
+  </si>
+  <si>
+    <t>15 -</t>
   </si>
   <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>300,00 лв.</t>
+    <t>1 500,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>5 106,52 лв.</t>
+    <t>5 495,00 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -398,7 +356,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>6 439,66 лв.</t>
+    <t>6 054,75 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -410,25 +368,22 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>1 060,07 лв.</t>
+    <t>618,59 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
-    <t>111,56 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>5 106,43 лв.</t>
-  </si>
-  <si>
-    <t>Ресто:</t>
-  </si>
-  <si>
-    <t>0,09 лв.</t>
+    <t>5 497,39 лв.</t>
+  </si>
+  <si>
+    <t>Задължение:</t>
+  </si>
+  <si>
+    <t>2,39 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -1460,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1496,7 +1451,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45573</v>
+        <v>45576</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1557,7 +1512,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001171380</v>
+        <v>920857</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1579,7 +1534,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001171393</v>
+        <v>1001173106</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1601,7 +1556,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001171394</v>
+        <v>1001173200</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1623,7 +1578,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001171399</v>
+        <v>1001173202</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
@@ -1645,7 +1600,7 @@
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001172196</v>
+        <v>1001173205</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>21</v>
@@ -1667,7 +1622,7 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001172197</v>
+        <v>1001173206</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>24</v>
@@ -1689,7 +1644,7 @@
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001172198</v>
+        <v>1001173207</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>27</v>
@@ -1711,7 +1666,7 @@
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001172201</v>
+        <v>1001173209</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>30</v>
@@ -1726,14 +1681,14 @@
         <v>9</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001172205</v>
+        <v>1001173210</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>33</v>
@@ -1748,20 +1703,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001172208</v>
+        <v>1001173224</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H15" s="32"/>
     </row>
@@ -1770,20 +1725,20 @@
         <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001172215</v>
+        <v>1001173233</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H16" s="30"/>
     </row>
@@ -1792,20 +1747,20 @@
         <v>12</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="25">
-        <v>1001172217</v>
+        <v>1001173236</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H17" s="32"/>
     </row>
@@ -1814,20 +1769,20 @@
         <v>13</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
-        <v>1001172250</v>
+        <v>1001173253</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H18" s="30"/>
     </row>
@@ -1836,20 +1791,20 @@
         <v>14</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="25">
-        <v>1001172251</v>
+        <v>1001173426</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H19" s="32"/>
     </row>
@@ -1858,20 +1813,20 @@
         <v>15</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
-        <v>1001172258</v>
+        <v>1001173427</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H20" s="30"/>
     </row>
@@ -1880,20 +1835,20 @@
         <v>16</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="25">
-        <v>1001172262</v>
+        <v>1001173429</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H21" s="32"/>
     </row>
@@ -1902,20 +1857,20 @@
         <v>17</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
-        <v>1001172264</v>
+        <v>1001173430</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H22" s="30"/>
     </row>
@@ -1924,20 +1879,20 @@
         <v>18</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="25">
-        <v>1001172266</v>
+        <v>1001173433</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H23" s="32"/>
     </row>
@@ -1946,20 +1901,20 @@
         <v>19</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22">
-        <v>1001172398</v>
+        <v>1001173434</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H24" s="30"/>
     </row>
@@ -1968,26 +1923,26 @@
         <v>20</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="25">
-        <v>1001172406</v>
+        <v>1001173437</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -2002,20 +1957,20 @@
         <v>1</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="22">
-        <v>1001172249</v>
+        <v>1001173213</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H27" s="30"/>
     </row>
@@ -2024,20 +1979,20 @@
         <v>2</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="25">
-        <v>1001172257</v>
+        <v>1001173215</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H28" s="32"/>
     </row>
@@ -2046,20 +2001,20 @@
         <v>3</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="22">
-        <v>1001172261</v>
+        <v>1001173226</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H29" s="30"/>
     </row>
@@ -2068,26 +2023,26 @@
         <v>4</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="25">
-        <v>1001172267</v>
+        <v>1001173441</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="33" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -2102,26 +2057,26 @@
         <v>1</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="22">
-        <v>1001171678</v>
+        <v>1001171618</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H32" s="30"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="33" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -2139,24 +2094,24 @@
         <v>80</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D34" s="37"/>
       <c r="E34" s="38">
-        <v>1001171375</v>
+        <v>1001173431</v>
       </c>
       <c r="F34" s="36" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="H34" s="39"/>
     </row>
     <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C52" s="46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
@@ -2166,315 +2121,238 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="F53" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="42" t="s">
         <v>97</v>
-      </c>
-      <c r="G53" s="42" t="s">
-        <v>101</v>
       </c>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="41" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C54" s="51" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E54" s="45" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="F54" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="54"/>
+      <c r="F55" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G54" s="44" t="s">
+      <c r="H55" s="57"/>
+    </row>
+    <row r="56" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B56" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="H54" s="52"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B55" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C55" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="E55" s="43" t="s">
+      <c r="C56" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="62"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="59"/>
+      <c r="C57" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="69"/>
+    </row>
+    <row r="58" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B58" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="F55" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G55" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="H55" s="50"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B56" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="E56" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="F56" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G56" s="44" t="s">
+      <c r="C58" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="H56" s="52"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B57" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="E57" s="43" t="s">
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="69"/>
+    </row>
+    <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="60"/>
+      <c r="C59" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="F57" s="42" t="s">
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="G57" s="42" t="s">
+      <c r="G59" s="1"/>
+      <c r="H59" s="69"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C60" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="H57" s="50"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B58" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="E58" s="45" t="s">
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B61" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="F58" s="44" t="s">
+      <c r="D61" s="65"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="G58" s="44" t="s">
+      <c r="G61" s="10"/>
+      <c r="H61" s="71"/>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="H58" s="52"/>
-    </row>
-    <row r="59" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C59" s="53"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="55" t="s">
+      <c r="F62" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="G59" s="56" t="s">
-        <v>116</v>
-      </c>
-      <c r="H59" s="57"/>
-    </row>
-    <row r="60" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B60" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="61" t="s">
+      <c r="G62" s="73"/>
+      <c r="H62" s="74"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B63" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D60" s="62"/>
-      <c r="E60" s="62"/>
-      <c r="F60" s="67" t="s">
+      <c r="E63" s="17"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="G60" s="4"/>
-      <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="59"/>
-      <c r="C61" s="63" t="s">
+      <c r="C64" s="77"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="77"/>
+      <c r="C65" s="77"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="69"/>
-    </row>
-    <row r="62" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B62" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="C62" s="63" t="s">
+      <c r="C66" s="78"/>
+      <c r="E66" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="F66" s="78"/>
+      <c r="G66" s="78"/>
+      <c r="H66" s="78"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D67" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="69"/>
-    </row>
-    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="60"/>
-      <c r="C63" s="63" t="s">
+      <c r="E67" s="17"/>
+    </row>
+    <row r="68" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="69" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B69" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="68" t="s">
-        <v>124</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="69"/>
-    </row>
-    <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C64" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="D64" s="64"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="G64" s="1"/>
-      <c r="H64" s="69"/>
-    </row>
-    <row r="65" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="C65" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="65"/>
-      <c r="E65" s="65"/>
-      <c r="F65" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="G65" s="10"/>
-      <c r="H65" s="71"/>
-    </row>
-    <row r="66" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="76" t="s">
-        <v>132</v>
-      </c>
-      <c r="E66" s="66" t="s">
-        <v>129</v>
-      </c>
-      <c r="F66" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="G66" s="73"/>
-      <c r="H66" s="74"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="C68" s="77"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B69" s="77"/>
-      <c r="C69" s="77"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B70" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="C70" s="78"/>
+    </row>
+    <row r="70" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="79">
+        <v>45579</v>
+      </c>
       <c r="E70" s="78" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="F70" s="78"/>
       <c r="G70" s="78"/>
       <c r="H70" s="78"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D71" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E71" s="17"/>
-    </row>
-    <row r="72" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="73" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B73" s="75" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="79">
-        <v>45573</v>
-      </c>
-      <c r="E74" s="78" t="s">
-        <v>136</v>
-      </c>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-    </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="E74:H74"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
     <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C69"/>
-    <mergeCell ref="B70:C70"/>
     <mergeCell ref="E70:H70"/>
-    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
     <mergeCell ref="F62:H62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B64:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="E66:H66"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="A31:H31"/>

</xml_diff>

<commit_message>
Add icon to navigation buttons.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="650" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A66EF075-5A04-42D5-9A55-96A165C5CB19}"/>
+  <xr:revisionPtr revIDLastSave="696" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21E4185-112C-4440-8342-219698703682}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,271 +65,238 @@
     <t>Плащане в брой</t>
   </si>
   <si>
+    <t>2 299,78 лв.</t>
+  </si>
+  <si>
+    <t>Фуудс 1990 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Данте</t>
+  </si>
+  <si>
+    <t>404,20 лв.</t>
+  </si>
+  <si>
+    <t>Пици Викторов ЕООД</t>
+  </si>
+  <si>
+    <t>Пица на дърва</t>
+  </si>
+  <si>
+    <t>1 401,66 лв.</t>
+  </si>
+  <si>
+    <t>Мартини БГ ООД</t>
+  </si>
+  <si>
+    <t>Мартини Бар Варна</t>
+  </si>
+  <si>
+    <t>Плащане по банка</t>
+  </si>
+  <si>
+    <t>236,29 лв.</t>
+  </si>
+  <si>
+    <t>Банка</t>
+  </si>
+  <si>
+    <t>Вазаро Комерс ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Вазаро</t>
+  </si>
+  <si>
+    <t>2 246,22 лв.</t>
+  </si>
+  <si>
+    <t>Трънчев ООД</t>
+  </si>
+  <si>
+    <t>Магазин Булмаг</t>
+  </si>
+  <si>
+    <t>1 061,65 лв.</t>
+  </si>
+  <si>
+    <t>Море 2020 ООД</t>
+  </si>
+  <si>
+    <t>Стария Чинар Черно Море</t>
+  </si>
+  <si>
+    <t>316,92 лв.</t>
+  </si>
+  <si>
+    <t>Лагардер Травъл Ритейл ЕООД</t>
+  </si>
+  <si>
+    <t>Уан минът ЕС253 Добрич</t>
+  </si>
+  <si>
+    <t>617,74 лв.</t>
+  </si>
+  <si>
+    <t>Грийн Марк ООД</t>
+  </si>
+  <si>
+    <t>Грийн Марк</t>
+  </si>
+  <si>
+    <t>11 324,09 лв.</t>
+  </si>
+  <si>
+    <t>Хепи Лейди ООД</t>
+  </si>
+  <si>
+    <t>Хепи кухня майка</t>
+  </si>
+  <si>
+    <t>5 175,01 лв.</t>
+  </si>
+  <si>
+    <t>Едеа Ритейл АД</t>
+  </si>
+  <si>
+    <t>Едеа Магарин Русе</t>
+  </si>
+  <si>
+    <t>1 637,96 лв.</t>
+  </si>
+  <si>
+    <t>220,02 лв.</t>
+  </si>
+  <si>
+    <t>Барико Просеко Бар</t>
+  </si>
+  <si>
+    <t>1 461,71 лв.</t>
+  </si>
+  <si>
+    <t>322,40 лв.</t>
+  </si>
+  <si>
+    <t>Изида ООД</t>
+  </si>
+  <si>
+    <t>Хотел Изида</t>
+  </si>
+  <si>
+    <t>1 261,22 лв.</t>
+  </si>
+  <si>
+    <t>Сабросо 2012 ООД</t>
+  </si>
+  <si>
+    <t>Бурата</t>
+  </si>
+  <si>
+    <t>1 033,86 лв.</t>
+  </si>
+  <si>
+    <t>Железов 2017 ЕООД</t>
+  </si>
+  <si>
+    <t>Борса Дева</t>
+  </si>
+  <si>
+    <t>2 407,63 лв.</t>
+  </si>
+  <si>
+    <t>112,46 лв.</t>
+  </si>
+  <si>
+    <t>2 059,86 лв.</t>
+  </si>
+  <si>
+    <t>Триада -ГТ ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Триада</t>
+  </si>
+  <si>
+    <t>Кредитни известия</t>
+  </si>
+  <si>
+    <t>Кредитно</t>
+  </si>
+  <si>
+    <t>487,87 лв.</t>
+  </si>
+  <si>
+    <t>304,92 лв.</t>
+  </si>
+  <si>
+    <t>11,35 лв.</t>
+  </si>
+  <si>
+    <t>12,86 лв.</t>
+  </si>
+  <si>
+    <t>157,03 лв.</t>
+  </si>
+  <si>
+    <t>14,06 лв.</t>
+  </si>
+  <si>
+    <t>75,48 лв.</t>
+  </si>
+  <si>
+    <t>825,90 лв.</t>
+  </si>
+  <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Сохо Кафе ООД</t>
-  </si>
-  <si>
-    <t>Сохо Кафе - МОЛ България</t>
-  </si>
-  <si>
-    <t>98,50 лв.</t>
-  </si>
-  <si>
-    <t>Десерт Архитектура ООД</t>
-  </si>
-  <si>
-    <t>Пекарна - цех</t>
-  </si>
-  <si>
-    <t>339,29 лв.</t>
-  </si>
-  <si>
-    <t>Зефир 2002 - Жанел 2000 ДЗЗД</t>
-  </si>
-  <si>
-    <t>Бианко Карело</t>
-  </si>
-  <si>
-    <t>355,85 лв.</t>
-  </si>
-  <si>
-    <t>Франджипани ООД</t>
-  </si>
-  <si>
-    <t>Сно Бар</t>
-  </si>
-  <si>
-    <t>115,66 лв.</t>
-  </si>
-  <si>
-    <t>Градски Хан ООД</t>
-  </si>
-  <si>
-    <t>Градски Хан</t>
-  </si>
-  <si>
-    <t>145,16 лв.</t>
-  </si>
-  <si>
-    <t>Старата Италия ЕООД</t>
-  </si>
-  <si>
-    <t>Старата италия</t>
-  </si>
-  <si>
-    <t>79,43 лв.</t>
-  </si>
-  <si>
-    <t>Давчеви ООД</t>
-  </si>
-  <si>
-    <t>Паперино</t>
-  </si>
-  <si>
-    <t>74,40 лв.</t>
-  </si>
-  <si>
-    <t>ГМ Група ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Алекзандър</t>
-  </si>
-  <si>
-    <t>370,82 лв.</t>
-  </si>
-  <si>
-    <t>Маги - ИВ ЕООД</t>
-  </si>
-  <si>
-    <t>Пицария Ветрило - Стрелбище</t>
-  </si>
-  <si>
-    <t>425,27 лв.</t>
-  </si>
-  <si>
-    <t>СК Сървиз ЕООД</t>
-  </si>
-  <si>
-    <t>Спагети Къмпани - МОЛ България</t>
-  </si>
-  <si>
-    <t>162,78 лв.</t>
-  </si>
-  <si>
-    <t>Густо Гурме ЕООД</t>
-  </si>
-  <si>
-    <t>Густо Гурме</t>
-  </si>
-  <si>
-    <t>628,32 лв.</t>
-  </si>
-  <si>
-    <t>МД-МГ ООД</t>
-  </si>
-  <si>
-    <t>Пица на дърва - Павлово</t>
-  </si>
-  <si>
-    <t>246,18 лв.</t>
-  </si>
-  <si>
-    <t>Давиан ООД</t>
-  </si>
-  <si>
-    <t>Адоро - Нишава</t>
-  </si>
-  <si>
-    <t>306,23 лв.</t>
-  </si>
-  <si>
-    <t>Пица Миа 2022 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Миа София - Овча купел</t>
-  </si>
-  <si>
-    <t>792,88 лв.</t>
-  </si>
-  <si>
-    <t>Валпо ЕООД</t>
-  </si>
-  <si>
-    <t>Махана Винаената - Овча купел</t>
-  </si>
-  <si>
-    <t>159,96 лв.</t>
-  </si>
-  <si>
-    <t>Пица на дърва - Красно село</t>
-  </si>
-  <si>
-    <t>27,53 лв.</t>
-  </si>
-  <si>
-    <t>201,82 лв.</t>
-  </si>
-  <si>
-    <t>101,72 лв.</t>
-  </si>
-  <si>
-    <t>Антик 2020 ЕООД</t>
-  </si>
-  <si>
-    <t>Бар и Динър Антик</t>
-  </si>
-  <si>
-    <t>545,81 лв.</t>
-  </si>
-  <si>
-    <t>Мелинс ООД</t>
-  </si>
-  <si>
-    <t>Фейс - Горна баня</t>
-  </si>
-  <si>
-    <t>Плащане по банка</t>
-  </si>
-  <si>
-    <t>82,49 лв.</t>
-  </si>
-  <si>
-    <t>Банка</t>
-  </si>
-  <si>
-    <t>Арт 2000 ООД</t>
-  </si>
-  <si>
-    <t>Виктория - Абакус</t>
-  </si>
-  <si>
-    <t>231,54 лв.</t>
-  </si>
-  <si>
-    <t>Джи ЕН Продакшън ООД</t>
-  </si>
-  <si>
-    <t>Неро Фор Хоум</t>
-  </si>
-  <si>
-    <t>175,97 лв.</t>
-  </si>
-  <si>
-    <t>Слокоша ЕООД</t>
-  </si>
-  <si>
-    <t>Бесо</t>
-  </si>
-  <si>
-    <t>128,59 лв.</t>
-  </si>
-  <si>
-    <t>Хайв Айти ЕООД</t>
-  </si>
-  <si>
-    <t>Артизан Фактори</t>
-  </si>
-  <si>
-    <t>Стари сметки</t>
-  </si>
-  <si>
-    <t>319,78 лв.</t>
-  </si>
-  <si>
-    <t>Зефир 2002 ООД</t>
-  </si>
-  <si>
-    <t>Механа Каруцата</t>
-  </si>
-  <si>
-    <t>Неплатени</t>
-  </si>
-  <si>
-    <t>258,55 лв.</t>
-  </si>
-  <si>
-    <t>В брой</t>
-  </si>
-  <si>
     <t>Отчет на парите</t>
   </si>
   <si>
-    <t>3 -</t>
+    <t>1 -</t>
+  </si>
+  <si>
+    <t>0,05 лв.</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>10 -</t>
+  </si>
+  <si>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
   </si>
   <si>
     <t>5,00 лв.</t>
   </si>
   <si>
-    <t>15,00 лв.</t>
-  </si>
-  <si>
-    <t>16 -</t>
+    <t>4 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>160,00 лв.</t>
-  </si>
-  <si>
-    <t>36 -</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>720,00 лв.</t>
-  </si>
-  <si>
-    <t>62 -</t>
+    <t>40,00 лв.</t>
+  </si>
+  <si>
+    <t>27 -</t>
+  </si>
+  <si>
+    <t>540,00 лв.</t>
+  </si>
+  <si>
+    <t>40 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>3 100,00 лв.</t>
+    <t>2 000,00 лв.</t>
   </si>
   <si>
     <t>15 -</t>
@@ -344,7 +311,7 @@
     <t>Тотал:</t>
   </si>
   <si>
-    <t>5 495,00 лв.</t>
+    <t>4 105,65 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -356,7 +323,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>6 054,75 лв.</t>
+    <t>35 600,68 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -368,7 +335,7 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>618,59 лв.</t>
+    <t>31 495,04 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -377,19 +344,19 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>5 497,39 лв.</t>
-  </si>
-  <si>
-    <t>Задължение:</t>
-  </si>
-  <si>
-    <t>2,39 лв.</t>
+    <t>4 105,64 лв.</t>
+  </si>
+  <si>
+    <t>Ресто:</t>
+  </si>
+  <si>
+    <t>0,01 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
   </si>
   <si>
-    <t>СВ 3856 ХА</t>
+    <t>СА 2241 КК</t>
   </si>
   <si>
     <t>Съставил отчета / Предал:</t>
@@ -1415,7 +1382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1451,7 +1418,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45576</v>
+        <v>45582</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1512,7 +1479,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>920857</v>
+        <v>1001174480</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1534,7 +1501,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001173106</v>
+        <v>1001174502</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1556,7 +1523,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001173200</v>
+        <v>1001174505</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1567,294 +1534,284 @@
       <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="31">
-        <v>4</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25">
-        <v>1001173202</v>
-      </c>
-      <c r="F9" s="23" t="s">
+      <c r="A9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="32"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001173205</v>
+        <v>1001174465</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>25</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001173206</v>
+        <v>1001174466</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001173207</v>
+        <v>1001174468</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="31">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>32</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001173209</v>
+        <v>1001174470</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>34</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>35</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001173210</v>
+        <v>1001174481</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>38</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001173224</v>
+        <v>1001174489</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001173233</v>
+        <v>1001174497</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="31">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="25">
-        <v>1001173236</v>
+        <v>1001174498</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
-        <v>1001173253</v>
+        <v>1001174517</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="25">
-        <v>1001173426</v>
+        <v>1001174521</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
-        <v>1001173427</v>
+        <v>1001174527</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="31">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D21" s="24"/>
       <c r="E21" s="25">
-        <v>1001173429</v>
+        <v>1001174545</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>52</v>
@@ -1864,85 +1821,85 @@
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
-        <v>1001173430</v>
+        <v>1001174549</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="H22" s="30"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="25">
-        <v>1001173433</v>
+        <v>1001174550</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="29">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="22">
-        <v>1001173434</v>
+        <v>1001174551</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="H24" s="30"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="31">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="25">
-        <v>1001173437</v>
+        <v>1001174553</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -1957,20 +1914,20 @@
         <v>1</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="22">
-        <v>1001173213</v>
+        <v>1001173973</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H27" s="30"/>
     </row>
@@ -1979,20 +1936,20 @@
         <v>2</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="25">
-        <v>1001173215</v>
+        <v>1001173974</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H28" s="32"/>
     </row>
@@ -2001,20 +1958,20 @@
         <v>3</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="22">
-        <v>1001173226</v>
+        <v>1001174047</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H29" s="30"/>
     </row>
@@ -2023,95 +1980,137 @@
         <v>4</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="D30" s="24"/>
       <c r="E30" s="25">
-        <v>1001173441</v>
+        <v>1001174048</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G30" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="32"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="29">
+        <v>5</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22">
+        <v>1001174053</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="30"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="31">
+        <v>6</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25">
+        <v>1001174058</v>
+      </c>
+      <c r="F32" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="H30" s="32"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="34"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="29">
-        <v>1</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22">
-        <v>1001171618</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" s="30"/>
+      <c r="G32" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="34"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="35">
-        <v>1</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38">
-        <v>1001173431</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G34" s="36" t="s">
+      <c r="A33" s="29">
+        <v>7</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22">
+        <v>1001174059</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="31">
+        <v>8</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25">
+        <v>1001174060</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="32"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="35">
         <v>9</v>
       </c>
-      <c r="H34" s="39"/>
+      <c r="B35" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="37"/>
+      <c r="E35" s="38">
+        <v>1001174258</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H35" s="39"/>
     </row>
     <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C52" s="46" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
@@ -2121,243 +2120,286 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="40" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="G53" s="42" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="51" t="s">
+      <c r="H56" s="52"/>
+    </row>
+    <row r="57" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="44" t="s">
+      <c r="G57" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="E54" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54" s="52"/>
-    </row>
-    <row r="55" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="54"/>
-      <c r="F55" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="G55" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="H55" s="57"/>
-    </row>
-    <row r="56" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B56" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
-      <c r="F56" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="G56" s="4"/>
-      <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="59"/>
-      <c r="C57" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="D57" s="64"/>
-      <c r="E57" s="64"/>
-      <c r="F57" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="G57" s="1"/>
-      <c r="H57" s="69"/>
+      <c r="H57" s="57"/>
     </row>
     <row r="58" spans="2:8" ht="16" x14ac:dyDescent="0.35">
       <c r="B58" s="58" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="C58" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="5"/>
     </row>
     <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="60"/>
+      <c r="B59" s="59"/>
       <c r="C59" s="63" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D59" s="64"/>
       <c r="E59" s="64"/>
       <c r="F59" s="68" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="69"/>
     </row>
-    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C60" s="64" t="s">
-        <v>111</v>
+    <row r="60" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B60" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="63" t="s">
+        <v>97</v>
       </c>
       <c r="D60" s="64"/>
       <c r="E60" s="64"/>
       <c r="F60" s="68" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="69"/>
     </row>
-    <row r="61" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B61" s="75" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="65" t="s">
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="60"/>
+      <c r="C61" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C62" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="69"/>
+    </row>
+    <row r="63" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
+      <c r="F63" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="71"/>
+    </row>
+    <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="66" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="G64" s="73"/>
+      <c r="H64" s="74"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="77"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="77"/>
+      <c r="C67" s="77"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="78"/>
+      <c r="E68" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D69" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B71" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65"/>
-      <c r="F61" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="G61" s="10"/>
-      <c r="H61" s="71"/>
-    </row>
-    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="76" t="s">
-        <v>117</v>
-      </c>
-      <c r="E62" s="66" t="s">
-        <v>114</v>
-      </c>
-      <c r="F62" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="G62" s="73"/>
-      <c r="H62" s="74"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B63" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" s="17"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B64" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="77"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="77"/>
-      <c r="C65" s="77"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" s="78"/>
-      <c r="E66" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="F66" s="78"/>
-      <c r="G66" s="78"/>
-      <c r="H66" s="78"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D67" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="69" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B69" s="75" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="79">
-        <v>45579</v>
-      </c>
-      <c r="E70" s="78" t="s">
-        <v>121</v>
-      </c>
-      <c r="F70" s="78"/>
-      <c r="G70" s="78"/>
-      <c r="H70" s="78"/>
+    </row>
+    <row r="72" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="79">
+        <v>45583</v>
+      </c>
+      <c r="E72" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="78"/>
+      <c r="G72" s="78"/>
+      <c r="H72" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="E70:H70"/>
+  <mergeCells count="61">
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
     <mergeCell ref="C61:E61"/>
     <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C62:E62"/>
     <mergeCell ref="F62:H62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B64:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="E66:H66"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G57:H57"/>
     <mergeCell ref="C58:E58"/>
     <mergeCell ref="F58:H58"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="F59:H59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:H57"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
@@ -2381,7 +2423,7 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
Create conection whit delita_db. All entities in application automatic save in data base. Delete old file data base.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="696" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BC60B60-01B5-4D19-AC6F-9D611B756FDA}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30DFB605-A444-4059-B9B5-F461E61B9516}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,277 +65,247 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>2 299,78 лв.</t>
-  </si>
-  <si>
-    <t>Фуудс 1990 ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Данте</t>
-  </si>
-  <si>
-    <t>404,20 лв.</t>
-  </si>
-  <si>
-    <t>Пици Викторов ЕООД</t>
-  </si>
-  <si>
-    <t>Пица на дърва</t>
-  </si>
-  <si>
-    <t>1 401,66 лв.</t>
-  </si>
-  <si>
-    <t>Мартини БГ ООД</t>
-  </si>
-  <si>
-    <t>Мартини Бар Варна</t>
+    <t>171,52 лв.</t>
+  </si>
+  <si>
+    <t>Джеси - 1987 ООД</t>
+  </si>
+  <si>
+    <t>Кафе Гирос Диамандис</t>
+  </si>
+  <si>
+    <t>200,51 лв.</t>
+  </si>
+  <si>
+    <t>Тибора ЕООД</t>
+  </si>
+  <si>
+    <t>Кафе Аморе</t>
+  </si>
+  <si>
+    <t>687,87 лв.</t>
+  </si>
+  <si>
+    <t>Елби Строй ЕООД</t>
+  </si>
+  <si>
+    <t>Дийп Диш</t>
+  </si>
+  <si>
+    <t>51,20 лв.</t>
+  </si>
+  <si>
+    <t>85,04 лв.</t>
+  </si>
+  <si>
+    <t>Па 2016 ООД</t>
+  </si>
+  <si>
+    <t>Пепино кафе бар</t>
+  </si>
+  <si>
+    <t>150,48 лв.</t>
+  </si>
+  <si>
+    <t>Бенита 1 ЕООД</t>
+  </si>
+  <si>
+    <t>Томасаки Суши - Перник</t>
+  </si>
+  <si>
+    <t>296,22 лв.</t>
+  </si>
+  <si>
+    <t>Кофи Хаус Парк Бар ЕООД</t>
+  </si>
+  <si>
+    <t>Парк Бар</t>
+  </si>
+  <si>
+    <t>300,42 лв.</t>
+  </si>
+  <si>
+    <t>Адеа Индъстри 2013 ЕООД</t>
+  </si>
+  <si>
+    <t>Шот Спот</t>
+  </si>
+  <si>
+    <t>164,66 лв.</t>
+  </si>
+  <si>
+    <t>Аполон-92 ООД</t>
+  </si>
+  <si>
+    <t>Хапка Любов</t>
+  </si>
+  <si>
+    <t>392,56 лв.</t>
+  </si>
+  <si>
+    <t>Цех</t>
+  </si>
+  <si>
+    <t>245,62 лв.</t>
+  </si>
+  <si>
+    <t>Еко Чек ООД</t>
+  </si>
+  <si>
+    <t>Киндър Айлънд</t>
+  </si>
+  <si>
+    <t>172,67 лв.</t>
+  </si>
+  <si>
+    <t>Попов Мениджмънт ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Сенсо</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>236,29 лв.</t>
+    <t>913,92 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Вазаро Комерс ООД</t>
-  </si>
-  <si>
-    <t>Дистрибутор Вазаро</t>
-  </si>
-  <si>
-    <t>2 246,22 лв.</t>
-  </si>
-  <si>
-    <t>Трънчев ООД</t>
-  </si>
-  <si>
-    <t>Магазин Булмаг</t>
-  </si>
-  <si>
-    <t>1 061,65 лв.</t>
-  </si>
-  <si>
-    <t>Море 2020 ООД</t>
-  </si>
-  <si>
-    <t>Стария Чинар Черно Море</t>
-  </si>
-  <si>
-    <t>316,92 лв.</t>
+    <t>Дрийм Кейкс ЕООД</t>
+  </si>
+  <si>
+    <t>Романс сладкарски цех</t>
+  </si>
+  <si>
+    <t>378,57 лв.</t>
+  </si>
+  <si>
+    <t>Сиа Бейкъри ООД</t>
+  </si>
+  <si>
+    <t>БГ пица скуул - Ади</t>
+  </si>
+  <si>
+    <t>1 108,11 лв.</t>
+  </si>
+  <si>
+    <t>Грийн Марк Логистика ООД</t>
+  </si>
+  <si>
+    <t>Грийн Марк Логистика</t>
+  </si>
+  <si>
+    <t>1 071,31 лв.</t>
+  </si>
+  <si>
+    <t>2 503,24 лв.</t>
   </si>
   <si>
     <t>Лагардер Травъл Ритейл ЕООД</t>
   </si>
   <si>
-    <t>Уан минът ЕС253 Добрич</t>
-  </si>
-  <si>
-    <t>617,74 лв.</t>
-  </si>
-  <si>
-    <t>Грийн Марк ООД</t>
-  </si>
-  <si>
-    <t>Грийн Марк</t>
-  </si>
-  <si>
-    <t>11 324,09 лв.</t>
-  </si>
-  <si>
-    <t>Хепи Лейди ООД</t>
-  </si>
-  <si>
-    <t>Хепи кухня майка</t>
-  </si>
-  <si>
-    <t>5 175,01 лв.</t>
-  </si>
-  <si>
-    <t>Едеа Ритейл АД</t>
-  </si>
-  <si>
-    <t>Едеа Магарин Русе</t>
-  </si>
-  <si>
-    <t>1 637,96 лв.</t>
-  </si>
-  <si>
-    <t>220,02 лв.</t>
-  </si>
-  <si>
-    <t>Барико Просеко Бар</t>
-  </si>
-  <si>
-    <t>1 461,71 лв.</t>
-  </si>
-  <si>
-    <t>322,40 лв.</t>
-  </si>
-  <si>
-    <t>Изида ООД</t>
-  </si>
-  <si>
-    <t>Хотел Изида</t>
-  </si>
-  <si>
-    <t>1 261,22 лв.</t>
-  </si>
-  <si>
-    <t>Сабросо 2012 ООД</t>
-  </si>
-  <si>
-    <t>Бурата</t>
-  </si>
-  <si>
-    <t>1 033,86 лв.</t>
-  </si>
-  <si>
-    <t>Железов 2017 ЕООД</t>
-  </si>
-  <si>
-    <t>Борса Дева</t>
-  </si>
-  <si>
-    <t>2 407,63 лв.</t>
-  </si>
-  <si>
-    <t>112,46 лв.</t>
-  </si>
-  <si>
-    <t>2 059,86 лв.</t>
-  </si>
-  <si>
-    <t>Триада -ГТ ООД</t>
-  </si>
-  <si>
-    <t>Дистрибутор Триада</t>
-  </si>
-  <si>
-    <t>Кредитни известия</t>
-  </si>
-  <si>
-    <t>Кредитно</t>
-  </si>
-  <si>
-    <t>487,87 лв.</t>
-  </si>
-  <si>
-    <t>304,92 лв.</t>
-  </si>
-  <si>
-    <t>11,35 лв.</t>
-  </si>
-  <si>
-    <t>12,86 лв.</t>
-  </si>
-  <si>
-    <t>157,03 лв.</t>
-  </si>
-  <si>
-    <t>14,06 лв.</t>
-  </si>
-  <si>
-    <t>75,48 лв.</t>
-  </si>
-  <si>
-    <t>825,90 лв.</t>
+    <t>Онда Кафе - Кухня Майка</t>
+  </si>
+  <si>
+    <t>Отчет на парите</t>
+  </si>
+  <si>
+    <t>1 -</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>0,20 лв.</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>11 -</t>
+  </si>
+  <si>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>11,00 лв.</t>
+  </si>
+  <si>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
+    <t>5,00 лв.</t>
+  </si>
+  <si>
+    <t>39 -</t>
+  </si>
+  <si>
+    <t>10,00 лв.</t>
+  </si>
+  <si>
+    <t>390,00 лв.</t>
+  </si>
+  <si>
+    <t>43 -</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
+  </si>
+  <si>
+    <t>860,00 лв.</t>
+  </si>
+  <si>
+    <t>15 -</t>
+  </si>
+  <si>
+    <t>50,00 лв.</t>
+  </si>
+  <si>
+    <t>750,00 лв.</t>
+  </si>
+  <si>
+    <t>9 -</t>
+  </si>
+  <si>
+    <t>100,00 лв.</t>
+  </si>
+  <si>
+    <t>900,00 лв.</t>
+  </si>
+  <si>
+    <t>Тотал:</t>
+  </si>
+  <si>
+    <t>2 918,80 лв.</t>
+  </si>
+  <si>
+    <t>Преброена сума</t>
+  </si>
+  <si>
+    <t>Разлика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общо приходи от доставки: </t>
+  </si>
+  <si>
+    <t>8 893,92 лв.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общо приходи от стари сметки: </t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Отчет на парите</t>
-  </si>
-  <si>
-    <t>1 -</t>
-  </si>
-  <si>
-    <t>0,05 лв.</t>
-  </si>
-  <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>10 -</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>5,00 лв.</t>
-  </si>
-  <si>
-    <t>4 -</t>
-  </si>
-  <si>
-    <t>10,00 лв.</t>
-  </si>
-  <si>
-    <t>40,00 лв.</t>
-  </si>
-  <si>
-    <t>27 -</t>
-  </si>
-  <si>
-    <t>540,00 лв.</t>
-  </si>
-  <si>
-    <t>40 -</t>
-  </si>
-  <si>
-    <t>50,00 лв.</t>
-  </si>
-  <si>
-    <t>2 000,00 лв.</t>
-  </si>
-  <si>
-    <t>15 -</t>
-  </si>
-  <si>
-    <t>100,00 лв.</t>
-  </si>
-  <si>
-    <t>1 500,00 лв.</t>
-  </si>
-  <si>
-    <t>Тотал:</t>
-  </si>
-  <si>
-    <t>4 105,65 лв.</t>
-  </si>
-  <si>
-    <t>Преброена сума</t>
-  </si>
-  <si>
-    <t>Разлика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Общо приходи от доставки: </t>
-  </si>
-  <si>
-    <t>35 600,68 лв.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Общо приходи от стари сметки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Сума от неплатени сметки: </t>
   </si>
   <si>
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>31 495,04 лв.</t>
+    <t>5 975,15 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -344,19 +314,19 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>4 105,64 лв.</t>
+    <t>2 918,77 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,01 лв.</t>
+    <t>0,03 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
   </si>
   <si>
-    <t>СА 2241 КК</t>
+    <t>СВ 2241 КК</t>
   </si>
   <si>
     <t>Съставил отчета / Предал:</t>
@@ -1382,7 +1352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1418,7 +1388,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45582</v>
+        <v>45611</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1479,7 +1449,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001174480</v>
+        <v>1001181970</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1501,7 +1471,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001174502</v>
+        <v>1001181972</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1523,7 +1493,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001174505</v>
+        <v>1001181975</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1534,881 +1504,628 @@
       <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31">
+        <v>4</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25">
+        <v>1001181976</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="34"/>
+      <c r="G9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>22</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001174465</v>
+        <v>1001181998</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>25</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001174466</v>
+        <v>1001181999</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="29">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>28</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001174468</v>
+        <v>1001182003</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="31">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>31</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001174470</v>
+        <v>1001182030</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="29">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>34</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001174481</v>
+        <v>1001182060</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H14" s="30"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001174489</v>
+        <v>1001182061</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="29">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001174497</v>
+        <v>1001182062</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="31">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="25">
-        <v>1001174498</v>
+        <v>1001182079</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="29">
-        <v>9</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="21" t="s">
+      <c r="A18" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="34"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>1</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22">
+        <v>1001181971</v>
+      </c>
+      <c r="F19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22">
-        <v>1001174517</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="31">
-        <v>10</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25">
-        <v>1001174521</v>
-      </c>
-      <c r="F19" s="23" t="s">
+      <c r="G19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="32"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="29">
-        <v>11</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="A20" s="31">
+        <v>2</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25">
+        <v>1001181988</v>
+      </c>
+      <c r="F20" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22">
-        <v>1001174527</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="30"/>
+      <c r="G20" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="31">
-        <v>12</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="A21" s="29">
+        <v>3</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22">
+        <v>1001181994</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25">
-        <v>1001174545</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="32"/>
+      <c r="G21" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="29">
-        <v>13</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="A22" s="31">
+        <v>4</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="D22" s="24"/>
+      <c r="E22" s="25">
+        <v>1001182106</v>
+      </c>
+      <c r="F22" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22">
-        <v>1001174549</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="31">
-        <v>14</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25">
-        <v>1001174550</v>
-      </c>
-      <c r="F23" s="23" t="s">
+      <c r="G22" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="35">
+        <v>5</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38">
+        <v>1001182114</v>
+      </c>
+      <c r="F23" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="32"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="29">
-        <v>15</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22">
-        <v>1001174551</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="30"/>
+      <c r="G23" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="39"/>
+    </row>
+    <row r="24" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C24" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="31">
-        <v>16</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25">
-        <v>1001174553</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="32"/>
+      <c r="C25" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="34"/>
+      <c r="B26" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="52"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="29">
-        <v>1</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22">
-        <v>1001173973</v>
-      </c>
-      <c r="F27" s="20" t="s">
+      <c r="B27" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="30"/>
+      <c r="D27" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="31">
-        <v>2</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25">
-        <v>1001173974</v>
-      </c>
-      <c r="F28" s="23" t="s">
+      <c r="B28" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="H28" s="32"/>
+      <c r="C28" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="52"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="29">
-        <v>3</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22">
-        <v>1001174047</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H29" s="30"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="31">
-        <v>4</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B29" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25">
-        <v>1001174048</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" s="32"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="29">
-        <v>5</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22">
-        <v>1001174053</v>
-      </c>
-      <c r="F31" s="20" t="s">
+      <c r="C29" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="30"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="31">
-        <v>6</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25">
-        <v>1001174058</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="H32" s="32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="29">
-        <v>7</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22">
-        <v>1001174059</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="H33" s="30"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="31">
-        <v>8</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25">
-        <v>1001174060</v>
-      </c>
-      <c r="F34" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="H34" s="32"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="35">
-        <v>9</v>
-      </c>
-      <c r="B35" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38">
-        <v>1001174258</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="H35" s="39"/>
-    </row>
-    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C52" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="48"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B53" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" s="43" t="s">
+      <c r="D29" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="50"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C30" s="53"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="F53" s="42" t="s">
+      <c r="G30" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="42" t="s">
+      <c r="H30" s="57"/>
+    </row>
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B31" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="H53" s="50"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B54" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="E54" s="45" t="s">
+      <c r="C31" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="59"/>
+      <c r="C32" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="69"/>
+    </row>
+    <row r="33" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B33" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="F54" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H54" s="52"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B55" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F55" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="G55" s="42" t="s">
+      <c r="C33" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="H55" s="50"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B56" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="44" t="s">
+      <c r="G33" s="1"/>
+      <c r="H33" s="69"/>
+    </row>
+    <row r="34" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="60"/>
+      <c r="C34" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="G56" s="44" t="s">
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="H56" s="52"/>
-    </row>
-    <row r="57" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="D57" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="54"/>
-      <c r="F57" s="55" t="s">
+      <c r="G34" s="1"/>
+      <c r="H34" s="69"/>
+    </row>
+    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="G57" s="56" t="s">
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B36" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="H57" s="57"/>
-    </row>
-    <row r="58" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B58" s="58" t="s">
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="61" t="s">
+      <c r="G36" s="10"/>
+      <c r="H36" s="71"/>
+    </row>
+    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="62"/>
-      <c r="E58" s="62"/>
-      <c r="F58" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="G58" s="4"/>
-      <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="59"/>
-      <c r="C59" s="63" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="69"/>
-    </row>
-    <row r="60" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B60" s="58" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="63" t="s">
+      <c r="G37" s="73"/>
+      <c r="H37" s="74"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="69"/>
-    </row>
-    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="60"/>
-      <c r="C61" s="63" t="s">
+      <c r="D38" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="68" t="s">
+      <c r="E38" s="17"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="69"/>
-    </row>
-    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C62" s="64" t="s">
+      <c r="C39" s="77"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="69"/>
-    </row>
-    <row r="63" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="C63" s="65" t="s">
+      <c r="C41" s="78"/>
+      <c r="E41" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="78"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="78"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D42" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="D63" s="65"/>
-      <c r="E63" s="65"/>
-      <c r="F63" s="70" t="s">
+      <c r="E42" s="17"/>
+    </row>
+    <row r="43" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B44" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="G63" s="10"/>
-      <c r="H63" s="71"/>
-    </row>
-    <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="76" t="s">
-        <v>106</v>
-      </c>
-      <c r="E64" s="66" t="s">
-        <v>103</v>
-      </c>
-      <c r="F64" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="G64" s="73"/>
-      <c r="H64" s="74"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E65" s="17"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="77" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="77"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="77"/>
-      <c r="C67" s="77"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="78"/>
-      <c r="E68" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="F68" s="78"/>
-      <c r="G68" s="78"/>
-      <c r="H68" s="78"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D69" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69" s="17"/>
-    </row>
-    <row r="70" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="71" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B71" s="75" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="79">
-        <v>45583</v>
-      </c>
-      <c r="E72" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="78"/>
+    </row>
+    <row r="45" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="79">
+        <v>45614</v>
+      </c>
+      <c r="E45" s="78" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:H68"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+  <mergeCells count="49">
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B39:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
@@ -2423,7 +2140,7 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>

<commit_message>
Refactoring method that check if invoice is exists and if it is already pay in another day report using SQL procedure.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="547" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30DFB605-A444-4059-B9B5-F461E61B9516}"/>
+  <xr:revisionPtr revIDLastSave="622" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9741D463-F7A1-4056-9734-E1B3B1CA1180}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,220 +65,235 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>171,52 лв.</t>
-  </si>
-  <si>
-    <t>Джеси - 1987 ООД</t>
-  </si>
-  <si>
-    <t>Кафе Гирос Диамандис</t>
-  </si>
-  <si>
-    <t>200,51 лв.</t>
-  </si>
-  <si>
-    <t>Тибора ЕООД</t>
-  </si>
-  <si>
-    <t>Кафе Аморе</t>
-  </si>
-  <si>
-    <t>687,87 лв.</t>
-  </si>
-  <si>
-    <t>Елби Строй ЕООД</t>
-  </si>
-  <si>
-    <t>Дийп Диш</t>
-  </si>
-  <si>
-    <t>51,20 лв.</t>
-  </si>
-  <si>
-    <t>85,04 лв.</t>
-  </si>
-  <si>
-    <t>Па 2016 ООД</t>
-  </si>
-  <si>
-    <t>Пепино кафе бар</t>
-  </si>
-  <si>
-    <t>150,48 лв.</t>
-  </si>
-  <si>
-    <t>Бенита 1 ЕООД</t>
-  </si>
-  <si>
-    <t>Томасаки Суши - Перник</t>
-  </si>
-  <si>
-    <t>296,22 лв.</t>
-  </si>
-  <si>
-    <t>Кофи Хаус Парк Бар ЕООД</t>
-  </si>
-  <si>
-    <t>Парк Бар</t>
-  </si>
-  <si>
-    <t>300,42 лв.</t>
-  </si>
-  <si>
-    <t>Адеа Индъстри 2013 ЕООД</t>
-  </si>
-  <si>
-    <t>Шот Спот</t>
-  </si>
-  <si>
-    <t>164,66 лв.</t>
-  </si>
-  <si>
-    <t>Аполон-92 ООД</t>
-  </si>
-  <si>
-    <t>Хапка Любов</t>
-  </si>
-  <si>
-    <t>392,56 лв.</t>
-  </si>
-  <si>
-    <t>Цех</t>
-  </si>
-  <si>
-    <t>245,62 лв.</t>
-  </si>
-  <si>
-    <t>Еко Чек ООД</t>
-  </si>
-  <si>
-    <t>Киндър Айлънд</t>
-  </si>
-  <si>
-    <t>172,67 лв.</t>
-  </si>
-  <si>
-    <t>Попов Мениджмънт ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Сенсо</t>
+    <t>499,40 лв.</t>
+  </si>
+  <si>
+    <t>Дар-Ко Трейд 2018 ЕООД</t>
+  </si>
+  <si>
+    <t>Дар-Ко Трейд - Шумен</t>
+  </si>
+  <si>
+    <t>1 648,96 лв.</t>
+  </si>
+  <si>
+    <t>Фуудс 1990 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Данте</t>
+  </si>
+  <si>
+    <t>173,28 лв.</t>
+  </si>
+  <si>
+    <t>Бизнес Клуб - Валентина Петрова ЕООД</t>
+  </si>
+  <si>
+    <t>Бизнес хотел Валентина</t>
+  </si>
+  <si>
+    <t>327,24 лв.</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>913,92 лв.</t>
+    <t>501,30 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Дрийм Кейкс ЕООД</t>
-  </si>
-  <si>
-    <t>Романс сладкарски цех</t>
-  </si>
-  <si>
-    <t>378,57 лв.</t>
-  </si>
-  <si>
-    <t>Сиа Бейкъри ООД</t>
-  </si>
-  <si>
-    <t>БГ пица скуул - Ади</t>
-  </si>
-  <si>
-    <t>1 108,11 лв.</t>
-  </si>
-  <si>
-    <t>Грийн Марк Логистика ООД</t>
-  </si>
-  <si>
-    <t>Грийн Марк Логистика</t>
-  </si>
-  <si>
-    <t>1 071,31 лв.</t>
-  </si>
-  <si>
-    <t>2 503,24 лв.</t>
-  </si>
-  <si>
     <t>Лагардер Травъл Ритейл ЕООД</t>
   </si>
   <si>
-    <t>Онда Кафе - Кухня Майка</t>
+    <t>Уан минът ЕС253 Добрич</t>
+  </si>
+  <si>
+    <t>366,26 лв.</t>
+  </si>
+  <si>
+    <t>Изида ООД</t>
+  </si>
+  <si>
+    <t>Хотел Изида</t>
+  </si>
+  <si>
+    <t>467,32 лв.</t>
+  </si>
+  <si>
+    <t>Кафе Експрес ООД</t>
+  </si>
+  <si>
+    <t>Капитан Кук</t>
+  </si>
+  <si>
+    <t>280,24 лв.</t>
+  </si>
+  <si>
+    <t>Хаус Маркет България АД</t>
+  </si>
+  <si>
+    <t>Икеа Варна</t>
+  </si>
+  <si>
+    <t>2 295,37 лв.</t>
+  </si>
+  <si>
+    <t>Грийн Марк ООД</t>
+  </si>
+  <si>
+    <t>Грийн Марк</t>
+  </si>
+  <si>
+    <t>947,56 лв.</t>
+  </si>
+  <si>
+    <t>Трънчев ООД</t>
+  </si>
+  <si>
+    <t>Магазин Булмаг</t>
+  </si>
+  <si>
+    <t>1 277,24 лв.</t>
+  </si>
+  <si>
+    <t>Мартини БГ ООД</t>
+  </si>
+  <si>
+    <t>Мартини Бар Варна</t>
+  </si>
+  <si>
+    <t>2 938,37 лв.</t>
+  </si>
+  <si>
+    <t>Триада -ГТ ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Триада</t>
+  </si>
+  <si>
+    <t>287,06 лв.</t>
+  </si>
+  <si>
+    <t>10 014,03 лв.</t>
+  </si>
+  <si>
+    <t>1 217,44 лв.</t>
+  </si>
+  <si>
+    <t>Хепи Лейди ООД</t>
+  </si>
+  <si>
+    <t>Хепи кухня майка</t>
+  </si>
+  <si>
+    <t>1 179,55 лв.</t>
+  </si>
+  <si>
+    <t>Сабросо 2012 ООД</t>
+  </si>
+  <si>
+    <t>Бурата</t>
+  </si>
+  <si>
+    <t>328,31 лв.</t>
+  </si>
+  <si>
+    <t>1 039,82 лв.</t>
+  </si>
+  <si>
+    <t>Железов 2017 ЕООД</t>
+  </si>
+  <si>
+    <t>Борса Дева</t>
+  </si>
+  <si>
+    <t>1 539,80 лв.</t>
+  </si>
+  <si>
+    <t>28,21 лв.</t>
+  </si>
+  <si>
+    <t>253,52 лв.</t>
+  </si>
+  <si>
+    <t>78,62 лв.</t>
+  </si>
+  <si>
+    <t>72,23 лв.</t>
   </si>
   <si>
     <t>Отчет на парите</t>
   </si>
   <si>
+    <t>6 -</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>0,60 лв.</t>
+  </si>
+  <si>
+    <t>4 -</t>
+  </si>
+  <si>
+    <t>0,20 лв.</t>
+  </si>
+  <si>
+    <t>0,80 лв.</t>
+  </si>
+  <si>
+    <t>7 -</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>3,50 лв.</t>
+  </si>
+  <si>
+    <t>2 -</t>
+  </si>
+  <si>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
     <t>1 -</t>
   </si>
   <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>11 -</t>
-  </si>
-  <si>
-    <t>1,00 лв.</t>
-  </si>
-  <si>
-    <t>11,00 лв.</t>
-  </si>
-  <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>5,00 лв.</t>
-  </si>
-  <si>
-    <t>39 -</t>
-  </si>
-  <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>390,00 лв.</t>
-  </si>
-  <si>
-    <t>43 -</t>
-  </si>
-  <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>860,00 лв.</t>
-  </si>
-  <si>
-    <t>15 -</t>
+    <t>24 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>750,00 лв.</t>
-  </si>
-  <si>
-    <t>9 -</t>
+    <t>1 200,00 лв.</t>
+  </si>
+  <si>
+    <t>14 -</t>
   </si>
   <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>900,00 лв.</t>
+    <t>1 400,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>2 918,80 лв.</t>
+    <t>2 648,90 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -290,7 +305,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>8 893,92 лв.</t>
+    <t>27 761,13 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -305,7 +320,7 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>5 975,15 лв.</t>
+    <t>25 112,25 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -314,13 +329,13 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>2 918,77 лв.</t>
+    <t>2 648,88 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,03 лв.</t>
+    <t>0,02 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -1352,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1388,7 +1403,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45611</v>
+        <v>45617</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1449,7 +1464,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001181970</v>
+        <v>1001183392</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1471,7 +1486,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001181972</v>
+        <v>1001183394</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1493,7 +1508,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001181975</v>
+        <v>1001183395</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1508,14 +1523,14 @@
         <v>4</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001181976</v>
+        <v>1001183401</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
@@ -1526,262 +1541,262 @@
       <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
+      <c r="A10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22">
+        <v>1001183380</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="31">
+        <v>2</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25">
+        <v>1001183385</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
+        <v>3</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22">
+        <v>1001183387</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>4</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25">
+        <v>1001183388</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
         <v>5</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="21" t="s">
+      <c r="B15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22">
+        <v>1001183400</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22">
-        <v>1001181998</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="31">
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="31">
         <v>6</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25">
-        <v>1001181999</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
+      <c r="B16" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25">
+        <v>1001183414</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
         <v>7</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22">
-        <v>1001182003</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="31">
+      <c r="B17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22">
+        <v>1001183422</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="31">
         <v>8</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25">
-        <v>1001182030</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="29">
-        <v>9</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22">
-        <v>1001182060</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="31">
-        <v>10</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25">
-        <v>1001182061</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
-        <v>11</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22">
-        <v>1001182062</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="31">
-        <v>12</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25">
-        <v>1001182079</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
+      <c r="B18" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25">
+        <v>1001183431</v>
+      </c>
+      <c r="F18" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="34"/>
+      <c r="G18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="32"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="29">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="22">
-        <v>1001181971</v>
+        <v>1001183433</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H19" s="30"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="25">
-        <v>1001181988</v>
+        <v>1001183434</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="29">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="22">
-        <v>1001181994</v>
+        <v>1001183435</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="31">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>51</v>
@@ -1791,341 +1806,466 @@
       </c>
       <c r="D22" s="24"/>
       <c r="E22" s="25">
-        <v>1001182106</v>
+        <v>1001183437</v>
       </c>
       <c r="F22" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="29">
+        <v>13</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22">
+        <v>1001183445</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="H22" s="32"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="35">
-        <v>5</v>
-      </c>
-      <c r="B23" s="36" t="s">
+      <c r="G23" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="31">
+        <v>14</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C24" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38">
-        <v>1001182114</v>
-      </c>
-      <c r="F23" s="36" t="s">
+      <c r="D24" s="24"/>
+      <c r="E24" s="25">
+        <v>1001183449</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="39"/>
-    </row>
-    <row r="24" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C24" s="46" t="s">
+      <c r="G24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="32"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="29">
+        <v>15</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22">
+        <v>1001183453</v>
+      </c>
+      <c r="F25" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="40" t="s">
+      <c r="G25" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
+        <v>16</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25">
+        <v>1001183454</v>
+      </c>
+      <c r="F26" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="G26" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="29">
+        <v>17</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22">
+        <v>1001183466</v>
+      </c>
+      <c r="F27" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="42" t="s">
+      <c r="G27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="31">
+        <v>18</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25">
+        <v>1001183469</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="35">
+        <v>19</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38">
+        <v>1001183508</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="39"/>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="H53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="50"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B26" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="E26" s="45" t="s">
+      <c r="C54" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="D54" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="44" t="s">
+      <c r="E54" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="52"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="43" t="s">
+      <c r="C55" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="D55" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="42" t="s">
+      <c r="E55" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="45" t="s">
+      <c r="C56" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="44" t="s">
+      <c r="D56" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="E56" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F56" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56" s="52"/>
+    </row>
+    <row r="57" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="53"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="57"/>
-    </row>
-    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B31" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="67" t="s">
+      <c r="C57" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="54"/>
+      <c r="F57" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="59"/>
-      <c r="C32" s="63" t="s">
+      <c r="G57" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="68" t="s">
+      <c r="H57" s="57"/>
+    </row>
+    <row r="58" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B58" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="69"/>
-    </row>
-    <row r="33" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B33" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="63" t="s">
+      <c r="C58" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="59"/>
+      <c r="C59" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="69"/>
+    </row>
+    <row r="60" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B60" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="69"/>
-    </row>
-    <row r="34" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="60"/>
-      <c r="C34" s="63" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="69"/>
-    </row>
-    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C35" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="69"/>
-    </row>
-    <row r="36" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B36" s="75" t="s">
+      <c r="C60" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="60"/>
+      <c r="C61" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C62" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="71"/>
-    </row>
-    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="76" t="s">
+      <c r="G62" s="1"/>
+      <c r="H62" s="69"/>
+    </row>
+    <row r="63" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="75" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" s="72" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="73"/>
-      <c r="H37" s="74"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B38" s="18" t="s">
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
+      <c r="F63" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="G63" s="10"/>
+      <c r="H63" s="71"/>
+    </row>
+    <row r="64" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="E64" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="17"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B39" s="77" t="s">
+      <c r="F64" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="77"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" s="78"/>
-      <c r="E41" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D42" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" s="17"/>
-    </row>
-    <row r="43" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B44" s="75" t="s">
+      <c r="G64" s="73"/>
+      <c r="H64" s="74"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="18" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="79">
-        <v>45614</v>
-      </c>
-      <c r="E45" s="78" t="s">
-        <v>100</v>
-      </c>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
+      <c r="D65" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="17"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="77"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="77"/>
+      <c r="C67" s="77"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="78"/>
+      <c r="E68" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="F68" s="78"/>
+      <c r="G68" s="78"/>
+      <c r="H68" s="78"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D69" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="17"/>
+    </row>
+    <row r="70" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B71" s="75" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="79">
+        <v>45618</v>
+      </c>
+      <c r="E72" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" s="78"/>
+      <c r="G72" s="78"/>
+      <c r="H72" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B39:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
+  <mergeCells count="55">
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
@@ -2141,7 +2281,7 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>

<commit_message>
Create application host and remove config in to. Companies, objects and traders now work with EF Core.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{99DC7265-1D0E-46FF-A801-6BD8AEB0A3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="690" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0FB1B63-4907-4C96-A0E2-E66CBEF6F779}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,46 +65,172 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>5 108,60 лв.</t>
-  </si>
-  <si>
-    <t>Ай Пи Фууд 2012 ООД</t>
-  </si>
-  <si>
-    <t>Ай Пи Фууд - Разлог</t>
-  </si>
-  <si>
-    <t>8 402,30 лв.</t>
-  </si>
-  <si>
-    <t>Тиенди ООД</t>
-  </si>
-  <si>
-    <t>Тиенди - Разлог</t>
+    <t>469,96 лв.</t>
+  </si>
+  <si>
+    <t>Пици Викторов ЕООД</t>
+  </si>
+  <si>
+    <t>Пица на дърва</t>
+  </si>
+  <si>
+    <t>3 186,47 лв.</t>
+  </si>
+  <si>
+    <t>Фуудс 1990 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Данте</t>
+  </si>
+  <si>
+    <t>603,48 лв.</t>
+  </si>
+  <si>
+    <t>Никгра ЕООД</t>
+  </si>
+  <si>
+    <t>Никгра - Дистрибутор Шумен</t>
+  </si>
+  <si>
+    <t>47,11 лв.</t>
+  </si>
+  <si>
+    <t>1 509,25 лв.</t>
+  </si>
+  <si>
+    <t>40,08 лв.</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>543,08 лв.</t>
+    <t>2 089,28 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Вит-Маркет ООД</t>
-  </si>
-  <si>
-    <t>Вит Маркет - Разлог</t>
-  </si>
-  <si>
-    <t>6 584,10 лв.</t>
-  </si>
-  <si>
-    <t>Равани ЕООД</t>
-  </si>
-  <si>
-    <t>Равани - Благоевград</t>
+    <t>Море 2020 ООД</t>
+  </si>
+  <si>
+    <t>Стария Чинар Черно Море</t>
+  </si>
+  <si>
+    <t>337,34 лв.</t>
+  </si>
+  <si>
+    <t>Живис ООД</t>
+  </si>
+  <si>
+    <t>Живис</t>
+  </si>
+  <si>
+    <t>423,91 лв.</t>
+  </si>
+  <si>
+    <t>Лагардер Травъл Ритейл ЕООД</t>
+  </si>
+  <si>
+    <t>Уан минът ЕС253 Добрич</t>
+  </si>
+  <si>
+    <t>799,55 лв.</t>
+  </si>
+  <si>
+    <t>Грийн Марк ООД</t>
+  </si>
+  <si>
+    <t>Грийн Марк</t>
+  </si>
+  <si>
+    <t>4 499,62 лв.</t>
+  </si>
+  <si>
+    <t>1 653,44 лв.</t>
+  </si>
+  <si>
+    <t>Трънчев ООД</t>
+  </si>
+  <si>
+    <t>Магазин Булмаг</t>
+  </si>
+  <si>
+    <t>1 864,52 лв.</t>
+  </si>
+  <si>
+    <t>158,63 лв.</t>
+  </si>
+  <si>
+    <t>Барико Просеко Бар</t>
+  </si>
+  <si>
+    <t>3 660,06 лв.</t>
+  </si>
+  <si>
+    <t>Триада -ГТ ООД</t>
+  </si>
+  <si>
+    <t>Дистрибутор Триада</t>
+  </si>
+  <si>
+    <t>2 765,44 лв.</t>
+  </si>
+  <si>
+    <t>Хепи Лейди ООД</t>
+  </si>
+  <si>
+    <t>Хепи кухня майка</t>
+  </si>
+  <si>
+    <t>215,86 лв.</t>
+  </si>
+  <si>
+    <t>554,47 лв.</t>
+  </si>
+  <si>
+    <t>Изида ООД</t>
+  </si>
+  <si>
+    <t>Хотел Изида</t>
+  </si>
+  <si>
+    <t>918,13 лв.</t>
+  </si>
+  <si>
+    <t>Сабросо 2012 ООД</t>
+  </si>
+  <si>
+    <t>Бурата</t>
+  </si>
+  <si>
+    <t>144,07 лв.</t>
+  </si>
+  <si>
+    <t>Кредитни известия</t>
+  </si>
+  <si>
+    <t>Кредитно</t>
+  </si>
+  <si>
+    <t>65,02 лв.</t>
+  </si>
+  <si>
+    <t>105,38 лв.</t>
+  </si>
+  <si>
+    <t>-26,30 лв.</t>
+  </si>
+  <si>
+    <t>86,41 лв.</t>
+  </si>
+  <si>
+    <t>7,03 лв.</t>
+  </si>
+  <si>
+    <t>214,26 лв.</t>
+  </si>
+  <si>
+    <t>0,00 лв.</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -113,34 +239,55 @@
     <t>1 -</t>
   </si>
   <si>
-    <t>0,10 лв.</t>
+    <t>0,05 лв.</t>
   </si>
   <si>
     <t>4 -</t>
   </si>
   <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>0,80 лв.</t>
+    <t>5,00 лв.</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
+  </si>
+  <si>
+    <t>77 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>270 -</t>
+    <t>770,00 лв.</t>
+  </si>
+  <si>
+    <t>42 -</t>
+  </si>
+  <si>
+    <t>840,00 лв.</t>
+  </si>
+  <si>
+    <t>52 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>13 500,00 лв.</t>
+    <t>2 600,00 лв.</t>
+  </si>
+  <si>
+    <t>16 -</t>
+  </si>
+  <si>
+    <t>100,00 лв.</t>
+  </si>
+  <si>
+    <t>1 600,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>13 510,90 лв.</t>
+    <t>5 830,05 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -152,25 +299,25 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>20 638,08 лв.</t>
+    <t>25 940,67 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
   </si>
   <si>
-    <t>0,00 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сума от неплатени сметки: </t>
   </si>
   <si>
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>7 127,18 лв.</t>
+    <t>20 084,32 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
+  </si>
+  <si>
+    <t>26,30 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
@@ -673,29 +820,107 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -709,6 +934,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
@@ -719,156 +953,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -886,10 +1036,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1209,11 +1355,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1227,391 +1371,1027 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="57" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72">
-        <v>45657</v>
-      </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8">
+        <v>45673</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="75" t="s">
+      <c r="G3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="77"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="74"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="78"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="61"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="3">
-        <v>1001192776</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="22">
+        <v>1001196160</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+      <c r="A7" s="31">
         <v>2</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="5">
-        <v>1001192794</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="24"/>
+      <c r="E7" s="25">
+        <v>1001196161</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="9"/>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="29">
+        <v>3</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22">
+        <v>1001196168</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="66"/>
+      <c r="G8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="31">
+        <v>4</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25">
+        <v>1001196169</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>5</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22">
+        <v>1001196170</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="31">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25">
+        <v>1001196211</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="3">
-        <v>1001192772</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="B13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22">
+        <v>1001196094</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>2</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25">
+        <v>1001196095</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
+        <v>3</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22">
+        <v>1001196096</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="31">
+        <v>4</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25">
+        <v>1001196122</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
+        <v>5</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22">
+        <v>1001196126</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="31">
+        <v>6</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25">
+        <v>1001196132</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>7</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22">
+        <v>1001196142</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="31">
+        <v>8</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25">
+        <v>1001196145</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>9</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22">
+        <v>1001196153</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="31">
+        <v>10</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25">
+        <v>1001196171</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="29">
+        <v>11</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22">
+        <v>1001196183</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="31">
+        <v>12</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25">
+        <v>1001196214</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="32"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="29">
+        <v>13</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22">
+        <v>1001196223</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
+        <v>14</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25">
+        <v>1001196230</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="29">
+        <v>1</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22">
+        <v>1001195058</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>2</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25">
+        <v>1001196102</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="32"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
+        <v>3</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="C30" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="67"/>
-      <c r="E10" s="12">
-        <v>1001192781</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="22">
+        <v>1001196108</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="31">
+        <v>4</v>
+      </c>
+      <c r="B31" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="C31" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="53"/>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B15" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="28"/>
-      <c r="C16" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
-    </row>
-    <row r="17" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B17" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
-    </row>
-    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="29"/>
-      <c r="C18" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
-    </row>
-    <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-    </row>
-    <row r="20" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B20" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37" t="s">
+      <c r="D31" s="24"/>
+      <c r="E31" s="25">
+        <v>1001196111</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="32"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="29">
+        <v>5</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
-    </row>
-    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="43"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="E25" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D26" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="34"/>
-    </row>
-    <row r="27" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B28" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="33">
-        <v>45657</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22">
+        <v>1001196112</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="31">
+        <v>6</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25">
+        <v>1001196113</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="29">
+        <v>7</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22">
+        <v>1001196194</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="31">
+        <v>8</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25">
+        <v>1001196195</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="32"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="35">
+        <v>9</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38">
+        <v>1001196196</v>
+      </c>
+      <c r="F36" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="39"/>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C56" s="53"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="G56" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56" s="57"/>
+    </row>
+    <row r="57" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B57" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="59"/>
+      <c r="C58" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="69"/>
+    </row>
+    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B59" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="69"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="60"/>
+      <c r="C60" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C61" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="71"/>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="G63" s="73"/>
+      <c r="H63" s="74"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="77" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="77"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="77"/>
+      <c r="C66" s="77"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="78"/>
+      <c r="E67" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="F67" s="78"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D68" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B70" s="75" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="79">
+        <v>45674</v>
+      </c>
+      <c r="E71" s="78" t="s">
+        <v>101</v>
+      </c>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="62">
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
@@ -1622,32 +2402,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="E25:H25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement day report exporter
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{9AE82A2D-E54D-4994-AA5E-B3565C568B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="536" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A263B01-5BE1-4BE2-9D82-32D18BC1ED4A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,289 +65,172 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>361,33 лв.</t>
-  </si>
-  <si>
-    <t>100,00 лв.</t>
-  </si>
-  <si>
-    <t>(A)--&gt;Миналият Век ЕООД</t>
-  </si>
-  <si>
-    <t>Миналият век</t>
-  </si>
-  <si>
-    <t>35,93 лв.</t>
-  </si>
-  <si>
-    <t>Фуудс 1990 ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Данте</t>
-  </si>
-  <si>
-    <t>33,22 лв.</t>
-  </si>
-  <si>
-    <t>Пици Викторов ЕООД</t>
-  </si>
-  <si>
-    <t>Пица на дърва</t>
-  </si>
-  <si>
-    <t>Плащане с карта</t>
-  </si>
-  <si>
-    <t>261,33 лв.</t>
+    <t>303,12 лв.</t>
+  </si>
+  <si>
+    <t>Каскадас Маг ЕООД</t>
+  </si>
+  <si>
+    <t>СуперМаркет Смокиня</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>1 326,83 лв.</t>
+    <t>524,97 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Порт Варна ООД</t>
-  </si>
-  <si>
-    <t>Стария чинар Варна</t>
-  </si>
-  <si>
-    <t>1 043,29 лв.</t>
-  </si>
-  <si>
-    <t>Море 2020 ООД</t>
-  </si>
-  <si>
-    <t>Стария Чинар</t>
-  </si>
-  <si>
-    <t>2 358,36 лв.</t>
-  </si>
-  <si>
-    <t>Едеа Ритейл АД</t>
-  </si>
-  <si>
-    <t>Едеа Магарин Русе</t>
-  </si>
-  <si>
-    <t>550,67 лв.</t>
-  </si>
-  <si>
-    <t>Живис ООД</t>
-  </si>
-  <si>
-    <t>Живис</t>
-  </si>
-  <si>
-    <t>1 847,33 лв.</t>
-  </si>
-  <si>
-    <t>Трънчев ООД</t>
-  </si>
-  <si>
-    <t>Магазин Булмаг</t>
-  </si>
-  <si>
-    <t>5 894,06 лв.</t>
-  </si>
-  <si>
-    <t>Хепи Лейди ООД</t>
-  </si>
-  <si>
-    <t>Хепи кухня майка</t>
-  </si>
-  <si>
-    <t>710,65 лв.</t>
-  </si>
-  <si>
-    <t>Лагардер Травъл Ритейл ЕООД</t>
-  </si>
-  <si>
-    <t>Барико Просеко Бар</t>
-  </si>
-  <si>
-    <t>2 660,79 лв.</t>
-  </si>
-  <si>
-    <t>Триада -ГТ ООД</t>
-  </si>
-  <si>
-    <t>Дистрибутор Триада</t>
-  </si>
-  <si>
-    <t>931,54 лв.</t>
-  </si>
-  <si>
-    <t>Изида ООД</t>
-  </si>
-  <si>
-    <t>Хотел Изида</t>
-  </si>
-  <si>
-    <t>148,50 лв.</t>
-  </si>
-  <si>
-    <t>Уан минът ЕС253 Добрич</t>
-  </si>
-  <si>
-    <t>1 019,03 лв.</t>
-  </si>
-  <si>
-    <t>Сабросо 2012 ООД</t>
-  </si>
-  <si>
-    <t>Бурата</t>
-  </si>
-  <si>
-    <t>79,09 лв.</t>
-  </si>
-  <si>
-    <t>Железов 2017 ЕООД</t>
-  </si>
-  <si>
-    <t>Борса Дева</t>
-  </si>
-  <si>
-    <t>189,52 лв.</t>
-  </si>
-  <si>
-    <t>3 002,29 лв.</t>
-  </si>
-  <si>
-    <t>2 222,85 лв.</t>
-  </si>
-  <si>
-    <t>201,10 лв.</t>
-  </si>
-  <si>
-    <t>Балкански Център Дипломат ООД</t>
-  </si>
-  <si>
-    <t>Дипломат Хотел</t>
-  </si>
-  <si>
-    <t>280,24 лв.</t>
-  </si>
-  <si>
-    <t>Хаус Маркет България АД</t>
-  </si>
-  <si>
-    <t>Икеа Варна</t>
-  </si>
-  <si>
-    <t>Кредитни известия</t>
-  </si>
-  <si>
-    <t>Кредитно</t>
-  </si>
-  <si>
-    <t>20,32 лв.</t>
-  </si>
-  <si>
-    <t>Неплатени</t>
-  </si>
-  <si>
-    <t>539,50 лв.</t>
-  </si>
-  <si>
-    <t>506,28 лв.</t>
-  </si>
-  <si>
-    <t>За кредитно</t>
-  </si>
-  <si>
-    <t>3 305,33 лв.</t>
-  </si>
-  <si>
-    <t>3 125,97 лв.</t>
-  </si>
-  <si>
-    <t>179,36 лв.</t>
+    <t>Брадърс Комерс ООД</t>
+  </si>
+  <si>
+    <t>Брадърс Комерс</t>
+  </si>
+  <si>
+    <t>161,68 лв.</t>
+  </si>
+  <si>
+    <t>Атрактив 2016 ООД</t>
+  </si>
+  <si>
+    <t>Пицария Уно Пю</t>
+  </si>
+  <si>
+    <t>Рестком 2 ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Алафранги</t>
+  </si>
+  <si>
+    <t>192,19 лв.</t>
+  </si>
+  <si>
+    <t>193,39 лв.</t>
+  </si>
+  <si>
+    <t>Омега - 75 Г ООД</t>
+  </si>
+  <si>
+    <t>Омега</t>
+  </si>
+  <si>
+    <t>2 915,13 лв.</t>
+  </si>
+  <si>
+    <t>Ник - Инвест - Казанлък ЕООД</t>
+  </si>
+  <si>
+    <t>Ники Инвест</t>
+  </si>
+  <si>
+    <t>775,01 лв.</t>
+  </si>
+  <si>
+    <t>229,84 лв.</t>
+  </si>
+  <si>
+    <t>Дес Комерс ООД</t>
+  </si>
+  <si>
+    <t>Дес Комерс</t>
+  </si>
+  <si>
+    <t>1 960,20 лв.</t>
+  </si>
+  <si>
+    <t>Жанет Свиленград ООД</t>
+  </si>
+  <si>
+    <t>Жанет</t>
+  </si>
+  <si>
+    <t>3 873,84 лв.</t>
+  </si>
+  <si>
+    <t>31,00 лв.</t>
+  </si>
+  <si>
+    <t>124,15 лв.</t>
+  </si>
+  <si>
+    <t>703,13 лв.</t>
+  </si>
+  <si>
+    <t>9 182,58 лв.</t>
+  </si>
+  <si>
+    <t>315,26 лв.</t>
+  </si>
+  <si>
+    <t>2 148,02 лв.</t>
+  </si>
+  <si>
+    <t>7 089,79 лв.</t>
+  </si>
+  <si>
+    <t>1 348,57 лв.</t>
+  </si>
+  <si>
+    <t>Отчет на парите</t>
+  </si>
+  <si>
+    <t>1 -</t>
+  </si>
+  <si>
+    <t>0,02 лв.</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>3 -</t>
+  </si>
+  <si>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>3,00 лв.</t>
+  </si>
+  <si>
+    <t>30 -</t>
+  </si>
+  <si>
+    <t>10,00 лв.</t>
+  </si>
+  <si>
+    <t>300,00 лв.</t>
+  </si>
+  <si>
+    <t>Тотал:</t>
+  </si>
+  <si>
+    <t>Преброена сума</t>
+  </si>
+  <si>
+    <t>Разлика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общо приходи от доставки: </t>
+  </si>
+  <si>
+    <t>32 233,55 лв.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общо приходи от стари сметки: </t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>В брой</t>
-  </si>
-  <si>
-    <t>Отчет на парите</t>
-  </si>
-  <si>
-    <t>1 -</t>
-  </si>
-  <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>4 -</t>
-  </si>
-  <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>0,80 лв.</t>
-  </si>
-  <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>5 -</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>52 -</t>
-  </si>
-  <si>
-    <t>50,00 лв.</t>
-  </si>
-  <si>
-    <t>2 600,00 лв.</t>
-  </si>
-  <si>
-    <t>11 -</t>
-  </si>
-  <si>
-    <t>1 100,00 лв.</t>
-  </si>
-  <si>
-    <t>Тотал:</t>
-  </si>
-  <si>
-    <t>3 801,40 лв.</t>
-  </si>
-  <si>
-    <t>Преброена сума</t>
-  </si>
-  <si>
-    <t>Разлика</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Общо приходи от доставки: </t>
-  </si>
-  <si>
-    <t>28 920,81 лв.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Общо приходи от стари сметки: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Сума от неплатени сметки: </t>
   </si>
   <si>
-    <t>653,27 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>24 466,14 лв.</t>
+    <t>31 930,43 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -371,7 +254,7 @@
     <t>Приел отчета:</t>
   </si>
   <si>
-    <t>Александър Сергеевич Добров</t>
+    <t>Александр Добров</t>
   </si>
   <si>
     <t>(име, фамилия, подпис)</t>
@@ -870,12 +753,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -916,11 +799,26 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -943,23 +841,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -991,6 +883,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,24 +899,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1066,6 +949,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1385,9 +1272,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
@@ -1410,11 +1297,11 @@
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="70"/>
@@ -1423,13 +1310,13 @@
       <c r="D2" s="71"/>
       <c r="E2" s="71"/>
       <c r="F2" s="72">
-        <v>45554</v>
+        <v>45426</v>
       </c>
       <c r="G2" s="72"/>
       <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="75" t="s">
@@ -1461,854 +1348,663 @@
       <c r="H4" s="78"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="67"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="3">
-        <v>1001167596</v>
+        <v>1001138212</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
-        <v>2</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="5">
-        <v>1001167614</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="9"/>
+      <c r="A7" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="67"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="3">
+        <v>1001138003</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="5">
+        <v>1001138005</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="3">
-        <v>1001167680</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61"/>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="62"/>
+        <v>20</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="50"/>
       <c r="E10" s="3">
-        <v>1001167596</v>
+        <v>1001138006</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="5">
+        <v>1001138010</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="62"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="3">
-        <v>1001167541</v>
+        <v>1001138011</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="5">
-        <v>1001167542</v>
+        <v>1001138017</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="62"/>
+        <v>15</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="50"/>
       <c r="E14" s="3">
-        <v>1001167543</v>
+        <v>1001138098</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="63"/>
+        <v>31</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="49"/>
       <c r="E15" s="5">
-        <v>1001167544</v>
+        <v>1001138102</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="62"/>
+        <v>34</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="50"/>
       <c r="E16" s="3">
-        <v>1001167578</v>
+        <v>1001138103</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="63"/>
+        <v>31</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="E17" s="5">
-        <v>1001167580</v>
+        <v>1001138107</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="62"/>
+        <v>24</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="50"/>
       <c r="E18" s="3">
-        <v>1001167591</v>
+        <v>1001138110</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="63"/>
+        <v>20</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="49"/>
       <c r="E19" s="5">
-        <v>1001167609</v>
+        <v>1001138112</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="62"/>
+        <v>34</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="50"/>
       <c r="E20" s="3">
-        <v>1001167610</v>
+        <v>1001138113</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="63"/>
+        <v>27</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="49"/>
       <c r="E21" s="5">
-        <v>1001167615</v>
+        <v>1001138123</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="62"/>
+        <v>27</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="50"/>
       <c r="E22" s="3">
-        <v>1001167617</v>
+        <v>1001138127</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="63"/>
+        <v>24</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="49"/>
       <c r="E23" s="5">
-        <v>1001167630</v>
+        <v>1001138143</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="3">
+        <v>1001138175</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="10">
+        <v>18</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="51"/>
+      <c r="E25" s="12">
+        <v>1001138188</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C26" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="3">
-        <v>1001167632</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="C27" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="23"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="56"/>
+    </row>
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B30" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="8">
-        <v>14</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="63" t="s">
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61"/>
+    </row>
+    <row r="31" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="28"/>
+      <c r="C31" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="39"/>
+      <c r="H31" s="40"/>
+    </row>
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B32" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="5">
-        <v>1001167634</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
-        <v>15</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="62"/>
-      <c r="E26" s="3">
-        <v>1001167642</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
-        <v>16</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="C32" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40"/>
+    </row>
+    <row r="33" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="29"/>
+      <c r="C33" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="5">
-        <v>1001167660</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="G33" s="39"/>
+      <c r="H33" s="40"/>
+    </row>
+    <row r="34" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="62" t="s">
+      <c r="G34" s="39"/>
+      <c r="H34" s="40"/>
+    </row>
+    <row r="35" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B35" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="3">
-        <v>1001167672</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="59" t="s">
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="43"/>
+      <c r="H35" s="44"/>
+    </row>
+    <row r="36" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="61"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="62"/>
-      <c r="E30" s="3">
-        <v>1001166992</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="59" t="s">
+      <c r="F36" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="46"/>
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="61"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="62" t="s">
+      <c r="D37" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="36"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="34"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="3">
-        <v>1001167539</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="8">
-        <v>2</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="63" t="s">
+      <c r="C40" s="35"/>
+      <c r="E40" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="63"/>
-      <c r="E33" s="5">
-        <v>1001167592</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D41" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="E41" s="36"/>
+    </row>
+    <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B43" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="H33" s="9"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="10">
-        <v>3</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="12">
-        <v>1001167673</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="13"/>
-    </row>
-    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C52" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="51"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B53" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H53" s="21"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B54" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="H54" s="23"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B55" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F55" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="H55" s="21"/>
-    </row>
-    <row r="56" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C56" s="24"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G56" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="H56" s="53"/>
-    </row>
-    <row r="57" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B57" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C57" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="G57" s="57"/>
-      <c r="H57" s="58"/>
-    </row>
-    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="28"/>
-      <c r="C58" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="47"/>
-      <c r="H58" s="48"/>
-    </row>
-    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B59" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="G59" s="47"/>
-      <c r="H59" s="48"/>
-    </row>
-    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="29"/>
-      <c r="C60" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="G60" s="47"/>
-      <c r="H60" s="48"/>
-    </row>
-    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C61" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
-      <c r="F61" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="G61" s="47"/>
-      <c r="H61" s="48"/>
-    </row>
-    <row r="62" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C62" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="G62" s="38"/>
-      <c r="H62" s="39"/>
-    </row>
-    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="E63" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F63" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="G63" s="41"/>
-      <c r="H63" s="42"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B64" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="E64" s="34"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C65" s="43"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="43"/>
-      <c r="C66" s="43"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="35"/>
-      <c r="E67" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D68" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E68" s="34"/>
-    </row>
-    <row r="69" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B70" s="31" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="33">
-        <v>45555</v>
-      </c>
-      <c r="E71" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35"/>
-      <c r="H71" s="35"/>
+    </row>
+    <row r="44" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="33">
+        <v>45427</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="C10:D10"/>
+  <mergeCells count="51">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -2318,56 +2014,48 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:H4"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A7:H7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="F30:H30"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="E71:H71"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="E44:H44"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove company object reference to company after crud operation with invoice. This may possible initiate new search in company objects box on the whole company objects DB.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="581" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC3F299A-DC65-429B-A2F6-DAAEB84887C9}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26BA4BCF-95E2-4E0B-8DB3-F82267B82DE2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="110">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,172 +65,154 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>108,00 лв.</t>
-  </si>
-  <si>
-    <t>Ддах Кофи Шоп ЕООД</t>
-  </si>
-  <si>
-    <t>Магазин Кофи Шоп - Кюстендил</t>
-  </si>
-  <si>
-    <t>141,98 лв.</t>
-  </si>
-  <si>
-    <t>В И М Мюзик 1 ЕООД</t>
-  </si>
-  <si>
-    <t>Революшън</t>
-  </si>
-  <si>
-    <t>535,75 лв.</t>
-  </si>
-  <si>
-    <t>Черешката ЕООД</t>
-  </si>
-  <si>
-    <t>Белканто</t>
-  </si>
-  <si>
-    <t>461,84 лв.</t>
-  </si>
-  <si>
-    <t>Арт Ен Фън 003 ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Къщата</t>
-  </si>
-  <si>
-    <t>495,07 лв.</t>
-  </si>
-  <si>
-    <t>Стримон Спа АД</t>
-  </si>
-  <si>
-    <t>Парк Хотел - Кюстендил</t>
-  </si>
-  <si>
-    <t>88,19 лв.</t>
-  </si>
-  <si>
-    <t>Рамира Кюстендил ООД</t>
-  </si>
-  <si>
-    <t>Хотел Рамира</t>
-  </si>
-  <si>
-    <t>836,40 лв.</t>
-  </si>
-  <si>
-    <t>Флора Бургер ЕООД</t>
-  </si>
-  <si>
-    <t>Кафе Флора - Кюстендил</t>
-  </si>
-  <si>
-    <t>211,67 лв.</t>
-  </si>
-  <si>
-    <t>Планинец ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Рибарника</t>
-  </si>
-  <si>
-    <t>451,91 лв.</t>
-  </si>
-  <si>
-    <t>Каталина 2024 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Роял - Кюстендил</t>
-  </si>
-  <si>
-    <t>627,32 лв.</t>
-  </si>
-  <si>
-    <t>ТМА 2011 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Наполи</t>
-  </si>
-  <si>
-    <t>568,54 лв.</t>
-  </si>
-  <si>
-    <t>Радостин Тренев ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Уест</t>
-  </si>
-  <si>
-    <t>412,49 лв.</t>
-  </si>
-  <si>
-    <t>Рекпласт ЕООД</t>
-  </si>
-  <si>
-    <t>Кафе ABC</t>
-  </si>
-  <si>
-    <t>471,36 лв.</t>
-  </si>
-  <si>
-    <t>МСД 2016 ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Терасата</t>
-  </si>
-  <si>
-    <t>123,96 лв.</t>
-  </si>
-  <si>
-    <t>Емил Станоев - Еми ЕТ</t>
-  </si>
-  <si>
-    <t>Бързо Хранене</t>
-  </si>
-  <si>
-    <t>1 044,70 лв.</t>
-  </si>
-  <si>
-    <t>Хотел Стримон гардън</t>
+    <t>7 397,22 лв.</t>
+  </si>
+  <si>
+    <t>Тиенди ООД</t>
+  </si>
+  <si>
+    <t>Тиенди - Разлог</t>
+  </si>
+  <si>
+    <t>1 971,56 лв.</t>
+  </si>
+  <si>
+    <t>Ай Пи Фууд 2012 ООД</t>
+  </si>
+  <si>
+    <t>Ай Пи Фууд - Разлог</t>
+  </si>
+  <si>
+    <t>49,94 лв.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Търговец - Атанас Колев </t>
+  </si>
+  <si>
+    <t>Търговец - Атанас Колев</t>
+  </si>
+  <si>
+    <t>251,71 лв.</t>
+  </si>
+  <si>
+    <t>България Холидейз ЕООД</t>
+  </si>
+  <si>
+    <t>Пирин голф и спа - Разлог</t>
+  </si>
+  <si>
+    <t>1 469,66 лв.</t>
+  </si>
+  <si>
+    <t>269,40 лв.</t>
+  </si>
+  <si>
+    <t>700,22 лв.</t>
+  </si>
+  <si>
+    <t>299,70 лв.</t>
+  </si>
+  <si>
+    <t>799,94 лв.</t>
+  </si>
+  <si>
+    <t>Енте ООД</t>
+  </si>
+  <si>
+    <t>Ресторант 4 Посоки - Банско</t>
+  </si>
+  <si>
+    <t>150,66 лв.</t>
+  </si>
+  <si>
+    <t>284,53 лв.</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>1 657,69 лв.</t>
+    <t>970,26 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Станби ЕООД</t>
-  </si>
-  <si>
-    <t>Френдс бар и грил</t>
+    <t>Хотелс Енд Дриймс ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Леонардо Банско</t>
+  </si>
+  <si>
+    <t>748,10 лв.</t>
+  </si>
+  <si>
+    <t>Рентали ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Гарлик - Банско</t>
+  </si>
+  <si>
+    <t>129,46 лв.</t>
+  </si>
+  <si>
+    <t>Гехард ЕООД</t>
+  </si>
+  <si>
+    <t>Хотел Кенпински Банско</t>
+  </si>
+  <si>
+    <t>1 132,56 лв.</t>
+  </si>
+  <si>
+    <t>Приват Турс 2000 ЕООД</t>
+  </si>
+  <si>
+    <t>Фор Пойнтс - Банско</t>
+  </si>
+  <si>
+    <t>2 007,60 лв.</t>
+  </si>
+  <si>
+    <t>Майсторови 2016 ООД</t>
+  </si>
+  <si>
+    <t>Майсторови - Гоце Делчев</t>
+  </si>
+  <si>
+    <t>230,56 лв.</t>
+  </si>
+  <si>
+    <t>482,72 лв.</t>
+  </si>
+  <si>
+    <t>Фокача Експрес ЕООД</t>
+  </si>
+  <si>
+    <t>Фокача Джано - Банско</t>
+  </si>
+  <si>
+    <t>4 231,19 лв.</t>
+  </si>
+  <si>
+    <t>Буларм Груп ООД</t>
+  </si>
+  <si>
+    <t>Буларм - Банско</t>
+  </si>
+  <si>
+    <t>228,12 лв.</t>
+  </si>
+  <si>
+    <t>33,50 лв.</t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Дар Г.Н. ООД</t>
-  </si>
-  <si>
-    <t>F29</t>
-  </si>
-  <si>
-    <t>Неплатени</t>
-  </si>
-  <si>
-    <t>Хилс 1940 ЕООД</t>
-  </si>
-  <si>
-    <t>364,03 лв.</t>
-  </si>
-  <si>
-    <t>Cash</t>
+    <t>Юлен АД</t>
+  </si>
+  <si>
+    <t>Юлен - Бъндеришка Вип</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -242,91 +224,85 @@
     <t>0,02 лв.</t>
   </si>
   <si>
+    <t>4 -</t>
+  </si>
+  <si>
     <t>0,05 лв.</t>
   </si>
   <si>
-    <t>4 -</t>
+    <t>0,20 лв.</t>
+  </si>
+  <si>
+    <t>9 -</t>
   </si>
   <si>
     <t>0,10 лв.</t>
   </si>
   <si>
-    <t>0,40 лв.</t>
-  </si>
-  <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>0,80 лв.</t>
+    <t>0,90 лв.</t>
+  </si>
+  <si>
+    <t>3 -</t>
   </si>
   <si>
     <t>0,50 лв.</t>
   </si>
   <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>7 -</t>
+    <t>1,50 лв.</t>
+  </si>
+  <si>
+    <t>17 -</t>
   </si>
   <si>
     <t>1,00 лв.</t>
   </si>
   <si>
-    <t>7,00 лв.</t>
-  </si>
-  <si>
-    <t>14,00 лв.</t>
-  </si>
-  <si>
-    <t>17 -</t>
+    <t>17,00 лв.</t>
   </si>
   <si>
     <t>5,00 лв.</t>
   </si>
   <si>
-    <t>85,00 лв.</t>
-  </si>
-  <si>
-    <t>81 -</t>
+    <t>69 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>810,00 лв.</t>
-  </si>
-  <si>
-    <t>48 -</t>
+    <t>690,00 лв.</t>
+  </si>
+  <si>
+    <t>104 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>960,00 лв.</t>
-  </si>
-  <si>
-    <t>44 -</t>
+    <t>2 080,00 лв.</t>
+  </si>
+  <si>
+    <t>205 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>2 200,00 лв.</t>
-  </si>
-  <si>
-    <t>25 -</t>
+    <t>10 250,00 лв.</t>
+  </si>
+  <si>
+    <t>6 -</t>
   </si>
   <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>2 500,00 лв.</t>
+    <t>600,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>6 579,27 лв.</t>
+    <t>13 644,62 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -338,7 +314,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>8 600,90 лв.</t>
+    <t>23 838,61 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -350,25 +326,28 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
+    <t>10 194,07 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>6 579,18 лв.</t>
+    <t>13 644,54 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,09 лв.</t>
+    <t>0,08 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
   </si>
   <si>
-    <t>СВ 2241 КК</t>
+    <t>СВ 2611 НТ</t>
   </si>
   <si>
     <t>Съставил отчета / Предал:</t>
@@ -951,15 +930,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1394,7 +1373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1430,7 +1409,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45702</v>
+        <v>45692</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1491,7 +1470,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001203059</v>
+        <v>1001200506</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1513,7 +1492,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001203062</v>
+        <v>1001200510</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1535,7 +1514,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001203066</v>
+        <v>1001200511</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1557,7 +1536,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001203067</v>
+        <v>1001200515</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
@@ -1572,14 +1551,14 @@
         <v>5</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001203073</v>
+        <v>1001200516</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>21</v>
@@ -1594,20 +1573,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001203074</v>
+        <v>1001200518</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11" s="32"/>
     </row>
@@ -1616,20 +1595,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001203076</v>
+        <v>1001200533</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H12" s="30"/>
     </row>
@@ -1638,20 +1617,20 @@
         <v>8</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001203077</v>
+        <v>1001200540</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H13" s="32"/>
     </row>
@@ -1660,20 +1639,20 @@
         <v>9</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001203082</v>
+        <v>1001200542</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H14" s="30"/>
     </row>
@@ -1682,20 +1661,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001203084</v>
+        <v>1001200544</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H15" s="32"/>
     </row>
@@ -1704,530 +1683,658 @@
         <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001203099</v>
+        <v>1001200557</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="31">
-        <v>12</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25">
-        <v>1001203102</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="32"/>
+      <c r="A17" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
-        <v>1001203103</v>
+        <v>1001200501</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="25">
-        <v>1001203134</v>
+        <v>1001200509</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
-        <v>1001203136</v>
+        <v>1001200512</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="34"/>
+      <c r="A21" s="31">
+        <v>4</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25">
+        <v>1001200514</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="32"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
-        <v>1001203078</v>
+        <v>1001200517</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="H22" s="30"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="25">
-        <v>949927</v>
+        <v>1001200529</v>
       </c>
       <c r="F23" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="29">
+        <v>7</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22">
+        <v>1001200536</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="30"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="31">
+        <v>8</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25">
+        <v>1001200539</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="29">
+        <v>9</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22">
+        <v>1001200545</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="31">
+        <v>10</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25">
+        <v>1001200554</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="32"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="29">
+        <v>11</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="32"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
+      <c r="D28" s="21"/>
+      <c r="E28" s="22">
+        <v>947373</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="30"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="31">
+        <v>12</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25">
+        <v>947374</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="32"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="29">
+        <v>13</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22">
+        <v>947412</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="30"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="35">
+        <v>14</v>
+      </c>
+      <c r="B31" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38">
+        <v>947500</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="39"/>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="34"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="35">
-        <v>1</v>
-      </c>
-      <c r="B25" s="36" t="s">
+      <c r="D53" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C54" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38">
-        <v>1001203075</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C26" s="46" t="s">
+      <c r="E54" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
+      <c r="C55" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="D55" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="42" t="s">
+      <c r="E55" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="51" t="s">
+      <c r="G55" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="44" t="s">
+      <c r="C56" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="F56" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="42" t="s">
+      <c r="G56" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="H56" s="52"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="42" t="s">
+      <c r="C57" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="42" t="s">
+      <c r="F57" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="45" t="s">
+      <c r="G57" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="H57" s="50"/>
+    </row>
+    <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C58" s="53"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="44" t="s">
+      <c r="G58" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="43" t="s">
+      <c r="H58" s="57"/>
+    </row>
+    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B59" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="C59" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="59"/>
+      <c r="C60" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B61" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="G32" s="44" t="s">
+      <c r="C61" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="H32" s="52"/>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="55" t="s">
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="60"/>
+      <c r="C62" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="56" t="s">
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="57"/>
-    </row>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B34" s="58" t="s">
+      <c r="G62" s="1"/>
+      <c r="H62" s="69"/>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C63" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="61" t="s">
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="69"/>
+    </row>
+    <row r="64" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="65"/>
+      <c r="E64" s="65"/>
+      <c r="F64" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="67" t="s">
+      <c r="G64" s="10"/>
+      <c r="H64" s="71"/>
+    </row>
+    <row r="65" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="E65" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="59"/>
-      <c r="C35" s="63" t="s">
+      <c r="F65" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="69"/>
-    </row>
-    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B36" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="69"/>
-    </row>
-    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="60"/>
-      <c r="C37" s="63" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="69"/>
-    </row>
-    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C38" s="64" t="s">
+      <c r="G65" s="73"/>
+      <c r="H65" s="74"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="69"/>
-    </row>
-    <row r="39" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="75" t="s">
+      <c r="D66" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="17"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="77" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="77"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" s="77"/>
+      <c r="C68" s="77"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="78"/>
+      <c r="E69" s="78" t="s">
+        <v>107</v>
+      </c>
+      <c r="F69" s="78"/>
+      <c r="G69" s="78"/>
+      <c r="H69" s="78"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D70" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="72" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B72" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="71"/>
-    </row>
-    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="66" t="s">
+    </row>
+    <row r="73" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B73" s="79">
+        <v>45693</v>
+      </c>
+      <c r="E73" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="72" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="77"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="78"/>
-      <c r="E44" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D45" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B47" s="75" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="79">
-        <v>45705</v>
-      </c>
-      <c r="E48" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="78"/>
+      <c r="H73" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:H37"/>
+  <mergeCells count="57">
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A17:H17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>

</xml_diff>

<commit_message>
Fix bug with pay method in export file. Change order in list invoce. Replace day report id from day report load box and put it on the background.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="655" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26BA4BCF-95E2-4E0B-8DB3-F82267B82DE2}"/>
+  <xr:revisionPtr revIDLastSave="581" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11C91595-5CA9-4C0E-879A-8E065E405DAB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,154 +65,172 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>7 397,22 лв.</t>
-  </si>
-  <si>
-    <t>Тиенди ООД</t>
-  </si>
-  <si>
-    <t>Тиенди - Разлог</t>
-  </si>
-  <si>
-    <t>1 971,56 лв.</t>
-  </si>
-  <si>
-    <t>Ай Пи Фууд 2012 ООД</t>
-  </si>
-  <si>
-    <t>Ай Пи Фууд - Разлог</t>
-  </si>
-  <si>
-    <t>49,94 лв.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Търговец - Атанас Колев </t>
-  </si>
-  <si>
-    <t>Търговец - Атанас Колев</t>
-  </si>
-  <si>
-    <t>251,71 лв.</t>
-  </si>
-  <si>
-    <t>България Холидейз ЕООД</t>
-  </si>
-  <si>
-    <t>Пирин голф и спа - Разлог</t>
-  </si>
-  <si>
-    <t>1 469,66 лв.</t>
-  </si>
-  <si>
-    <t>269,40 лв.</t>
-  </si>
-  <si>
-    <t>700,22 лв.</t>
-  </si>
-  <si>
-    <t>299,70 лв.</t>
-  </si>
-  <si>
-    <t>799,94 лв.</t>
-  </si>
-  <si>
-    <t>Енте ООД</t>
-  </si>
-  <si>
-    <t>Ресторант 4 Посоки - Банско</t>
-  </si>
-  <si>
-    <t>150,66 лв.</t>
-  </si>
-  <si>
-    <t>284,53 лв.</t>
+    <t>108,00 лв.</t>
+  </si>
+  <si>
+    <t>Ддах Кофи Шоп ЕООД</t>
+  </si>
+  <si>
+    <t>Магазин Кофи Шоп - Кюстендил</t>
+  </si>
+  <si>
+    <t>141,98 лв.</t>
+  </si>
+  <si>
+    <t>В И М Мюзик 1 ЕООД</t>
+  </si>
+  <si>
+    <t>Революшън</t>
+  </si>
+  <si>
+    <t>535,75 лв.</t>
+  </si>
+  <si>
+    <t>Черешката ЕООД</t>
+  </si>
+  <si>
+    <t>Белканто</t>
+  </si>
+  <si>
+    <t>461,84 лв.</t>
+  </si>
+  <si>
+    <t>Арт Ен Фън 003 ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Къщата</t>
+  </si>
+  <si>
+    <t>495,07 лв.</t>
+  </si>
+  <si>
+    <t>Стримон Спа АД</t>
+  </si>
+  <si>
+    <t>Парк Хотел - Кюстендил</t>
+  </si>
+  <si>
+    <t>88,19 лв.</t>
+  </si>
+  <si>
+    <t>Рамира Кюстендил ООД</t>
+  </si>
+  <si>
+    <t>Хотел Рамира</t>
+  </si>
+  <si>
+    <t>836,40 лв.</t>
+  </si>
+  <si>
+    <t>Флора Бургер ЕООД</t>
+  </si>
+  <si>
+    <t>Кафе Флора - Кюстендил</t>
+  </si>
+  <si>
+    <t>211,67 лв.</t>
+  </si>
+  <si>
+    <t>Планинец ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Рибарника</t>
+  </si>
+  <si>
+    <t>451,91 лв.</t>
+  </si>
+  <si>
+    <t>Каталина 2024 ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Роял - Кюстендил</t>
+  </si>
+  <si>
+    <t>627,32 лв.</t>
+  </si>
+  <si>
+    <t>ТМА 2011 ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Наполи</t>
+  </si>
+  <si>
+    <t>568,54 лв.</t>
+  </si>
+  <si>
+    <t>Радостин Тренев ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Уест</t>
+  </si>
+  <si>
+    <t>412,49 лв.</t>
+  </si>
+  <si>
+    <t>Рекпласт ЕООД</t>
+  </si>
+  <si>
+    <t>Кафе ABC</t>
+  </si>
+  <si>
+    <t>471,36 лв.</t>
+  </si>
+  <si>
+    <t>МСД 2016 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Терасата</t>
+  </si>
+  <si>
+    <t>123,96 лв.</t>
+  </si>
+  <si>
+    <t>Емил Станоев - Еми ЕТ</t>
+  </si>
+  <si>
+    <t>Бързо Хранене</t>
+  </si>
+  <si>
+    <t>1 044,70 лв.</t>
+  </si>
+  <si>
+    <t>Хотел Стримон гардън</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>970,26 лв.</t>
+    <t>1 657,69 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Хотелс Енд Дриймс ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Леонардо Банско</t>
-  </si>
-  <si>
-    <t>748,10 лв.</t>
-  </si>
-  <si>
-    <t>Рентали ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Гарлик - Банско</t>
-  </si>
-  <si>
-    <t>129,46 лв.</t>
-  </si>
-  <si>
-    <t>Гехард ЕООД</t>
-  </si>
-  <si>
-    <t>Хотел Кенпински Банско</t>
-  </si>
-  <si>
-    <t>1 132,56 лв.</t>
-  </si>
-  <si>
-    <t>Приват Турс 2000 ЕООД</t>
-  </si>
-  <si>
-    <t>Фор Пойнтс - Банско</t>
-  </si>
-  <si>
-    <t>2 007,60 лв.</t>
-  </si>
-  <si>
-    <t>Майсторови 2016 ООД</t>
-  </si>
-  <si>
-    <t>Майсторови - Гоце Делчев</t>
-  </si>
-  <si>
-    <t>230,56 лв.</t>
-  </si>
-  <si>
-    <t>482,72 лв.</t>
-  </si>
-  <si>
-    <t>Фокача Експрес ЕООД</t>
-  </si>
-  <si>
-    <t>Фокача Джано - Банско</t>
-  </si>
-  <si>
-    <t>4 231,19 лв.</t>
-  </si>
-  <si>
-    <t>Буларм Груп ООД</t>
-  </si>
-  <si>
-    <t>Буларм - Банско</t>
-  </si>
-  <si>
-    <t>228,12 лв.</t>
-  </si>
-  <si>
-    <t>33,50 лв.</t>
+    <t>Станби ЕООД</t>
+  </si>
+  <si>
+    <t>Френдс бар и грил</t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Юлен АД</t>
-  </si>
-  <si>
-    <t>Юлен - Бъндеришка Вип</t>
+    <t>Дар Г.Н. ООД</t>
+  </si>
+  <si>
+    <t>F29</t>
+  </si>
+  <si>
+    <t>Неплатени</t>
+  </si>
+  <si>
+    <t>Хилс 1940 ЕООД</t>
+  </si>
+  <si>
+    <t>364,03 лв.</t>
+  </si>
+  <si>
+    <t>В брой</t>
   </si>
   <si>
     <t>Отчет на парите</t>
@@ -224,85 +242,91 @@
     <t>0,02 лв.</t>
   </si>
   <si>
+    <t>0,05 лв.</t>
+  </si>
+  <si>
     <t>4 -</t>
   </si>
   <si>
-    <t>0,05 лв.</t>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>0,40 лв.</t>
   </si>
   <si>
     <t>0,20 лв.</t>
   </si>
   <si>
-    <t>9 -</t>
-  </si>
-  <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>0,90 лв.</t>
-  </si>
-  <si>
-    <t>3 -</t>
+    <t>0,80 лв.</t>
   </si>
   <si>
     <t>0,50 лв.</t>
   </si>
   <si>
-    <t>1,50 лв.</t>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
+    <t>7 -</t>
+  </si>
+  <si>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>7,00 лв.</t>
+  </si>
+  <si>
+    <t>14,00 лв.</t>
   </si>
   <si>
     <t>17 -</t>
   </si>
   <si>
-    <t>1,00 лв.</t>
-  </si>
-  <si>
-    <t>17,00 лв.</t>
-  </si>
-  <si>
     <t>5,00 лв.</t>
   </si>
   <si>
-    <t>69 -</t>
+    <t>85,00 лв.</t>
+  </si>
+  <si>
+    <t>81 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>690,00 лв.</t>
-  </si>
-  <si>
-    <t>104 -</t>
+    <t>810,00 лв.</t>
+  </si>
+  <si>
+    <t>48 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>2 080,00 лв.</t>
-  </si>
-  <si>
-    <t>205 -</t>
+    <t>960,00 лв.</t>
+  </si>
+  <si>
+    <t>44 -</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>10 250,00 лв.</t>
-  </si>
-  <si>
-    <t>6 -</t>
+    <t>2 200,00 лв.</t>
+  </si>
+  <si>
+    <t>25 -</t>
   </si>
   <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>600,00 лв.</t>
+    <t>2 500,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>13 644,62 лв.</t>
+    <t>6 579,27 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -314,7 +338,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>23 838,61 лв.</t>
+    <t>8 600,90 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -326,28 +350,25 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>10 194,07 лв.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>13 644,54 лв.</t>
+    <t>6 579,18 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,08 лв.</t>
+    <t>0,09 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
   </si>
   <si>
-    <t>СВ 2611 НТ</t>
+    <t>СВ 2241 КК</t>
   </si>
   <si>
     <t>Съставил отчета / Предал:</t>
@@ -930,15 +951,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1373,7 +1394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1409,7 +1430,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45692</v>
+        <v>45702</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1470,7 +1491,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001200506</v>
+        <v>1001203059</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1492,7 +1513,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001200510</v>
+        <v>1001203062</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1514,7 +1535,7 @@
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001200511</v>
+        <v>1001203066</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1536,7 +1557,7 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001200515</v>
+        <v>1001203067</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>18</v>
@@ -1551,14 +1572,14 @@
         <v>5</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="22">
-        <v>1001200516</v>
+        <v>1001203073</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>21</v>
@@ -1573,20 +1594,20 @@
         <v>6</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="25">
-        <v>1001200518</v>
+        <v>1001203074</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H11" s="32"/>
     </row>
@@ -1595,20 +1616,20 @@
         <v>7</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="22">
-        <v>1001200533</v>
+        <v>1001203076</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H12" s="30"/>
     </row>
@@ -1617,20 +1638,20 @@
         <v>8</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="25">
-        <v>1001200540</v>
+        <v>1001203077</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H13" s="32"/>
     </row>
@@ -1639,20 +1660,20 @@
         <v>9</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="22">
-        <v>1001200542</v>
+        <v>1001203082</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H14" s="30"/>
     </row>
@@ -1661,20 +1682,20 @@
         <v>10</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="25">
-        <v>1001200544</v>
+        <v>1001203084</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H15" s="32"/>
     </row>
@@ -1683,658 +1704,530 @@
         <v>11</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="22">
-        <v>1001200557</v>
+        <v>1001203099</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="34"/>
+      <c r="A17" s="31">
+        <v>12</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25">
+        <v>1001203102</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="22">
-        <v>1001200501</v>
+        <v>1001203103</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="31">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="25">
-        <v>1001200509</v>
+        <v>1001203134</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="H19" s="32"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="29">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="22">
-        <v>1001200512</v>
+        <v>1001203136</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="31">
-        <v>4</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25">
-        <v>1001200514</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="32"/>
+      <c r="A21" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="22">
-        <v>1001200517</v>
+        <v>1001203078</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H22" s="30"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="25">
-        <v>1001200529</v>
+        <v>949927</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="H23" s="32"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="29">
-        <v>7</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22">
-        <v>1001200536</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="30"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="31">
-        <v>8</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25">
-        <v>1001200539</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="32"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="29">
-        <v>9</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="22">
-        <v>1001200545</v>
-      </c>
-      <c r="F26" s="20" t="s">
+      <c r="A24" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="35">
+        <v>1</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38">
+        <v>1001203075</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C26" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="48"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="50"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="52"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="50"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="52"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="50"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="52"/>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" s="53"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="57"/>
+    </row>
+    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B34" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="59"/>
+      <c r="C35" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="69"/>
+    </row>
+    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B36" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="69"/>
+    </row>
+    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="60"/>
+      <c r="C37" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="30"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="31">
-        <v>10</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25">
-        <v>1001200554</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="32"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="29">
-        <v>11</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="21" t="s">
+      <c r="G37" s="1"/>
+      <c r="H37" s="69"/>
+    </row>
+    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22">
-        <v>947373</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="31">
-        <v>12</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25">
-        <v>947374</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G29" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H29" s="32"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="29">
-        <v>13</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22">
-        <v>947412</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="30"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="35">
-        <v>14</v>
-      </c>
-      <c r="B31" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="37"/>
-      <c r="E31" s="38">
-        <v>947500</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="39"/>
-    </row>
-    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C52" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="48"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B53" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="E53" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="G53" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="H53" s="50"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B54" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="F54" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="G54" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="H54" s="52"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B55" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="F55" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="G55" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" s="50"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B56" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="E56" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="F56" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="G56" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="H56" s="52"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B57" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F57" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="G57" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="H57" s="50"/>
-    </row>
-    <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C58" s="53"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="55" t="s">
-        <v>87</v>
-      </c>
-      <c r="G58" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="H58" s="57"/>
-    </row>
-    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B59" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="62"/>
-      <c r="E59" s="62"/>
-      <c r="F59" s="67" t="s">
-        <v>92</v>
-      </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="59"/>
-      <c r="C60" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="69"/>
-    </row>
-    <row r="61" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B61" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="C61" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="D61" s="64"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="G61" s="1"/>
-      <c r="H61" s="69"/>
-    </row>
-    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="60"/>
-      <c r="C62" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="64"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="G62" s="1"/>
-      <c r="H62" s="69"/>
-    </row>
-    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C63" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="69"/>
-    </row>
-    <row r="64" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B64" s="75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C64" s="65" t="s">
-        <v>98</v>
-      </c>
-      <c r="D64" s="65"/>
-      <c r="E64" s="65"/>
-      <c r="F64" s="70" t="s">
-        <v>99</v>
-      </c>
-      <c r="G64" s="10"/>
-      <c r="H64" s="71"/>
-    </row>
-    <row r="65" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="F65" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="G65" s="73"/>
-      <c r="H65" s="74"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D66" s="17" t="s">
+      <c r="G38" s="1"/>
+      <c r="H38" s="69"/>
+    </row>
+    <row r="39" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="77" t="s">
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="77"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B68" s="77"/>
-      <c r="C68" s="77"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B69" s="78" t="s">
+      <c r="G39" s="10"/>
+      <c r="H39" s="71"/>
+    </row>
+    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="66" t="s">
         <v>107</v>
       </c>
-      <c r="C69" s="78"/>
-      <c r="E69" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="F69" s="78"/>
-      <c r="G69" s="78"/>
-      <c r="H69" s="78"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D70" s="17" t="s">
+      <c r="F40" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B72" s="75" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B73" s="79">
-        <v>45693</v>
-      </c>
-      <c r="E73" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="F73" s="78"/>
-      <c r="G73" s="78"/>
-      <c r="H73" s="78"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="74"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="17"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="77"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="77"/>
+      <c r="C43" s="77"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="78"/>
+      <c r="E44" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="78"/>
+      <c r="G44" s="78"/>
+      <c r="H44" s="78"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D45" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B47" s="75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="79">
+        <v>45705</v>
+      </c>
+      <c r="E48" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="F48" s="78"/>
+      <c r="G48" s="78"/>
+      <c r="H48" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="E69:H69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:H59"/>
+  <mergeCells count="51">
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:H37"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>

</xml_diff>

<commit_message>
Fix bug in add return product with new product and description.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="581" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11C91595-5CA9-4C0E-879A-8E065E405DAB}"/>
+  <xr:revisionPtr revIDLastSave="677" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E8486D-5FA8-4611-8DBF-11859F01811F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="102">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,268 +65,220 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>108,00 лв.</t>
-  </si>
-  <si>
-    <t>Ддах Кофи Шоп ЕООД</t>
-  </si>
-  <si>
-    <t>Магазин Кофи Шоп - Кюстендил</t>
-  </si>
-  <si>
-    <t>141,98 лв.</t>
-  </si>
-  <si>
-    <t>В И М Мюзик 1 ЕООД</t>
-  </si>
-  <si>
-    <t>Революшън</t>
-  </si>
-  <si>
-    <t>535,75 лв.</t>
-  </si>
-  <si>
-    <t>Черешката ЕООД</t>
-  </si>
-  <si>
-    <t>Белканто</t>
-  </si>
-  <si>
-    <t>461,84 лв.</t>
-  </si>
-  <si>
-    <t>Арт Ен Фън 003 ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Къщата</t>
-  </si>
-  <si>
-    <t>495,07 лв.</t>
-  </si>
-  <si>
-    <t>Стримон Спа АД</t>
-  </si>
-  <si>
-    <t>Парк Хотел - Кюстендил</t>
-  </si>
-  <si>
-    <t>88,19 лв.</t>
-  </si>
-  <si>
-    <t>Рамира Кюстендил ООД</t>
-  </si>
-  <si>
-    <t>Хотел Рамира</t>
-  </si>
-  <si>
-    <t>836,40 лв.</t>
-  </si>
-  <si>
-    <t>Флора Бургер ЕООД</t>
-  </si>
-  <si>
-    <t>Кафе Флора - Кюстендил</t>
-  </si>
-  <si>
-    <t>211,67 лв.</t>
-  </si>
-  <si>
-    <t>Планинец ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Рибарника</t>
-  </si>
-  <si>
-    <t>451,91 лв.</t>
-  </si>
-  <si>
-    <t>Каталина 2024 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Роял - Кюстендил</t>
-  </si>
-  <si>
-    <t>627,32 лв.</t>
-  </si>
-  <si>
-    <t>ТМА 2011 ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Наполи</t>
-  </si>
-  <si>
-    <t>568,54 лв.</t>
-  </si>
-  <si>
-    <t>Радостин Тренев ЕООД</t>
-  </si>
-  <si>
-    <t>Пица Уест</t>
-  </si>
-  <si>
-    <t>412,49 лв.</t>
-  </si>
-  <si>
-    <t>Рекпласт ЕООД</t>
-  </si>
-  <si>
-    <t>Кафе ABC</t>
-  </si>
-  <si>
-    <t>471,36 лв.</t>
-  </si>
-  <si>
-    <t>МСД 2016 ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Терасата</t>
-  </si>
-  <si>
-    <t>123,96 лв.</t>
-  </si>
-  <si>
-    <t>Емил Станоев - Еми ЕТ</t>
-  </si>
-  <si>
-    <t>Бързо Хранене</t>
-  </si>
-  <si>
-    <t>1 044,70 лв.</t>
-  </si>
-  <si>
-    <t>Хотел Стримон гардън</t>
+    <t>1 289,63 лв.</t>
+  </si>
+  <si>
+    <t>Енте ООД</t>
+  </si>
+  <si>
+    <t>Ресторант 4 Посоки - Банско</t>
+  </si>
+  <si>
+    <t>199,20 лв.</t>
+  </si>
+  <si>
+    <t>Мир-2006 ООД</t>
+  </si>
+  <si>
+    <t>Ла Пиер - Банско</t>
+  </si>
+  <si>
+    <t>144,47 лв.</t>
+  </si>
+  <si>
+    <t>207,72 лв.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Търговец - Атанас Колев </t>
+  </si>
+  <si>
+    <t>Търговец - Атанас Колев</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>1 657,69 лв.</t>
+    <t>107,88 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Станби ЕООД</t>
-  </si>
-  <si>
-    <t>Френдс бар и грил</t>
+    <t>Гехард ЕООД</t>
+  </si>
+  <si>
+    <t>Хотел Кенпински Банско</t>
+  </si>
+  <si>
+    <t>138,60 лв.</t>
+  </si>
+  <si>
+    <t>Хотел Перун - Банско ЕООД</t>
+  </si>
+  <si>
+    <t>Хотел Перун - Банско</t>
+  </si>
+  <si>
+    <t>173,59 лв.</t>
+  </si>
+  <si>
+    <t>532,19 лв.</t>
+  </si>
+  <si>
+    <t>Рентали ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Гарлик - Банско</t>
+  </si>
+  <si>
+    <t>3 159,43 лв.</t>
+  </si>
+  <si>
+    <t>Буларм Груп ООД</t>
+  </si>
+  <si>
+    <t>Буларм - Банско</t>
+  </si>
+  <si>
+    <t>685,40 лв.</t>
+  </si>
+  <si>
+    <t>Фокача Експрес ЕООД</t>
+  </si>
+  <si>
+    <t>Фокача Джано - Банско</t>
+  </si>
+  <si>
+    <t>675,90 лв.</t>
+  </si>
+  <si>
+    <t>Хотелс Енд Дриймс ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Леонардо Банско</t>
+  </si>
+  <si>
+    <t>333,71 лв.</t>
+  </si>
+  <si>
+    <t>Майсторови 2016 ООД</t>
+  </si>
+  <si>
+    <t>Майсторови - Гоце Делчев</t>
+  </si>
+  <si>
+    <t>158,29 лв.</t>
+  </si>
+  <si>
+    <t>Емарди ООД</t>
+  </si>
+  <si>
+    <t>Кафе Емар - Банско</t>
+  </si>
+  <si>
+    <t>763,19 лв.</t>
+  </si>
+  <si>
+    <t>344,74 лв.</t>
+  </si>
+  <si>
+    <t>1 571,54 лв.</t>
+  </si>
+  <si>
+    <t>1 446,47 лв.</t>
+  </si>
+  <si>
+    <t>Приват Турс 2000 ЕООД</t>
+  </si>
+  <si>
+    <t>Фор Пойнтс - Банско</t>
+  </si>
+  <si>
+    <t>84,12 лв.</t>
+  </si>
+  <si>
+    <t>395,83 лв.</t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Дар Г.Н. ООД</t>
-  </si>
-  <si>
-    <t>F29</t>
-  </si>
-  <si>
-    <t>Неплатени</t>
-  </si>
-  <si>
-    <t>Хилс 1940 ЕООД</t>
-  </si>
-  <si>
-    <t>364,03 лв.</t>
-  </si>
-  <si>
-    <t>В брой</t>
+    <t>Юлен АД</t>
+  </si>
+  <si>
+    <t>Юлен - Бъндеришка Вип</t>
+  </si>
+  <si>
+    <t>Юлен - Шилигарника Бла Бла</t>
+  </si>
+  <si>
+    <t>Юлен - Начална Хепи Енд</t>
+  </si>
+  <si>
+    <t>Юлен - Бъндеришки Щеки</t>
+  </si>
+  <si>
+    <t>Юлен Бъчвите - Бъндеришка Поляна</t>
+  </si>
+  <si>
+    <t>Юлен - Начална Етно</t>
   </si>
   <si>
     <t>Отчет на парите</t>
   </si>
   <si>
+    <t>4 -</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>0,40 лв.</t>
+  </si>
+  <si>
     <t>1 -</t>
   </si>
   <si>
-    <t>0,02 лв.</t>
-  </si>
-  <si>
-    <t>0,05 лв.</t>
-  </si>
-  <si>
-    <t>4 -</t>
-  </si>
-  <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>0,40 лв.</t>
-  </si>
-  <si>
     <t>0,20 лв.</t>
   </si>
   <si>
-    <t>0,80 лв.</t>
-  </si>
-  <si>
     <t>0,50 лв.</t>
   </si>
   <si>
-    <t>2,00 лв.</t>
-  </si>
-  <si>
-    <t>7 -</t>
-  </si>
-  <si>
-    <t>1,00 лв.</t>
-  </si>
-  <si>
-    <t>7,00 лв.</t>
-  </si>
-  <si>
-    <t>14,00 лв.</t>
-  </si>
-  <si>
-    <t>17 -</t>
-  </si>
-  <si>
-    <t>5,00 лв.</t>
-  </si>
-  <si>
-    <t>85,00 лв.</t>
-  </si>
-  <si>
-    <t>81 -</t>
+    <t>10 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
-    <t>810,00 лв.</t>
-  </si>
-  <si>
-    <t>48 -</t>
+    <t>100,00 лв.</t>
+  </si>
+  <si>
+    <t>22 -</t>
   </si>
   <si>
     <t>20,00 лв.</t>
   </si>
   <si>
-    <t>960,00 лв.</t>
-  </si>
-  <si>
-    <t>44 -</t>
+    <t>440,00 лв.</t>
   </si>
   <si>
     <t>50,00 лв.</t>
   </si>
   <si>
-    <t>2 200,00 лв.</t>
-  </si>
-  <si>
-    <t>25 -</t>
-  </si>
-  <si>
-    <t>100,00 лв.</t>
-  </si>
-  <si>
-    <t>2 500,00 лв.</t>
+    <t>1 100,00 лв.</t>
+  </si>
+  <si>
+    <t>2 -</t>
+  </si>
+  <si>
+    <t>200,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>6 579,27 лв.</t>
+    <t>1 841,10 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -338,7 +290,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>8 600,90 лв.</t>
+    <t>12 411,90 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -350,19 +302,22 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
+    <t>10 570,88 лв.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Разходи + КИ: </t>
   </si>
   <si>
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>6 579,18 лв.</t>
+    <t>1 841,02 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,09 лв.</t>
+    <t>0,08 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -951,15 +906,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -987,8 +942,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1394,7 +1349,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1430,7 +1385,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45702</v>
+        <v>45706</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1491,7 +1446,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001203059</v>
+        <v>1001203860</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1513,7 +1468,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001203062</v>
+        <v>1001203875</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1528,14 +1483,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001203066</v>
+        <v>1001203879</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1550,684 +1505,846 @@
         <v>4</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001203067</v>
+        <v>1001203916</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>1</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22">
+        <v>1001203845</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="30"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="31">
+        <v>2</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25">
+        <v>1001203851</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="29">
+        <v>3</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22">
+        <v>1001203852</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="30"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="31">
+        <v>4</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25">
+        <v>1001203853</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="29">
+        <v>5</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22">
+        <v>1001203856</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="31">
+        <v>6</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25">
+        <v>1001203857</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="29">
+        <v>7</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22">
+        <v>1001203867</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="31">
+        <v>8</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25">
+        <v>1001203868</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="29">
+        <v>9</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22">
+        <v>1001203870</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="31">
+        <v>10</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25">
+        <v>1001203873</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="32"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="29">
+        <v>11</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22">
+        <v>1001203874</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="31">
+        <v>12</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25">
+        <v>1001203877</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="29">
+        <v>13</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22">
+        <v>1001203895</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="31">
+        <v>14</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25">
+        <v>1001203902</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="32"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="29">
+        <v>15</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="22">
+        <v>1001203904</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="31">
+        <v>16</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="25">
+        <v>950705</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="29">
+        <v>17</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22">
+        <v>950726</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="31">
         <v>18</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
-        <v>5</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="B28" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25">
+        <v>950733</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="29">
+        <v>19</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22">
+        <v>950737</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="30"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="31">
+        <v>20</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="25">
+        <v>950738</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="32"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="29">
+        <v>21</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22">
+        <v>950739</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="30"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="31">
         <v>22</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="B32" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="25">
+        <v>950789</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="29">
         <v>23</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22">
-        <v>1001203073</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="31">
-        <v>6</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25">
-        <v>1001203074</v>
-      </c>
-      <c r="F11" s="23" t="s">
+      <c r="B33" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22">
+        <v>1001203859</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="35">
         <v>24</v>
       </c>
-      <c r="G11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="32"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
-        <v>7</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22">
-        <v>1001203076</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="31">
-        <v>8</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25">
-        <v>1001203077</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="32"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="29">
-        <v>9</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22">
-        <v>1001203082</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="31">
-        <v>10</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25">
-        <v>1001203084</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
-        <v>11</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="B34" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22">
-        <v>1001203099</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="30"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="31">
-        <v>12</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25">
-        <v>1001203102</v>
-      </c>
-      <c r="F17" s="23" t="s">
+      <c r="C34" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="29">
-        <v>13</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22">
-        <v>1001203103</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="30"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="31">
-        <v>14</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25">
-        <v>1001203134</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="29">
-        <v>15</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22">
-        <v>1001203136</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="30"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="34"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="29">
-        <v>1</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22">
-        <v>1001203078</v>
-      </c>
-      <c r="F22" s="20" t="s">
+      <c r="D34" s="37"/>
+      <c r="E34" s="38">
+        <v>1001203869</v>
+      </c>
+      <c r="F34" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="30"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="31">
-        <v>2</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25">
-        <v>949927</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="32"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="34"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="35">
-        <v>1</v>
-      </c>
-      <c r="B25" s="36" t="s">
+      <c r="G34" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="C52" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="48"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="38">
-        <v>1001203075</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C26" s="46" t="s">
+      <c r="D53" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
+      <c r="E53" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C54" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D54" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E54" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="G54" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="42" t="s">
+      <c r="H54" s="52"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C55" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="H55" s="50"/>
+    </row>
+    <row r="56" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="54"/>
+      <c r="F56" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="50"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="45" t="s">
+      <c r="G56" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="F28" s="44" t="s">
+      <c r="H56" s="57"/>
+    </row>
+    <row r="57" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B57" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="44" t="s">
+      <c r="C57" s="61" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="59"/>
+      <c r="C58" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="64"/>
+      <c r="E58" s="64"/>
+      <c r="F58" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="69"/>
+    </row>
+    <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B59" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="H28" s="52"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B29" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H29" s="50"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B30" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="45" t="s">
+      <c r="C59" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="D59" s="64"/>
+      <c r="E59" s="64"/>
+      <c r="F59" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="69"/>
+    </row>
+    <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="60"/>
+      <c r="C60" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="44" t="s">
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="H30" s="52"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B31" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="43" t="s">
+      <c r="G60" s="1"/>
+      <c r="H60" s="69"/>
+    </row>
+    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C61" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="42" t="s">
+      <c r="D61" s="64"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="G61" s="1"/>
+      <c r="H61" s="69"/>
+    </row>
+    <row r="62" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="H31" s="50"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B32" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="45" t="s">
+      <c r="G62" s="10"/>
+      <c r="H62" s="71"/>
+    </row>
+    <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="E63" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="44" t="s">
+      <c r="F63" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="H32" s="52"/>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C33" s="53"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" s="56" t="s">
+      <c r="G63" s="73"/>
+      <c r="H63" s="74"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="57"/>
-    </row>
-    <row r="34" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B34" s="58" t="s">
+      <c r="D64" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="61" t="s">
+      <c r="E64" s="17"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" s="77" t="s">
+        <v>98</v>
+      </c>
+      <c r="C65" s="77"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" s="77"/>
+      <c r="C66" s="77"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B67" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="67" t="s">
+      <c r="C67" s="78"/>
+      <c r="E67" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" s="78"/>
+      <c r="G67" s="78"/>
+      <c r="H67" s="78"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D68" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="59"/>
-      <c r="C35" s="63" t="s">
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B70" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="69"/>
-    </row>
-    <row r="36" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B36" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="69"/>
-    </row>
-    <row r="37" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="60"/>
-      <c r="C37" s="63" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="69"/>
-    </row>
-    <row r="38" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C38" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="64"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="69"/>
-    </row>
-    <row r="39" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B39" s="75" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="71"/>
-    </row>
-    <row r="40" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="72" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" s="17"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B42" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="77"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B44" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" s="78"/>
-      <c r="E44" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D45" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B47" s="75" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="79">
-        <v>45705</v>
-      </c>
-      <c r="E48" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="78"/>
+    </row>
+    <row r="71" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="79">
+        <v>45706</v>
+      </c>
+      <c r="E71" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" s="78"/>
+      <c r="G71" s="78"/>
+      <c r="H71" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:H44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:H37"/>
+  <mergeCells count="60">
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
@@ -2240,7 +2357,7 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>

<commit_message>
Next stable version. Add Asp.Core.Identity. Implement ReturnProtocolBuildersStore, ReturnProtocolBuilderService and 2 new ReturnProtocolBuilders. Implement WPF Login View and logic to create users in Asp.Core.Identity. Remove Unusing classes.
</commit_message>
<xml_diff>
--- a/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
+++ b/DayReportsDataBase/ExportFiles/ExportedDayReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97594842f5de2827/Документы/DelitaTrade/DayReportsDataBase/ExportFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\source\repos\DelitaTrade\DayReportsDataBase\ExportFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="677" documentId="8_{18A9DDBF-BD83-45C8-AB2A-24D344D9F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E8486D-5FA8-4611-8DBF-11859F01811F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E210478-A456-4885-9E3F-55E1B53D73EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{68D2A0A9-2297-4A68-B6D0-4C9D918D7251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="124">
   <si>
     <t>Дневен Отчет</t>
   </si>
@@ -65,220 +65,286 @@
     <t>Плащане в брой</t>
   </si>
   <si>
-    <t>1 289,63 лв.</t>
-  </si>
-  <si>
-    <t>Енте ООД</t>
-  </si>
-  <si>
-    <t>Ресторант 4 Посоки - Банско</t>
-  </si>
-  <si>
-    <t>199,20 лв.</t>
-  </si>
-  <si>
-    <t>Мир-2006 ООД</t>
-  </si>
-  <si>
-    <t>Ла Пиер - Банско</t>
-  </si>
-  <si>
-    <t>144,47 лв.</t>
-  </si>
-  <si>
-    <t>207,72 лв.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Търговец - Атанас Колев </t>
-  </si>
-  <si>
-    <t>Търговец - Атанас Колев</t>
+    <t>145,82 лв.</t>
+  </si>
+  <si>
+    <t>Кристин 05 ЕООД</t>
+  </si>
+  <si>
+    <t>Дупнишка скара</t>
+  </si>
+  <si>
+    <t>504,43 лв.</t>
+  </si>
+  <si>
+    <t>Арт Ен Фън 003 ЕООД</t>
+  </si>
+  <si>
+    <t>Ресторант Къщата</t>
+  </si>
+  <si>
+    <t>134,88 лв.</t>
+  </si>
+  <si>
+    <t>ТК Фуут ЕООД</t>
+  </si>
+  <si>
+    <t>Тихият кът</t>
+  </si>
+  <si>
+    <t>157,22 лв.</t>
+  </si>
+  <si>
+    <t>Рамира Кюстендил ООД</t>
+  </si>
+  <si>
+    <t>Хотел Рамира</t>
+  </si>
+  <si>
+    <t>155,09 лв.</t>
+  </si>
+  <si>
+    <t>В И М Мюзик 1 ЕООД</t>
+  </si>
+  <si>
+    <t>Революшън</t>
+  </si>
+  <si>
+    <t>80,05 лв.</t>
+  </si>
+  <si>
+    <t>360,98 лв.</t>
+  </si>
+  <si>
+    <t>Хилс 1940 ЕООД</t>
+  </si>
+  <si>
+    <t>Пассионе</t>
+  </si>
+  <si>
+    <t>532,87 лв.</t>
+  </si>
+  <si>
+    <t>Флора Бургер ЕООД</t>
+  </si>
+  <si>
+    <t>Кафе Флора - Кюстендил</t>
+  </si>
+  <si>
+    <t>1 083,13 лв.</t>
+  </si>
+  <si>
+    <t>Рекпласт ЕООД</t>
+  </si>
+  <si>
+    <t>Кафе ABC</t>
+  </si>
+  <si>
+    <t>601,16 лв.</t>
+  </si>
+  <si>
+    <t>МСД 2016 ООД</t>
+  </si>
+  <si>
+    <t>Ресторант Терасата</t>
+  </si>
+  <si>
+    <t>2 035,72 лв.</t>
+  </si>
+  <si>
+    <t>Дринк Фактори ООД</t>
+  </si>
+  <si>
+    <t>Дринк Фактори - Дупница</t>
+  </si>
+  <si>
+    <t>813,17 лв.</t>
+  </si>
+  <si>
+    <t>Радостин Тренев ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Уест</t>
+  </si>
+  <si>
+    <t>593,32 лв.</t>
+  </si>
+  <si>
+    <t>Уин Клуб ООД</t>
+  </si>
+  <si>
+    <t>Уин Клуб - Дупница</t>
+  </si>
+  <si>
+    <t>166,39 лв.</t>
+  </si>
+  <si>
+    <t>Емил Станоев - Еми ЕТ</t>
+  </si>
+  <si>
+    <t>Бързо Хранене</t>
+  </si>
+  <si>
+    <t>364,68 лв.</t>
+  </si>
+  <si>
+    <t>ТМА 2011 ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Наполи</t>
+  </si>
+  <si>
+    <t>689,98 лв.</t>
+  </si>
+  <si>
+    <t>Каталина 2024 ЕООД</t>
+  </si>
+  <si>
+    <t>Пица Роял - Кюстендил</t>
+  </si>
+  <si>
+    <t>933,07 лв.</t>
+  </si>
+  <si>
+    <t>Стримон Спа АД</t>
+  </si>
+  <si>
+    <t>Хотел Стримон гардън</t>
   </si>
   <si>
     <t>Плащане по банка</t>
   </si>
   <si>
-    <t>107,88 лв.</t>
+    <t>326,16 лв.</t>
   </si>
   <si>
     <t>Банка</t>
   </si>
   <si>
-    <t>Гехард ЕООД</t>
-  </si>
-  <si>
-    <t>Хотел Кенпински Банско</t>
-  </si>
-  <si>
-    <t>138,60 лв.</t>
-  </si>
-  <si>
-    <t>Хотел Перун - Банско ЕООД</t>
-  </si>
-  <si>
-    <t>Хотел Перун - Банско</t>
-  </si>
-  <si>
-    <t>173,59 лв.</t>
-  </si>
-  <si>
-    <t>532,19 лв.</t>
-  </si>
-  <si>
-    <t>Рентали ЕООД</t>
-  </si>
-  <si>
-    <t>Ресторант Гарлик - Банско</t>
-  </si>
-  <si>
-    <t>3 159,43 лв.</t>
-  </si>
-  <si>
-    <t>Буларм Груп ООД</t>
-  </si>
-  <si>
-    <t>Буларм - Банско</t>
-  </si>
-  <si>
-    <t>685,40 лв.</t>
-  </si>
-  <si>
-    <t>Фокача Експрес ЕООД</t>
-  </si>
-  <si>
-    <t>Фокача Джано - Банско</t>
-  </si>
-  <si>
-    <t>675,90 лв.</t>
-  </si>
-  <si>
-    <t>Хотелс Енд Дриймс ООД</t>
-  </si>
-  <si>
-    <t>Ресторант Леонардо Банско</t>
-  </si>
-  <si>
-    <t>333,71 лв.</t>
-  </si>
-  <si>
-    <t>Майсторови 2016 ООД</t>
-  </si>
-  <si>
-    <t>Майсторови - Гоце Делчев</t>
-  </si>
-  <si>
-    <t>158,29 лв.</t>
-  </si>
-  <si>
-    <t>Емарди ООД</t>
-  </si>
-  <si>
-    <t>Кафе Емар - Банско</t>
-  </si>
-  <si>
-    <t>763,19 лв.</t>
-  </si>
-  <si>
-    <t>344,74 лв.</t>
-  </si>
-  <si>
-    <t>1 571,54 лв.</t>
-  </si>
-  <si>
-    <t>1 446,47 лв.</t>
-  </si>
-  <si>
-    <t>Приват Турс 2000 ЕООД</t>
-  </si>
-  <si>
-    <t>Фор Пойнтс - Банско</t>
-  </si>
-  <si>
-    <t>84,12 лв.</t>
-  </si>
-  <si>
-    <t>395,83 лв.</t>
+    <t>Черешката ЕООД</t>
+  </si>
+  <si>
+    <t>Белканто</t>
+  </si>
+  <si>
+    <t>187,91 лв.</t>
+  </si>
+  <si>
+    <t>Ресторант Алея - Кюстендил</t>
+  </si>
+  <si>
+    <t>2 336,20 лв.</t>
+  </si>
+  <si>
+    <t>Станби ЕООД</t>
+  </si>
+  <si>
+    <t>Френдс бар и грил</t>
+  </si>
+  <si>
+    <t>204,62 лв.</t>
   </si>
   <si>
     <t>0,00 лв.</t>
   </si>
   <si>
-    <t>Юлен АД</t>
-  </si>
-  <si>
-    <t>Юлен - Бъндеришка Вип</t>
-  </si>
-  <si>
-    <t>Юлен - Шилигарника Бла Бла</t>
-  </si>
-  <si>
-    <t>Юлен - Начална Хепи Енд</t>
-  </si>
-  <si>
-    <t>Юлен - Бъндеришки Щеки</t>
-  </si>
-  <si>
-    <t>Юлен Бъчвите - Бъндеришка Поляна</t>
-  </si>
-  <si>
-    <t>Юлен - Начална Етно</t>
+    <t>Дар Г.Н. ООД</t>
+  </si>
+  <si>
+    <t>F29</t>
   </si>
   <si>
     <t>Отчет на парите</t>
   </si>
   <si>
+    <t>1 -</t>
+  </si>
+  <si>
+    <t>0,10 лв.</t>
+  </si>
+  <si>
+    <t>7 -</t>
+  </si>
+  <si>
+    <t>0,20 лв.</t>
+  </si>
+  <si>
+    <t>1,40 лв.</t>
+  </si>
+  <si>
+    <t>5 -</t>
+  </si>
+  <si>
+    <t>0,50 лв.</t>
+  </si>
+  <si>
+    <t>2,50 лв.</t>
+  </si>
+  <si>
     <t>4 -</t>
   </si>
   <si>
-    <t>0,10 лв.</t>
-  </si>
-  <si>
-    <t>0,40 лв.</t>
-  </si>
-  <si>
-    <t>1 -</t>
-  </si>
-  <si>
-    <t>0,20 лв.</t>
-  </si>
-  <si>
-    <t>0,50 лв.</t>
-  </si>
-  <si>
-    <t>10 -</t>
+    <t>1,00 лв.</t>
+  </si>
+  <si>
+    <t>4,00 лв.</t>
+  </si>
+  <si>
+    <t>2 -</t>
+  </si>
+  <si>
+    <t>2,00 лв.</t>
+  </si>
+  <si>
+    <t>8 -</t>
+  </si>
+  <si>
+    <t>5,00 лв.</t>
+  </si>
+  <si>
+    <t>40,00 лв.</t>
+  </si>
+  <si>
+    <t>144 -</t>
   </si>
   <si>
     <t>10,00 лв.</t>
   </si>
   <si>
+    <t>1 440,00 лв.</t>
+  </si>
+  <si>
+    <t>68 -</t>
+  </si>
+  <si>
+    <t>20,00 лв.</t>
+  </si>
+  <si>
+    <t>1 360,00 лв.</t>
+  </si>
+  <si>
+    <t>82 -</t>
+  </si>
+  <si>
+    <t>50,00 лв.</t>
+  </si>
+  <si>
+    <t>4 100,00 лв.</t>
+  </si>
+  <si>
+    <t>24 -</t>
+  </si>
+  <si>
     <t>100,00 лв.</t>
   </si>
   <si>
-    <t>22 -</t>
-  </si>
-  <si>
-    <t>20,00 лв.</t>
-  </si>
-  <si>
-    <t>440,00 лв.</t>
-  </si>
-  <si>
-    <t>50,00 лв.</t>
-  </si>
-  <si>
-    <t>1 100,00 лв.</t>
-  </si>
-  <si>
-    <t>2 -</t>
-  </si>
-  <si>
-    <t>200,00 лв.</t>
+    <t>2 400,00 лв.</t>
   </si>
   <si>
     <t>Тотал:</t>
   </si>
   <si>
-    <t>1 841,10 лв.</t>
+    <t>9 352,00 лв.</t>
   </si>
   <si>
     <t>Преброена сума</t>
@@ -290,7 +356,7 @@
     <t xml:space="preserve">Общо приходи от доставки: </t>
   </si>
   <si>
-    <t>12 411,90 лв.</t>
+    <t>12 406,85 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Общо приходи от стари сметки: </t>
@@ -302,7 +368,7 @@
     <t xml:space="preserve">Сума от документи по банка: </t>
   </si>
   <si>
-    <t>10 570,88 лв.</t>
+    <t>3 054,89 лв.</t>
   </si>
   <si>
     <t xml:space="preserve">Разходи + КИ: </t>
@@ -311,13 +377,13 @@
     <t xml:space="preserve">Тотал - Отчетена сума: </t>
   </si>
   <si>
-    <t>1 841,02 лв.</t>
+    <t>9 351,96 лв.</t>
   </si>
   <si>
     <t>Ресто:</t>
   </si>
   <si>
-    <t>0,08 лв.</t>
+    <t>0,04 лв.</t>
   </si>
   <si>
     <t>Превозно средство №:</t>
@@ -332,7 +398,7 @@
     <t>Приел отчета:</t>
   </si>
   <si>
-    <t>Александр Добров</t>
+    <t>Александър Добров</t>
   </si>
   <si>
     <t>(име, фамилия, подпис)</t>
@@ -351,7 +417,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ mmmm\ yyyy\ \'\г\.\'"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +480,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -805,7 +893,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -877,14 +965,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,27 +994,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -942,9 +1030,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -953,7 +1041,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -973,7 +1061,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1006,10 +1094,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1349,7 +1437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBEBE22-6398-4FFA-8860-0277F3C7BC62}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1385,7 +1473,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="8">
-        <v>45706</v>
+        <v>45814</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="9"/>
@@ -1446,7 +1534,7 @@
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="22">
-        <v>1001203860</v>
+        <v>1001230330</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>9</v>
@@ -1468,7 +1556,7 @@
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25">
-        <v>1001203875</v>
+        <v>1001230374</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>12</v>
@@ -1483,14 +1571,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="22">
-        <v>1001203879</v>
+        <v>1001230378</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>15</v>
@@ -1505,567 +1593,435 @@
         <v>4</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="25">
-        <v>1001203916</v>
+        <v>1001230381</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="32"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="29">
+        <v>5</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22">
+        <v>1001230385</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="31">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25">
+        <v>1001230386</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>7</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22">
+        <v>1001230387</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="31">
+        <v>8</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25">
+        <v>1001230396</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="32"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="29">
+        <v>9</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22">
+        <v>1001230404</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="31">
+        <v>10</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25">
+        <v>1001230416</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="32"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="29">
+        <v>11</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22">
+        <v>1001230417</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="31">
+        <v>12</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25">
+        <v>1001230418</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="29">
+        <v>13</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22">
+        <v>1001230420</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="31">
+        <v>14</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25">
+        <v>1001230422</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="32"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
+        <v>15</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22">
+        <v>1001230425</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="30"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="31">
         <v>16</v>
       </c>
-      <c r="G9" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="32"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="34"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
+      <c r="B21" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25">
+        <v>1001230426</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="29">
+        <v>17</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22">
+        <v>1001230466</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="29">
         <v>1</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22">
-        <v>1001203845</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="31">
+      <c r="B24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22">
+        <v>1001230397</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="30"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="31">
         <v>2</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25">
-        <v>1001203851</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="32"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="29">
+      <c r="B25" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25">
+        <v>1001230413</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="32"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="29">
         <v>3</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22">
-        <v>1001203852</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="31">
+      <c r="B26" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22">
+        <v>1001230414</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="31">
         <v>4</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25">
-        <v>1001203853</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
+      <c r="B27" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25">
+        <v>1001230415</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="32"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="35">
         <v>5</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22">
-        <v>1001203856</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="31">
-        <v>6</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25">
-        <v>1001203857</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
-        <v>7</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22">
-        <v>1001203867</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="30"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="31">
-        <v>8</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25">
-        <v>1001203868</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="29">
-        <v>9</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="22">
-        <v>1001203870</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="30"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="31">
-        <v>10</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25">
-        <v>1001203873</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="29">
-        <v>11</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22">
-        <v>1001203874</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="30"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="31">
-        <v>12</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25">
-        <v>1001203877</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="32"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="29">
-        <v>13</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22">
-        <v>1001203895</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="30"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="31">
-        <v>14</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="25">
-        <v>1001203902</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="32"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="29">
-        <v>15</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="22">
-        <v>1001203904</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="30"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="31">
-        <v>16</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="24"/>
-      <c r="E26" s="25">
-        <v>950705</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="32"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="29">
-        <v>17</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="22">
-        <v>950726</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="30"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="31">
-        <v>18</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25">
-        <v>950733</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" s="32"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="29">
-        <v>19</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22">
-        <v>950737</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="30"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="31">
-        <v>20</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B28" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38">
+        <v>976434</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="25">
-        <v>950738</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="32"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="29">
-        <v>21</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22">
-        <v>950739</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="30"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="31">
-        <v>22</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="25">
-        <v>950789</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="32"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="29">
-        <v>23</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22">
-        <v>1001203859</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="30"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="35">
-        <v>24</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38">
-        <v>1001203869</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" s="39"/>
+      <c r="H28" s="39"/>
     </row>
     <row r="51" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="52" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
       <c r="C52" s="46" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
@@ -2075,266 +2031,295 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="40" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C53" s="49" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E53" s="43" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="G53" s="42" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="H53" s="50"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="41" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C54" s="51" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E54" s="45" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="F54" s="44" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G54" s="44" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H54" s="52"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55" s="40" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C55" s="49" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="E55" s="43" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G55" s="42" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="H55" s="50"/>
     </row>
-    <row r="56" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C56" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="E56" s="54"/>
-      <c r="F56" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="H56" s="57"/>
-    </row>
-    <row r="57" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B57" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C56" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="62"/>
-      <c r="E57" s="62"/>
-      <c r="F57" s="67" t="s">
+      <c r="E56" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" s="52"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="G57" s="4"/>
-      <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="59"/>
-      <c r="C58" s="63" t="s">
+      <c r="C57" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="64"/>
-      <c r="F58" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="69"/>
+      <c r="D57" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" s="50"/>
+    </row>
+    <row r="58" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C58" s="53"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="54"/>
+      <c r="F58" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="G58" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="H58" s="57"/>
     </row>
     <row r="59" spans="2:8" ht="16" x14ac:dyDescent="0.35">
       <c r="B59" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="D59" s="64"/>
-      <c r="E59" s="64"/>
-      <c r="F59" s="68" t="s">
-        <v>54</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="69"/>
+        <v>103</v>
+      </c>
+      <c r="C59" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="G59" s="4"/>
+      <c r="H59" s="5"/>
     </row>
     <row r="60" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="60"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="63" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D60" s="64"/>
       <c r="E60" s="64"/>
       <c r="F60" s="68" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="69"/>
     </row>
-    <row r="61" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C61" s="64" t="s">
-        <v>89</v>
+    <row r="61" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B61" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="63" t="s">
+        <v>108</v>
       </c>
       <c r="D61" s="64"/>
       <c r="E61" s="64"/>
       <c r="F61" s="68" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="69"/>
     </row>
-    <row r="62" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="B62" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="C62" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D62" s="65"/>
-      <c r="E62" s="65"/>
-      <c r="F62" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="G62" s="10"/>
-      <c r="H62" s="71"/>
+    <row r="62" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="60"/>
+      <c r="C62" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="64"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="G62" s="1"/>
+      <c r="H62" s="69"/>
     </row>
     <row r="63" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="76" t="s">
-        <v>95</v>
-      </c>
-      <c r="E63" s="66" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="G63" s="73"/>
-      <c r="H63" s="74"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B64" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E64" s="17"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B65" s="77" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" s="77"/>
+      <c r="C63" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="69"/>
+    </row>
+    <row r="64" spans="2:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="D64" s="65"/>
+      <c r="E64" s="65"/>
+      <c r="F64" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="71"/>
+    </row>
+    <row r="65" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="F65" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="G65" s="73"/>
+      <c r="H65" s="74"/>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B66" s="77"/>
-      <c r="C66" s="77"/>
+      <c r="B66" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="17"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B67" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="78"/>
-      <c r="E67" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="F67" s="78"/>
-      <c r="G67" s="78"/>
-      <c r="H67" s="78"/>
+      <c r="B67" s="77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" s="77"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="D68" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="70" spans="2:8" ht="16" x14ac:dyDescent="0.35">
-      <c r="B70" s="75" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="79">
-        <v>45706</v>
-      </c>
-      <c r="E71" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="F71" s="78"/>
-      <c r="G71" s="78"/>
-      <c r="H71" s="78"/>
+      <c r="B68" s="77"/>
+      <c r="C68" s="77"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="C69" s="78"/>
+      <c r="E69" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" s="78"/>
+      <c r="G69" s="78"/>
+      <c r="H69" s="78"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D70" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="72" spans="2:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="B72" s="75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B73" s="79">
+        <v>45817</v>
+      </c>
+      <c r="E73" s="78" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="78"/>
+      <c r="G73" s="78"/>
+      <c r="H73" s="78"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="E71:H71"/>
+  <mergeCells count="54">
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:H61"/>
     <mergeCell ref="C62:E62"/>
     <mergeCell ref="F62:H62"/>
+    <mergeCell ref="C63:E63"/>
     <mergeCell ref="F63:H63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="G58:H58"/>
     <mergeCell ref="C59:E59"/>
     <mergeCell ref="F59:H59"/>
     <mergeCell ref="C60:E60"/>
     <mergeCell ref="F60:H60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
@@ -2357,7 +2342,7 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F2:H2"/>

</xml_diff>